<commit_message>
changed variable type descriptions
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -207,6 +207,9 @@
     <t xml:space="preserve">dataelementgroup</t>
   </si>
   <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D2;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataelement</t>
   </si>
   <si>
@@ -225,6 +228,9 @@
     <t xml:space="preserve">=SVERWEIS(dataelements!$D5;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
     <t xml:space="preserve">=SVERWEIS(dataelements!$D6;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
@@ -292,6 +298,12 @@
   </si>
   <si>
     <t xml:space="preserve">de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paragraph 21 (DQA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diese Gruppe enthält die Datenelemente des Paragraph 21, die im Rahmen der DQ-Analyse geprüft werden.</t>
   </si>
   <si>
     <t xml:space="preserve">Aufnahmeanlass</t>
@@ -479,22 +491,262 @@
 Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
   </si>
   <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designation of data element (in first defined language)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designation of value (in first defined language)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataelement_id</t>
   </si>
   <si>
     <t xml:space="preserve">key</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
     <t xml:space="preserve">Designation of date element (first defined language)</t>
   </si>
   <si>
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
@@ -503,7 +755,7 @@
     <t xml:space="preserve">p21csv</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_source"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["AUFNAHMEANLASS"],"source_table_name":["FALL.CSV"],"value_set":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.admission_source"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["AUFNAHMEANLASS"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
@@ -512,7 +764,7 @@
     <t xml:space="preserve">i2b2</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"value_set":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNAN%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNAN%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
@@ -521,61 +773,61 @@
     <t xml:space="preserve">omop</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"variable_type":["integer"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_source"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_TAGEN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"value_set":["{\"min\": 0, \"max\": 366}"],"value_threshold":[0]}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_source"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_TAGEN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"value_set":["{\"min\": 0, \"max\": 366}"],"value_threshold":[0],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AITAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AITAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"min\": 0, \"max\": 366}"],"value_threshold":[0],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 8512"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 8512"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"variable_type":["integer"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_source"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_JAHREN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"value_set":["{\"min\": 0, \"max\": 110}"],"value_threshold":[5]}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_source"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_JAHREN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"value_set":["{\"min\": 0, \"max\": 110}"],"value_threshold":[5],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AIJAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AIJAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"min\": 0, \"max\": 110}"],"value_threshold":[5],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 9448"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 9448"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
@@ -599,7 +851,7 @@
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
@@ -623,55 +875,55 @@
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_source"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["Diagnoseart"],"source_table_name":["ICD.CSV"],"value_set":["{\"value_set\": \"HD, ND\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_source"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["Diagnoseart"],"source_table_name":["ICD.CSV"],"constraints":["{\"value_set\": \"HD, ND\"}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["modifier_cd"],"source_table_name":["observation_fact"],"value_set":["{\"value_set\": \"HD, ND\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["modifier_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"HD, ND\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A24;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["condition_type_concept_id"],"source_table_name":["condition_occurrence"],"value_set":["{\"value_set\": \"44786627, 44786629\"}"],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["condition_occurrence"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["condition_type_concept_id"],"source_table_name":["condition_occurrence"],"constraints":["{\"value_set\": \"44786627, 44786629\"}"],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["condition_occurrence"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A25;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A26;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_source"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["ENTLASSUNGSGRUND"],"source_table_name":["FALL.CSV"],"value_set":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_source"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["ENTLASSUNGSGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A27;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"value_set":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ENTLGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ENTLGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A28;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation"],"sql_where":["observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation"],"sql_where":["observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A29;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"variable_type":["factor"],"plausibility_relation":["{\"uniqueness\": {\"patient_identifier_value\": {\"name\": \"Pl.uniqueness.Item02\", \"description\": \"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\": {\"patient_identifier_value\": {\"name\": \"Pl.uniqueness.Item02\", \"description\": \"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A30;dataelements!A:G;7;FALSCH)</t>
@@ -695,7 +947,7 @@
     <t xml:space="preserve">=SVERWEIS($A33;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"variable_type":["date"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A34;dataelements!A:G;7;FALSCH)</t>
@@ -719,7 +971,7 @@
     <t xml:space="preserve">=SVERWEIS($A37;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"variable_type":["date"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A38;dataelements!A:G;7;FALSCH)</t>
@@ -743,55 +995,55 @@
     <t xml:space="preserve">=SVERWEIS($A41;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"variable_type":["factor"],"plausibility_relation":["{\"atemporal\": {\"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item01\", \"description\": \"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"O[0-9]\", \"i2b2\": \"O[0-9]\", \"p21csv\": \"O[0-9]\"}, \"join_crit\": \"encounter_identifier_value\", \"checks\": {\"value_set\": {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item02\", \"description\": \"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C5[1-8]\", \"i2b2\": \"C5[1-8]\", \"p21csv\": \"C5[1-8]\"}, \"join_crit\": \"encounter_identifier_value\", \"checks\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item03\", \"description\": \"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C6[0-3]\", \"i2b2\": \"C6[0-3]\", \"p21csv\": \"C6[0-3]\"}, \"join_crit\": \"encounter_identifier_value\", \"checks\": {\"value_set\":  {\"omop\": \"m\", \"i2b2\": \"m\", \"p21csv\": \"m\"}}}, \"encounter_hospitalization_class\": {\"name\": \"Pl.atemporal.Item04\", \"description\": \"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\", \"filter\": {\"omop\": \"05xx\", \"i2b2\": \"05xx\", \"p21csv\": \"05xx\"}, \"join_crit\": \"encounter_identifier_value\", \"checks\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\": {\"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item01\", \"description\": \"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"O[0-9]\", \"i2b2\": \"O[0-9]\", \"p21csv\": \"O[0-9]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\": {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item02\", \"description\": \"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C5[1-8]\", \"i2b2\": \"C5[1-8]\", \"p21csv\": \"C5[1-8]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item03\", \"description\": \"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C6[0-3]\", \"i2b2\": \"C6[0-3]\", \"p21csv\": \"C6[0-3]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"m\", \"i2b2\": \"m\", \"p21csv\": \"m\"}}}, \"encounter_hospitalization_class\": {\"name\": \"Pl.atemporal.Item04\", \"description\": \"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\", \"filter\": {\"omop\": \"05xx\", \"i2b2\": \"05xx\", \"p21csv\": \"05xx\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A42;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_source"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["GESCHLECHT"],"source_table_name":["FALL.CSV"],"value_set":["{\"value_set\": \"m, w, x\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.gender_source"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["GESCHLECHT"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"m, w, x\"}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A43;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["sex_cd"],"source_table_name":["patient_dimension"],"value_set":["{\"value_set\": \"m, w, x\"}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["sex_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"value_set\": \"m, w, x\"}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A44;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["gender_source_value"],"source_table_name":["person"],"value_set":["{\"value_set\": \"m, w, x\"}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["gender_source_value"],"source_table_name":["person"],"constraints":["{\"value_set\": \"m, w, x\"}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A45;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A46;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_source"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["AUFNAHMEGRUND"],"source_table_name":["FALL.CSV"],"value_set":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_source"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["AUFNAHMEGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A47;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"value_set":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A48;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A49;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"variable_type":["factor"],"plausibility_relation":["{\"uniqueness\": {\"patient_birthDate\": {\"name\": \"Pl.uniqueness.Item01\", \"description\": \"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\": {\"patient_birthDate\": {\"name\": \"Pl.uniqueness.Item01\", \"description\": \"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A50;dataelements!A:G;7;FALSCH)</t>
@@ -815,7 +1067,7 @@
     <t xml:space="preserve">=SVERWEIS($A53;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A54;dataelements!A:G;7;FALSCH)</t>
@@ -839,7 +1091,7 @@
     <t xml:space="preserve">=SVERWEIS($A57;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"variable_type":["date"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A58;dataelements!A:G;7;FALSCH)</t>
@@ -863,7 +1115,7 @@
     <t xml:space="preserve">=SVERWEIS($A61;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A62;dataelements!A:G;7;FALSCH)</t>
@@ -887,7 +1139,7 @@
     <t xml:space="preserve">=SVERWEIS($A65;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"variable_type":["date"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A66;dataelements!A:G;7;FALSCH)</t>
@@ -911,7 +1163,7 @@
     <t xml:space="preserve">=SVERWEIS($A69;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"variable_type":["date"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A70;dataelements!A:G;7;FALSCH)</t>
@@ -935,31 +1187,31 @@
     <t xml:space="preserve">=SVERWEIS($A73;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"variable_type":["integer"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A74;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_source"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["BEATMUNGSSTUNDEN"],"source_table_name":["FALL.CSV"],"value_set":["{\"min\": 0, \"max\": 8766}"]}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_source"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["BEATMUNGSSTUNDEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A75;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"value_set":["{\"min\": 0, \"max\": 8766}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:BEATMST'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:BEATMST'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A76;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"value_set":["{\"min\": 0, \"max\": 8766}"],"sql_from":["observation"],"sql_where":["observation_concept_id = 4108449"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"],"sql_from":["observation"],"sql_where":["observation_concept_id = 4108449"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A77;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"variable_type":["factor"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A78;dataelements!A:G;7;FALSCH)</t>
@@ -1197,8 +1449,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D21" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D22" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D22"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1210,7 +1462,21 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E40"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="value"/>
+    <tableColumn id="3" name="definition_id"/>
+    <tableColumn id="4" name="Designation of data element (in first defined language)"/>
+    <tableColumn id="5" name="Designation of value (in first defined language)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:D81"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
@@ -3758,30 +4024,36 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
       <c r="E2"/>
       <c r="F2"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3"/>
+        <v>61</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4">
@@ -3789,20 +4061,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F4"/>
       <c r="G4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -3810,20 +4082,20 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F5"/>
       <c r="G5" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6">
@@ -3831,20 +4103,20 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" t="n">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F6"/>
       <c r="G6" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7">
@@ -3852,20 +4124,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F7"/>
       <c r="G7" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
@@ -3873,20 +4145,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" t="n">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8"/>
+        <v>61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9">
@@ -3894,20 +4168,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D9" t="n">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9"/>
+        <v>61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
@@ -3915,20 +4191,20 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" t="n">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F10"/>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
@@ -3936,20 +4212,20 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" t="n">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F11"/>
       <c r="G11" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -3957,20 +4233,20 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" t="n">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F12"/>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -3978,20 +4254,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D13" t="n">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13"/>
+        <v>61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
       <c r="G13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14">
@@ -3999,20 +4277,22 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" t="n">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14"/>
+        <v>61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -4020,20 +4300,20 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" t="n">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F15"/>
       <c r="G15" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16">
@@ -4041,20 +4321,20 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D16" t="n">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F16"/>
       <c r="G16" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
@@ -4062,20 +4342,20 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D17" t="n">
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F17"/>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -4083,20 +4363,20 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" t="n">
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F18"/>
       <c r="G18" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19">
@@ -4104,20 +4384,20 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -4125,20 +4405,20 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" t="n">
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21">
@@ -4146,20 +4426,20 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D21" t="n">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F21"/>
       <c r="G21" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
@@ -4167,20 +4447,20 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" t="n">
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F22"/>
       <c r="G22" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23">
@@ -5648,296 +5928,310 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" t="s">
-        <v>127</v>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -6988,33 +7282,527 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" ht="12.75" customHeight="1">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25" t="s">
+        <v>182</v>
+      </c>
+      <c r="E25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>191</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30" t="s">
+        <v>192</v>
+      </c>
+      <c r="E30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>195</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="D2" t="e">
-        <f t="array" ref="D2">VLOOKUP(validations_permittedValues!$A2,IF(dataelements!$E:$E="permittedValues",dataelements!$F:$G),2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E2" t="e">
-        <f>VLOOKUP($C2,definitions!$A:$C,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="D19" s="1"/>
+      <c r="B34" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35" t="s">
+        <v>202</v>
+      </c>
+      <c r="E35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>203</v>
+      </c>
+      <c r="C36"/>
+      <c r="D36" t="s">
+        <v>204</v>
+      </c>
+      <c r="E36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37"/>
+      <c r="D37" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>207</v>
+      </c>
+      <c r="C38"/>
+      <c r="D38" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39"/>
+      <c r="D39" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>211</v>
+      </c>
+      <c r="C40"/>
+      <c r="D40" t="s">
+        <v>212</v>
+      </c>
+      <c r="E40"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -7024,6 +7812,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12368,16 +13159,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>129</v>
+        <v>214</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2">
@@ -12385,13 +13176,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>217</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3">
@@ -12399,13 +13190,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
@@ -12413,13 +13204,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5">
@@ -12427,13 +13218,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>226</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6">
@@ -12441,13 +13232,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>228</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7">
@@ -12455,13 +13246,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
@@ -12469,13 +13260,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9">
@@ -12483,13 +13274,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>234</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10">
@@ -12497,13 +13288,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
       <c r="D10" t="s">
-        <v>153</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11">
@@ -12511,13 +13302,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>238</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12">
@@ -12525,13 +13316,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
-        <v>157</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13">
@@ -12539,13 +13330,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14">
@@ -12553,13 +13344,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15">
@@ -12567,13 +13358,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
@@ -12581,13 +13372,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>248</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17">
@@ -12595,13 +13386,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>250</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18">
@@ -12609,13 +13400,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
-        <v>168</v>
+        <v>252</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19">
@@ -12623,13 +13414,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>254</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20">
@@ -12637,13 +13428,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21">
@@ -12651,13 +13442,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>258</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22">
@@ -12665,13 +13456,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
+        <v>260</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23">
@@ -12679,13 +13470,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>262</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24">
@@ -12693,13 +13484,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>264</v>
       </c>
       <c r="D24" t="s">
-        <v>181</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25">
@@ -12707,13 +13498,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>266</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26">
@@ -12721,13 +13512,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C26" t="s">
-        <v>184</v>
+        <v>268</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27">
@@ -12735,13 +13526,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C27" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
       <c r="D27" t="s">
-        <v>187</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28">
@@ -12749,13 +13540,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C28" t="s">
-        <v>188</v>
+        <v>272</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29">
@@ -12763,13 +13554,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
-        <v>190</v>
+        <v>274</v>
       </c>
       <c r="D29" t="s">
-        <v>191</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30">
@@ -12777,13 +13568,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C30" t="s">
-        <v>192</v>
+        <v>276</v>
       </c>
       <c r="D30" t="s">
-        <v>193</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31">
@@ -12791,13 +13582,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C31" t="s">
-        <v>194</v>
+        <v>278</v>
       </c>
       <c r="D31" t="s">
-        <v>195</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32">
@@ -12805,13 +13596,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>280</v>
       </c>
       <c r="D32" t="s">
-        <v>197</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33">
@@ -12819,13 +13610,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>282</v>
       </c>
       <c r="D33" t="s">
-        <v>199</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34">
@@ -12833,13 +13624,13 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>284</v>
       </c>
       <c r="D34" t="s">
-        <v>201</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35">
@@ -12847,13 +13638,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>286</v>
       </c>
       <c r="D35" t="s">
-        <v>203</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36">
@@ -12861,13 +13652,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C36" t="s">
-        <v>204</v>
+        <v>288</v>
       </c>
       <c r="D36" t="s">
-        <v>205</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37">
@@ -12875,13 +13666,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C37" t="s">
-        <v>206</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>207</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38">
@@ -12889,13 +13680,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C38" t="s">
-        <v>208</v>
+        <v>292</v>
       </c>
       <c r="D38" t="s">
-        <v>209</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39">
@@ -12903,13 +13694,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C39" t="s">
-        <v>210</v>
+        <v>294</v>
       </c>
       <c r="D39" t="s">
-        <v>211</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40">
@@ -12917,13 +13708,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C40" t="s">
-        <v>212</v>
+        <v>296</v>
       </c>
       <c r="D40" t="s">
-        <v>213</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41">
@@ -12931,13 +13722,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C41" t="s">
-        <v>214</v>
+        <v>298</v>
       </c>
       <c r="D41" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42">
@@ -12945,13 +13736,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C42" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="D42" t="s">
-        <v>217</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43">
@@ -12959,13 +13750,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C43" t="s">
-        <v>218</v>
+        <v>302</v>
       </c>
       <c r="D43" t="s">
-        <v>219</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44">
@@ -12973,13 +13764,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>304</v>
       </c>
       <c r="D44" t="s">
-        <v>221</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45">
@@ -12987,13 +13778,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C45" t="s">
-        <v>222</v>
+        <v>306</v>
       </c>
       <c r="D45" t="s">
-        <v>223</v>
+        <v>307</v>
       </c>
     </row>
     <row r="46">
@@ -13001,13 +13792,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C46" t="s">
-        <v>224</v>
+        <v>308</v>
       </c>
       <c r="D46" t="s">
-        <v>225</v>
+        <v>309</v>
       </c>
     </row>
     <row r="47">
@@ -13015,13 +13806,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C47" t="s">
-        <v>226</v>
+        <v>310</v>
       </c>
       <c r="D47" t="s">
-        <v>227</v>
+        <v>311</v>
       </c>
     </row>
     <row r="48">
@@ -13029,13 +13820,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C48" t="s">
-        <v>228</v>
+        <v>312</v>
       </c>
       <c r="D48" t="s">
-        <v>229</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49">
@@ -13043,13 +13834,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>314</v>
       </c>
       <c r="D49" t="s">
-        <v>231</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50">
@@ -13057,13 +13848,13 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>316</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>317</v>
       </c>
     </row>
     <row r="51">
@@ -13071,13 +13862,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C51" t="s">
-        <v>234</v>
+        <v>318</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>319</v>
       </c>
     </row>
     <row r="52">
@@ -13085,13 +13876,13 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C52" t="s">
-        <v>236</v>
+        <v>320</v>
       </c>
       <c r="D52" t="s">
-        <v>237</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53">
@@ -13099,13 +13890,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>322</v>
       </c>
       <c r="D53" t="s">
-        <v>239</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54">
@@ -13113,13 +13904,13 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C54" t="s">
-        <v>240</v>
+        <v>324</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55">
@@ -13127,13 +13918,13 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C55" t="s">
-        <v>242</v>
+        <v>326</v>
       </c>
       <c r="D55" t="s">
-        <v>243</v>
+        <v>327</v>
       </c>
     </row>
     <row r="56">
@@ -13141,13 +13932,13 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C56" t="s">
-        <v>244</v>
+        <v>328</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
+        <v>329</v>
       </c>
     </row>
     <row r="57">
@@ -13155,13 +13946,13 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C57" t="s">
-        <v>246</v>
+        <v>330</v>
       </c>
       <c r="D57" t="s">
-        <v>247</v>
+        <v>331</v>
       </c>
     </row>
     <row r="58">
@@ -13169,13 +13960,13 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>248</v>
+        <v>332</v>
       </c>
       <c r="D58" t="s">
-        <v>249</v>
+        <v>333</v>
       </c>
     </row>
     <row r="59">
@@ -13183,13 +13974,13 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C59" t="s">
-        <v>250</v>
+        <v>334</v>
       </c>
       <c r="D59" t="s">
-        <v>251</v>
+        <v>335</v>
       </c>
     </row>
     <row r="60">
@@ -13197,13 +13988,13 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C60" t="s">
-        <v>252</v>
+        <v>336</v>
       </c>
       <c r="D60" t="s">
-        <v>253</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61">
@@ -13211,13 +14002,13 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C61" t="s">
-        <v>254</v>
+        <v>338</v>
       </c>
       <c r="D61" t="s">
-        <v>255</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62">
@@ -13225,13 +14016,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C62" t="s">
-        <v>256</v>
+        <v>340</v>
       </c>
       <c r="D62" t="s">
-        <v>257</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63">
@@ -13239,13 +14030,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C63" t="s">
-        <v>258</v>
+        <v>342</v>
       </c>
       <c r="D63" t="s">
-        <v>259</v>
+        <v>343</v>
       </c>
     </row>
     <row r="64">
@@ -13253,13 +14044,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C64" t="s">
-        <v>260</v>
+        <v>344</v>
       </c>
       <c r="D64" t="s">
-        <v>261</v>
+        <v>345</v>
       </c>
     </row>
     <row r="65">
@@ -13267,13 +14058,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C65" t="s">
-        <v>262</v>
+        <v>346</v>
       </c>
       <c r="D65" t="s">
-        <v>263</v>
+        <v>347</v>
       </c>
     </row>
     <row r="66">
@@ -13281,13 +14072,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C66" t="s">
-        <v>264</v>
+        <v>348</v>
       </c>
       <c r="D66" t="s">
-        <v>265</v>
+        <v>349</v>
       </c>
     </row>
     <row r="67">
@@ -13295,13 +14086,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C67" t="s">
-        <v>266</v>
+        <v>350</v>
       </c>
       <c r="D67" t="s">
-        <v>267</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68">
@@ -13309,13 +14100,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C68" t="s">
-        <v>268</v>
+        <v>352</v>
       </c>
       <c r="D68" t="s">
-        <v>269</v>
+        <v>353</v>
       </c>
     </row>
     <row r="69">
@@ -13323,13 +14114,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>354</v>
       </c>
       <c r="D69" t="s">
-        <v>271</v>
+        <v>355</v>
       </c>
     </row>
     <row r="70">
@@ -13337,13 +14128,13 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>272</v>
+        <v>356</v>
       </c>
       <c r="D70" t="s">
-        <v>273</v>
+        <v>357</v>
       </c>
     </row>
     <row r="71">
@@ -13351,13 +14142,13 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>274</v>
+        <v>358</v>
       </c>
       <c r="D71" t="s">
-        <v>275</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72">
@@ -13365,13 +14156,13 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C72" t="s">
-        <v>276</v>
+        <v>360</v>
       </c>
       <c r="D72" t="s">
-        <v>277</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73">
@@ -13379,13 +14170,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C73" t="s">
-        <v>278</v>
+        <v>362</v>
       </c>
       <c r="D73" t="s">
-        <v>279</v>
+        <v>363</v>
       </c>
     </row>
     <row r="74">
@@ -13393,13 +14184,13 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C74" t="s">
-        <v>280</v>
+        <v>364</v>
       </c>
       <c r="D74" t="s">
-        <v>281</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75">
@@ -13407,13 +14198,13 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>282</v>
+        <v>366</v>
       </c>
       <c r="D75" t="s">
-        <v>283</v>
+        <v>367</v>
       </c>
     </row>
     <row r="76">
@@ -13421,13 +14212,13 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C76" t="s">
-        <v>284</v>
+        <v>368</v>
       </c>
       <c r="D76" t="s">
-        <v>285</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77">
@@ -13435,13 +14226,13 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>286</v>
+        <v>370</v>
       </c>
       <c r="D77" t="s">
-        <v>287</v>
+        <v>371</v>
       </c>
     </row>
     <row r="78">
@@ -13449,13 +14240,13 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>132</v>
+        <v>216</v>
       </c>
       <c r="C78" t="s">
-        <v>288</v>
+        <v>372</v>
       </c>
       <c r="D78" t="s">
-        <v>289</v>
+        <v>373</v>
       </c>
     </row>
     <row r="79">
@@ -13463,13 +14254,13 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>135</v>
+        <v>219</v>
       </c>
       <c r="C79" t="s">
-        <v>290</v>
+        <v>374</v>
       </c>
       <c r="D79" t="s">
-        <v>291</v>
+        <v>375</v>
       </c>
     </row>
     <row r="80">
@@ -13477,13 +14268,13 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>138</v>
+        <v>222</v>
       </c>
       <c r="C80" t="s">
-        <v>292</v>
+        <v>376</v>
       </c>
       <c r="D80" t="s">
-        <v>293</v>
+        <v>377</v>
       </c>
     </row>
     <row r="81">
@@ -13491,13 +14282,13 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>141</v>
+        <v>225</v>
       </c>
       <c r="C81" t="s">
-        <v>294</v>
+        <v>378</v>
       </c>
       <c r="D81" t="s">
-        <v>295</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -13519,7 +14310,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
convert DQ-MDR to samply.import xlsx
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="425">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -306,23 +306,28 @@
     <t xml:space="preserve">Diese Gruppe enthält die Datenelemente des Paragraph 21, die im Rahmen der DQ-Analyse geprüft werden.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aufnahmeanlass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- E Einweisung durch einen Arzt 
-- Z Einweisung durch einen Zahnarzt 
-- N Notfall 
-- R Aufnahme nach vorausgehender Behandlung in einer Rehabilitationseinrichtung 
-- V Verlegung mit Behandlungsdauer im verlegenden Krankenhaus länger als 24 Stunden 
-- A Verlegung mit Behandlungsdauer im verlegenden Krankenhaus bis zu 24 Stunden  
-Zusatzschlüssel für besondere Kalkulationsanforderungen: 
-    - G Geburt (siehe Hinweis Neugeborene) 
-    - B Begleitperson oder mitaufgenommene Pflegekraft  
-Hinweise:  
-Einweisung durch einen Arzt ist im § 301-Aufnahmesatz im Segment Aufnahme durch die Arztnummer des einweisenden Arztes, Einweisung durch einen Zahnarzt durch die Zahnarztnummer des einweisenden Zahnarztes dokumentiert.  
-Verlegung ist im § 301-Aufnahmesatz durch das IK des die Aufnahme veranlassenden Krankenhauses dokumentiert. Wenn die Behandlungsdauer im verlegenden Krankenhaus nicht länger als 24 Stunden betrug ist als Aufnahmeanlass ‚A’, wenn sie länger als 24 Stunden betrug, ist ‚V’ anzugeben. Der Aufnahmeanlass ‚R’ wird in der § 301-Datenübermittlung nicht abgebildet, er soll übermittelt werden, wenn die Patientendatenhaltung dieses Zusatzmerkmal enthält.  
-Interne Verlegung mit Wechsel aus einem Entgeltbereich in einen anderen Entgeltbereich wird durch das eigene IK als IK des veranlassenden Krankenhauses dokumentiert.  
-Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">Alter (in Tagen)</t>
@@ -350,38 +355,67 @@
 Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Diagnoseart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsgrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01x Behandlung regulär beendet 
-- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
-- 03x Behandlung aus sonstigen Gründen beendet 
-- 04x Behandlung gegen ärztlichen Rat beendet 
-- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
-- 069 Verlegung in ein anderes Krankenhaus 
-- 079 Tod 
-- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
-- 099 Entlassung in eine Rehabilitationseinrichtung 
-- 109 Entlassung in eine Pflegeeinrichtung 
-- 119 Entlassung in ein Hospiz 
-- 139 externe Verlegung zur psychiatrischen Behandlung 
-- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
-- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
-- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
-- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
-- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
-- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
-- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
-Hinweise:  
-Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
-Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
-Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
+    <t xml:space="preserve">HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
   </si>
   <si>
     <t xml:space="preserve">Fallnummer</t>
@@ -416,27 +450,34 @@
 Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Geschlecht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- m männlich  
-- w weiblich  
-- x unbestimmt  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmegrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
-- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
-- 03xx Krankenhausbehandlung, teilstationär 
-- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
-- 05xx stationäre Entbindung 
-- 06xx Geburt 
-- 08xx Stationäre Aufnahme zur Organentnahme  
-Hinweise:  
-Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
-Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08xx</t>
   </si>
   <si>
     <t xml:space="preserve">Patientennummer</t>
@@ -500,238 +541,286 @@
     <t xml:space="preserve">Designation of value (in first defined language)</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Z</t>
+    <t xml:space="preserve">=SVERWEIS($C2;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
+    <t xml:space="preserve">=SVERWEIS($C3;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">R</t>
+    <t xml:space="preserve">=SVERWEIS($C4;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">V</t>
+    <t xml:space="preserve">=SVERWEIS($C5;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
+    <t xml:space="preserve">=SVERWEIS($C6;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">G</t>
+    <t xml:space="preserve">=SVERWEIS($C7;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t xml:space="preserve">=SVERWEIS($C8;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">HD</t>
+    <t xml:space="preserve">=SVERWEIS($C9;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">ND</t>
+    <t xml:space="preserve">=SVERWEIS($C10;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">01x</t>
+    <t xml:space="preserve">=SVERWEIS($C11;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">02x</t>
+    <t xml:space="preserve">=SVERWEIS($C12;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">03x</t>
+    <t xml:space="preserve">=SVERWEIS($C13;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">04x</t>
+    <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">059</t>
+    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">069</t>
+    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">079</t>
+    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">089</t>
+    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">099</t>
+    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">109</t>
+    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">119</t>
+    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">139</t>
+    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">14x</t>
+    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">15x</t>
+    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">179</t>
+    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">229</t>
+    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">239</t>
+    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">249</t>
+    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">259</t>
+    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">m</t>
+    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">w</t>
+    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">01xx</t>
+    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">02xx</t>
+    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">03xx</t>
+    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">04xx</t>
+    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">05xx</t>
+    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">06xx</t>
+    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
   </si>
   <si>
-    <t xml:space="preserve">08xx</t>
+    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range_from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range_to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit_of_measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A2;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A3;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A4;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A2;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A3;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A4;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A5;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A6;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
   </si>
   <si>
     <t xml:space="preserve">dataelement_id</t>
@@ -1449,8 +1538,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D56" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D56"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1476,7 +1565,33 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="range_from"/>
+    <tableColumn id="3" name="range_to"/>
+    <tableColumn id="4" name="unit_of_measure"/>
+    <tableColumn id="5" name="Designation of data element (in first defined language)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="format"/>
+    <tableColumn id="3" name="Designation of data element (in first defined language)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:D81"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
@@ -4072,7 +4187,9 @@
       <c r="E4" t="s">
         <v>63</v>
       </c>
-      <c r="F4"/>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>64</v>
       </c>
@@ -4093,7 +4210,9 @@
       <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="F5"/>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>65</v>
       </c>
@@ -4223,7 +4342,9 @@
       <c r="E11" t="s">
         <v>72</v>
       </c>
-      <c r="F11"/>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>73</v>
       </c>
@@ -4244,7 +4365,9 @@
       <c r="E12" t="s">
         <v>72</v>
       </c>
-      <c r="F12"/>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
@@ -4353,7 +4476,9 @@
       <c r="E17" t="s">
         <v>72</v>
       </c>
-      <c r="F17"/>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>79</v>
       </c>
@@ -4395,7 +4520,9 @@
       <c r="E19" t="s">
         <v>72</v>
       </c>
-      <c r="F19"/>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>81</v>
       </c>
@@ -4416,7 +4543,9 @@
       <c r="E20" t="s">
         <v>72</v>
       </c>
-      <c r="F20"/>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
       <c r="G20" s="1" t="s">
         <v>82</v>
       </c>
@@ -4437,7 +4566,9 @@
       <c r="E21" t="s">
         <v>63</v>
       </c>
-      <c r="F21"/>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
       <c r="G21" s="1" t="s">
         <v>83</v>
       </c>
@@ -5956,7 +6087,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="s">
         <v>89</v>
@@ -5965,273 +6096,749 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>1001</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>1002</v>
       </c>
       <c r="B5" t="s">
         <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>1003</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>1004</v>
       </c>
       <c r="B7" t="s">
         <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>1005</v>
       </c>
       <c r="B8" t="s">
         <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>1006</v>
       </c>
       <c r="B9" t="s">
         <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>1007</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>1008</v>
       </c>
       <c r="B15" t="s">
         <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>1009</v>
       </c>
       <c r="B16" t="s">
         <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>1010</v>
       </c>
       <c r="B17" t="s">
         <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>1011</v>
       </c>
       <c r="B18" t="s">
         <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>1012</v>
       </c>
       <c r="B19" t="s">
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>1013</v>
       </c>
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>1014</v>
       </c>
       <c r="B21" t="s">
         <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>1015</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
       </c>
       <c r="C22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1021</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1022</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1023</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1026</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1027</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1028</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>128</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" t="s">
         <v>130</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>9</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
         <v>131</v>
+      </c>
+      <c r="D37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>1029</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>1031</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1032</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1033</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1034</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1035</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>1036</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1037</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1038</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>15</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>17</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>18</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -7285,16 +7892,16 @@
         <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -7302,507 +7909,663 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2"/>
+        <v>92</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
       <c r="D2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2"/>
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3"/>
+        <v>93</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1001</v>
+      </c>
       <c r="D3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3"/>
+        <v>166</v>
+      </c>
+      <c r="E3" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4"/>
+        <v>94</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1002</v>
+      </c>
       <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4"/>
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5"/>
+        <v>95</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1003</v>
+      </c>
       <c r="D5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5"/>
+        <v>170</v>
+      </c>
+      <c r="E5" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6"/>
+        <v>96</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1004</v>
+      </c>
       <c r="D6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6"/>
+        <v>172</v>
+      </c>
+      <c r="E6" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7"/>
+        <v>97</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1005</v>
+      </c>
       <c r="D7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E7"/>
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8"/>
+        <v>98</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1006</v>
+      </c>
       <c r="D8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8"/>
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9"/>
+        <v>99</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1007</v>
+      </c>
       <c r="D9" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9"/>
+        <v>178</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10"/>
+        <v>108</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1008</v>
+      </c>
       <c r="D10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10"/>
+        <v>180</v>
+      </c>
+      <c r="E10" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C11"/>
+        <v>109</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1009</v>
+      </c>
       <c r="D11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E11"/>
+        <v>182</v>
+      </c>
+      <c r="E11" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12"/>
+        <v>110</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1010</v>
+      </c>
       <c r="D12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12"/>
+        <v>184</v>
+      </c>
+      <c r="E12" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C13"/>
+        <v>111</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1011</v>
+      </c>
       <c r="D13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13"/>
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
-      </c>
-      <c r="C14"/>
+        <v>112</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1012</v>
+      </c>
       <c r="D14" t="s">
-        <v>160</v>
-      </c>
-      <c r="E14"/>
+        <v>188</v>
+      </c>
+      <c r="E14" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C15"/>
+        <v>113</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1013</v>
+      </c>
       <c r="D15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E15"/>
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16"/>
+        <v>114</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1014</v>
+      </c>
       <c r="D16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16"/>
+        <v>192</v>
+      </c>
+      <c r="E16" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17"/>
+        <v>115</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1015</v>
+      </c>
       <c r="D17" t="s">
-        <v>166</v>
-      </c>
-      <c r="E17"/>
+        <v>194</v>
+      </c>
+      <c r="E17" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18"/>
+        <v>116</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1016</v>
+      </c>
       <c r="D18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E18"/>
+        <v>196</v>
+      </c>
+      <c r="E18" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19"/>
+        <v>117</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1017</v>
+      </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E19"/>
+        <v>198</v>
+      </c>
+      <c r="E19" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
-      </c>
-      <c r="C20"/>
+        <v>118</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1018</v>
+      </c>
       <c r="D20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E20"/>
+        <v>200</v>
+      </c>
+      <c r="E20" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21"/>
+        <v>119</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1019</v>
+      </c>
       <c r="D21" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21"/>
+        <v>202</v>
+      </c>
+      <c r="E21" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
-      </c>
-      <c r="C22"/>
+        <v>120</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1020</v>
+      </c>
       <c r="D22" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22"/>
+        <v>204</v>
+      </c>
+      <c r="E22" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C23"/>
+        <v>121</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1021</v>
+      </c>
       <c r="D23" t="s">
-        <v>178</v>
-      </c>
-      <c r="E23"/>
+        <v>206</v>
+      </c>
+      <c r="E23" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>179</v>
-      </c>
-      <c r="C24"/>
+        <v>122</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1022</v>
+      </c>
       <c r="D24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E24"/>
+        <v>208</v>
+      </c>
+      <c r="E24" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
-      </c>
-      <c r="C25"/>
+        <v>123</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1023</v>
+      </c>
       <c r="D25" t="s">
-        <v>182</v>
-      </c>
-      <c r="E25"/>
+        <v>210</v>
+      </c>
+      <c r="E25" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
-      </c>
-      <c r="C26"/>
+        <v>124</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1024</v>
+      </c>
       <c r="D26" t="s">
-        <v>184</v>
-      </c>
-      <c r="E26"/>
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27"/>
+        <v>125</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1025</v>
+      </c>
       <c r="D27" t="s">
-        <v>186</v>
-      </c>
-      <c r="E27"/>
+        <v>214</v>
+      </c>
+      <c r="E27" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28"/>
+        <v>126</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1026</v>
+      </c>
       <c r="D28" t="s">
-        <v>188</v>
-      </c>
-      <c r="E28"/>
+        <v>216</v>
+      </c>
+      <c r="E28" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C29"/>
+        <v>127</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1027</v>
+      </c>
       <c r="D29" t="s">
-        <v>190</v>
-      </c>
-      <c r="E29"/>
+        <v>218</v>
+      </c>
+      <c r="E29" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C30"/>
+        <v>128</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1028</v>
+      </c>
       <c r="D30" t="s">
-        <v>192</v>
-      </c>
-      <c r="E30"/>
+        <v>220</v>
+      </c>
+      <c r="E30" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>193</v>
-      </c>
-      <c r="C31"/>
+        <v>135</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1029</v>
+      </c>
       <c r="D31" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31"/>
+        <v>222</v>
+      </c>
+      <c r="E31" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
-      </c>
-      <c r="C32"/>
+        <v>136</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1030</v>
+      </c>
       <c r="D32" t="s">
-        <v>196</v>
-      </c>
-      <c r="E32"/>
+        <v>224</v>
+      </c>
+      <c r="E32" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>197</v>
-      </c>
-      <c r="C33"/>
+        <v>137</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1031</v>
+      </c>
       <c r="D33" t="s">
-        <v>198</v>
-      </c>
-      <c r="E33"/>
+        <v>226</v>
+      </c>
+      <c r="E33" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>199</v>
-      </c>
-      <c r="C34"/>
+        <v>138</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1032</v>
+      </c>
       <c r="D34" t="s">
-        <v>200</v>
-      </c>
-      <c r="E34"/>
+        <v>228</v>
+      </c>
+      <c r="E34" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>201</v>
-      </c>
-      <c r="C35"/>
+        <v>139</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1033</v>
+      </c>
       <c r="D35" t="s">
-        <v>202</v>
-      </c>
-      <c r="E35"/>
+        <v>230</v>
+      </c>
+      <c r="E35" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
-      </c>
-      <c r="C36"/>
+        <v>140</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1034</v>
+      </c>
       <c r="D36" t="s">
-        <v>204</v>
-      </c>
-      <c r="E36"/>
+        <v>232</v>
+      </c>
+      <c r="E36" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
-      </c>
-      <c r="C37"/>
+        <v>141</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1035</v>
+      </c>
       <c r="D37" t="s">
-        <v>206</v>
-      </c>
-      <c r="E37"/>
+        <v>234</v>
+      </c>
+      <c r="E37" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38"/>
+        <v>142</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1036</v>
+      </c>
       <c r="D38" t="s">
-        <v>208</v>
-      </c>
-      <c r="E38"/>
+        <v>236</v>
+      </c>
+      <c r="E38" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>209</v>
-      </c>
-      <c r="C39"/>
+        <v>143</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1037</v>
+      </c>
       <c r="D39" t="s">
-        <v>210</v>
-      </c>
-      <c r="E39"/>
+        <v>238</v>
+      </c>
+      <c r="E39" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>211</v>
-      </c>
-      <c r="C40"/>
+        <v>144</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1038</v>
+      </c>
       <c r="D40" t="s">
-        <v>212</v>
-      </c>
-      <c r="E40"/>
+        <v>240</v>
+      </c>
+      <c r="E40" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -11005,25 +11768,70 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>21</v>
+        <v>243</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>22</v>
+        <v>244</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="E2" t="e">
-        <f t="array" ref="E2">VLOOKUP(validations_integer!$A2,IF(dataelements!$E:$E="integer",dataelements!$F:$G),2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>366</v>
+      </c>
+      <c r="D2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8766</v>
+      </c>
+      <c r="D4" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -11034,6 +11842,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12076,19 +12887,68 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>251</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="C2" t="e">
-        <f t="array" ref="C2">VLOOKUP(validations_calendar!$A2,IF(dataelements!$E:$E="calendar",dataelements!$F:$G),2)</f>
-        <v>#N/A</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C6" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -12099,6 +12959,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId8"/>
+  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -13159,16 +14022,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>213</v>
+        <v>258</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>214</v>
+        <v>259</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2">
@@ -13176,13 +14039,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>217</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3">
@@ -13190,13 +14053,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
-        <v>220</v>
+        <v>265</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4">
@@ -13204,13 +14067,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5">
@@ -13218,13 +14081,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="D5" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6">
@@ -13232,13 +14095,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="D6" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7">
@@ -13246,13 +14109,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>275</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8">
@@ -13260,13 +14123,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
+        <v>277</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9">
@@ -13274,13 +14137,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C9" t="s">
-        <v>234</v>
+        <v>279</v>
       </c>
       <c r="D9" t="s">
-        <v>235</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10">
@@ -13288,13 +14151,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C10" t="s">
-        <v>236</v>
+        <v>281</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11">
@@ -13302,13 +14165,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>283</v>
       </c>
       <c r="D11" t="s">
-        <v>239</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12">
@@ -13316,13 +14179,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
-        <v>241</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13">
@@ -13330,13 +14193,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C13" t="s">
-        <v>242</v>
+        <v>287</v>
       </c>
       <c r="D13" t="s">
-        <v>243</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14">
@@ -13344,13 +14207,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C14" t="s">
-        <v>244</v>
+        <v>289</v>
       </c>
       <c r="D14" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15">
@@ -13358,13 +14221,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16">
@@ -13372,13 +14235,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C16" t="s">
-        <v>248</v>
+        <v>293</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17">
@@ -13386,13 +14249,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C17" t="s">
-        <v>250</v>
+        <v>295</v>
       </c>
       <c r="D17" t="s">
-        <v>251</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18">
@@ -13400,13 +14263,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C18" t="s">
-        <v>252</v>
+        <v>297</v>
       </c>
       <c r="D18" t="s">
-        <v>253</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19">
@@ -13414,13 +14277,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C19" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
       <c r="D19" t="s">
-        <v>255</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20">
@@ -13428,13 +14291,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>301</v>
       </c>
       <c r="D20" t="s">
-        <v>257</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21">
@@ -13442,13 +14305,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22">
@@ -13456,13 +14319,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C22" t="s">
-        <v>260</v>
+        <v>305</v>
       </c>
       <c r="D22" t="s">
-        <v>261</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23">
@@ -13470,13 +14333,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C23" t="s">
-        <v>262</v>
+        <v>307</v>
       </c>
       <c r="D23" t="s">
-        <v>263</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24">
@@ -13484,13 +14347,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C24" t="s">
-        <v>264</v>
+        <v>309</v>
       </c>
       <c r="D24" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25">
@@ -13498,13 +14361,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="D25" t="s">
-        <v>267</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26">
@@ -13512,13 +14375,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="D26" t="s">
-        <v>269</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27">
@@ -13526,13 +14389,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C27" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="D27" t="s">
-        <v>271</v>
+        <v>316</v>
       </c>
     </row>
     <row r="28">
@@ -13540,13 +14403,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C28" t="s">
-        <v>272</v>
+        <v>317</v>
       </c>
       <c r="D28" t="s">
-        <v>273</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29">
@@ -13554,13 +14417,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C29" t="s">
-        <v>274</v>
+        <v>319</v>
       </c>
       <c r="D29" t="s">
-        <v>275</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30">
@@ -13568,13 +14431,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C30" t="s">
-        <v>276</v>
+        <v>321</v>
       </c>
       <c r="D30" t="s">
-        <v>277</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31">
@@ -13582,13 +14445,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C31" t="s">
-        <v>278</v>
+        <v>323</v>
       </c>
       <c r="D31" t="s">
-        <v>279</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32">
@@ -13596,13 +14459,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C32" t="s">
-        <v>280</v>
+        <v>325</v>
       </c>
       <c r="D32" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33">
@@ -13610,13 +14473,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C33" t="s">
-        <v>282</v>
+        <v>327</v>
       </c>
       <c r="D33" t="s">
-        <v>283</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34">
@@ -13624,13 +14487,13 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C34" t="s">
-        <v>284</v>
+        <v>329</v>
       </c>
       <c r="D34" t="s">
-        <v>285</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35">
@@ -13638,13 +14501,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C35" t="s">
-        <v>286</v>
+        <v>331</v>
       </c>
       <c r="D35" t="s">
-        <v>287</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36">
@@ -13652,13 +14515,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
-        <v>288</v>
+        <v>333</v>
       </c>
       <c r="D36" t="s">
-        <v>289</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37">
@@ -13666,13 +14529,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>290</v>
+        <v>335</v>
       </c>
       <c r="D37" t="s">
-        <v>291</v>
+        <v>336</v>
       </c>
     </row>
     <row r="38">
@@ -13680,13 +14543,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C38" t="s">
-        <v>292</v>
+        <v>337</v>
       </c>
       <c r="D38" t="s">
-        <v>293</v>
+        <v>338</v>
       </c>
     </row>
     <row r="39">
@@ -13694,13 +14557,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s">
-        <v>294</v>
+        <v>339</v>
       </c>
       <c r="D39" t="s">
-        <v>295</v>
+        <v>340</v>
       </c>
     </row>
     <row r="40">
@@ -13708,13 +14571,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C40" t="s">
-        <v>296</v>
+        <v>341</v>
       </c>
       <c r="D40" t="s">
-        <v>297</v>
+        <v>342</v>
       </c>
     </row>
     <row r="41">
@@ -13722,13 +14585,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>298</v>
+        <v>343</v>
       </c>
       <c r="D41" t="s">
-        <v>299</v>
+        <v>344</v>
       </c>
     </row>
     <row r="42">
@@ -13736,13 +14599,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C42" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="D42" t="s">
-        <v>301</v>
+        <v>346</v>
       </c>
     </row>
     <row r="43">
@@ -13750,13 +14613,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C43" t="s">
-        <v>302</v>
+        <v>347</v>
       </c>
       <c r="D43" t="s">
-        <v>303</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44">
@@ -13764,13 +14627,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C44" t="s">
-        <v>304</v>
+        <v>349</v>
       </c>
       <c r="D44" t="s">
-        <v>305</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45">
@@ -13778,13 +14641,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C45" t="s">
-        <v>306</v>
+        <v>351</v>
       </c>
       <c r="D45" t="s">
-        <v>307</v>
+        <v>352</v>
       </c>
     </row>
     <row r="46">
@@ -13792,13 +14655,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C46" t="s">
-        <v>308</v>
+        <v>353</v>
       </c>
       <c r="D46" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
     </row>
     <row r="47">
@@ -13806,13 +14669,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C47" t="s">
-        <v>310</v>
+        <v>355</v>
       </c>
       <c r="D47" t="s">
-        <v>311</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48">
@@ -13820,13 +14683,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C48" t="s">
-        <v>312</v>
+        <v>357</v>
       </c>
       <c r="D48" t="s">
-        <v>313</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49">
@@ -13834,13 +14697,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C49" t="s">
-        <v>314</v>
+        <v>359</v>
       </c>
       <c r="D49" t="s">
-        <v>315</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50">
@@ -13848,13 +14711,13 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C50" t="s">
-        <v>316</v>
+        <v>361</v>
       </c>
       <c r="D50" t="s">
-        <v>317</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51">
@@ -13862,13 +14725,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="D51" t="s">
-        <v>319</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52">
@@ -13876,13 +14739,13 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C52" t="s">
-        <v>320</v>
+        <v>365</v>
       </c>
       <c r="D52" t="s">
-        <v>321</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53">
@@ -13890,13 +14753,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C53" t="s">
-        <v>322</v>
+        <v>367</v>
       </c>
       <c r="D53" t="s">
-        <v>323</v>
+        <v>368</v>
       </c>
     </row>
     <row r="54">
@@ -13904,13 +14767,13 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C54" t="s">
-        <v>324</v>
+        <v>369</v>
       </c>
       <c r="D54" t="s">
-        <v>325</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55">
@@ -13918,13 +14781,13 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C55" t="s">
-        <v>326</v>
+        <v>371</v>
       </c>
       <c r="D55" t="s">
-        <v>327</v>
+        <v>372</v>
       </c>
     </row>
     <row r="56">
@@ -13932,13 +14795,13 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C56" t="s">
-        <v>328</v>
+        <v>373</v>
       </c>
       <c r="D56" t="s">
-        <v>329</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57">
@@ -13946,13 +14809,13 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C57" t="s">
-        <v>330</v>
+        <v>375</v>
       </c>
       <c r="D57" t="s">
-        <v>331</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58">
@@ -13960,13 +14823,13 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C58" t="s">
-        <v>332</v>
+        <v>377</v>
       </c>
       <c r="D58" t="s">
-        <v>333</v>
+        <v>378</v>
       </c>
     </row>
     <row r="59">
@@ -13974,13 +14837,13 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C59" t="s">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="D59" t="s">
-        <v>335</v>
+        <v>380</v>
       </c>
     </row>
     <row r="60">
@@ -13988,13 +14851,13 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C60" t="s">
-        <v>336</v>
+        <v>381</v>
       </c>
       <c r="D60" t="s">
-        <v>337</v>
+        <v>382</v>
       </c>
     </row>
     <row r="61">
@@ -14002,13 +14865,13 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C61" t="s">
-        <v>338</v>
+        <v>383</v>
       </c>
       <c r="D61" t="s">
-        <v>339</v>
+        <v>384</v>
       </c>
     </row>
     <row r="62">
@@ -14016,13 +14879,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C62" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
       <c r="D62" t="s">
-        <v>341</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63">
@@ -14030,13 +14893,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C63" t="s">
-        <v>342</v>
+        <v>387</v>
       </c>
       <c r="D63" t="s">
-        <v>343</v>
+        <v>388</v>
       </c>
     </row>
     <row r="64">
@@ -14044,13 +14907,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C64" t="s">
-        <v>344</v>
+        <v>389</v>
       </c>
       <c r="D64" t="s">
-        <v>345</v>
+        <v>390</v>
       </c>
     </row>
     <row r="65">
@@ -14058,13 +14921,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C65" t="s">
-        <v>346</v>
+        <v>391</v>
       </c>
       <c r="D65" t="s">
-        <v>347</v>
+        <v>392</v>
       </c>
     </row>
     <row r="66">
@@ -14072,13 +14935,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C66" t="s">
-        <v>348</v>
+        <v>393</v>
       </c>
       <c r="D66" t="s">
-        <v>349</v>
+        <v>394</v>
       </c>
     </row>
     <row r="67">
@@ -14086,13 +14949,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C67" t="s">
-        <v>350</v>
+        <v>395</v>
       </c>
       <c r="D67" t="s">
-        <v>351</v>
+        <v>396</v>
       </c>
     </row>
     <row r="68">
@@ -14100,13 +14963,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C68" t="s">
-        <v>352</v>
+        <v>397</v>
       </c>
       <c r="D68" t="s">
-        <v>353</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69">
@@ -14114,13 +14977,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C69" t="s">
-        <v>354</v>
+        <v>399</v>
       </c>
       <c r="D69" t="s">
-        <v>355</v>
+        <v>400</v>
       </c>
     </row>
     <row r="70">
@@ -14128,13 +14991,13 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C70" t="s">
-        <v>356</v>
+        <v>401</v>
       </c>
       <c r="D70" t="s">
-        <v>357</v>
+        <v>402</v>
       </c>
     </row>
     <row r="71">
@@ -14142,13 +15005,13 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C71" t="s">
-        <v>358</v>
+        <v>403</v>
       </c>
       <c r="D71" t="s">
-        <v>359</v>
+        <v>404</v>
       </c>
     </row>
     <row r="72">
@@ -14156,13 +15019,13 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C72" t="s">
-        <v>360</v>
+        <v>405</v>
       </c>
       <c r="D72" t="s">
-        <v>361</v>
+        <v>406</v>
       </c>
     </row>
     <row r="73">
@@ -14170,13 +15033,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C73" t="s">
-        <v>362</v>
+        <v>407</v>
       </c>
       <c r="D73" t="s">
-        <v>363</v>
+        <v>408</v>
       </c>
     </row>
     <row r="74">
@@ -14184,13 +15047,13 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C74" t="s">
-        <v>364</v>
+        <v>409</v>
       </c>
       <c r="D74" t="s">
-        <v>365</v>
+        <v>410</v>
       </c>
     </row>
     <row r="75">
@@ -14198,13 +15061,13 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C75" t="s">
-        <v>366</v>
+        <v>411</v>
       </c>
       <c r="D75" t="s">
-        <v>367</v>
+        <v>412</v>
       </c>
     </row>
     <row r="76">
@@ -14212,13 +15075,13 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C76" t="s">
-        <v>368</v>
+        <v>413</v>
       </c>
       <c r="D76" t="s">
-        <v>369</v>
+        <v>414</v>
       </c>
     </row>
     <row r="77">
@@ -14226,13 +15089,13 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C77" t="s">
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="D77" t="s">
-        <v>371</v>
+        <v>416</v>
       </c>
     </row>
     <row r="78">
@@ -14240,13 +15103,13 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>261</v>
       </c>
       <c r="C78" t="s">
-        <v>372</v>
+        <v>417</v>
       </c>
       <c r="D78" t="s">
-        <v>373</v>
+        <v>418</v>
       </c>
     </row>
     <row r="79">
@@ -14254,13 +15117,13 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="C79" t="s">
-        <v>374</v>
+        <v>419</v>
       </c>
       <c r="D79" t="s">
-        <v>375</v>
+        <v>420</v>
       </c>
     </row>
     <row r="80">
@@ -14268,13 +15131,13 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
       <c r="C80" t="s">
-        <v>376</v>
+        <v>421</v>
       </c>
       <c r="D80" t="s">
-        <v>377</v>
+        <v>422</v>
       </c>
     </row>
     <row r="81">
@@ -14282,13 +15145,13 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>270</v>
       </c>
       <c r="C81" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
       <c r="D81" t="s">
-        <v>379</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -14310,7 +15173,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added email config; changed docker-compose files; added launchapp description
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -306,6 +306,25 @@
     <t xml:space="preserve">Diese Gruppe enthält die Datenelemente des Paragraph 21, die im Rahmen der DQ-Analyse geprüft werden.</t>
   </si>
   <si>
+    <t xml:space="preserve">Aufnahmeanlass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- E Einweisung durch einen Arzt 
+- Z Einweisung durch einen Zahnarzt 
+- N Notfall 
+- R Aufnahme nach vorausgehender Behandlung in einer Rehabilitationseinrichtung 
+- V Verlegung mit Behandlungsdauer im verlegenden Krankenhaus länger als 24 Stunden 
+- A Verlegung mit Behandlungsdauer im verlegenden Krankenhaus bis zu 24 Stunden  
+Zusatzschlüssel für besondere Kalkulationsanforderungen: 
+    - G Geburt (siehe Hinweis Neugeborene) 
+    - B Begleitperson oder mitaufgenommene Pflegekraft  
+Hinweise:  
+Einweisung durch einen Arzt ist im § 301-Aufnahmesatz im Segment Aufnahme durch die Arztnummer des einweisenden Arztes, Einweisung durch einen Zahnarzt durch die Zahnarztnummer des einweisenden Zahnarztes dokumentiert.  
+Verlegung ist im § 301-Aufnahmesatz durch das IK des die Aufnahme veranlassenden Krankenhauses dokumentiert. Wenn die Behandlungsdauer im verlegenden Krankenhaus nicht länger als 24 Stunden betrug ist als Aufnahmeanlass ‚A’, wenn sie länger als 24 Stunden betrug, ist ‚V’ anzugeben. Der Aufnahmeanlass ‚R’ wird in der § 301-Datenübermittlung nicht abgebildet, er soll übermittelt werden, wenn die Patientendatenhaltung dieses Zusatzmerkmal enthält.  
+Interne Verlegung mit Wechsel aus einem Entgeltbereich in einen anderen Entgeltbereich wird durch das eigene IK als IK des veranlassenden Krankenhauses dokumentiert.  
+Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
+  </si>
+  <si>
     <t xml:space="preserve">E</t>
   </si>
   <si>
@@ -355,10 +374,44 @@
 Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
   </si>
   <si>
+    <t xml:space="preserve">Diagnoseart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
+  </si>
+  <si>
     <t xml:space="preserve">HD</t>
   </si>
   <si>
     <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsgrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01x Behandlung regulär beendet 
+- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
+- 03x Behandlung aus sonstigen Gründen beendet 
+- 04x Behandlung gegen ärztlichen Rat beendet 
+- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
+- 069 Verlegung in ein anderes Krankenhaus 
+- 079 Tod 
+- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
+- 099 Entlassung in eine Rehabilitationseinrichtung 
+- 109 Entlassung in eine Pflegeeinrichtung 
+- 119 Entlassung in ein Hospiz 
+- 139 externe Verlegung zur psychiatrischen Behandlung 
+- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
+- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
+- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
+- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
+- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
+- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
+- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
+Hinweise:  
+Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
+Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
+Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
   </si>
   <si>
     <t xml:space="preserve">01x</t>
@@ -450,6 +503,14 @@
 Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
   </si>
   <si>
+    <t xml:space="preserve">Geschlecht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- m männlich  
+- w weiblich  
+- x unbestimmt  </t>
+  </si>
+  <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
@@ -457,6 +518,21 @@
   </si>
   <si>
     <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmegrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
+- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
+- 03xx Krankenhausbehandlung, teilstationär 
+- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
+- 05xx stationäre Entbindung 
+- 06xx Geburt 
+- 08xx Stationäre Aufnahme zur Organentnahme  
+Hinweise:  
+Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
+Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
   </si>
   <si>
     <t xml:space="preserve">01xx</t>
@@ -1538,8 +1614,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D56" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -6087,7 +6163,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>89</v>
@@ -6096,116 +6172,116 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B4" t="s">
         <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B5" t="s">
         <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B6" t="s">
         <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B7" t="s">
         <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B8" t="s">
         <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B9" t="s">
         <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B10" t="s">
         <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>1007</v>
       </c>
       <c r="B11" t="s">
         <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
         <v>101</v>
@@ -6213,7 +6289,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>89</v>
@@ -6227,7 +6303,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>89</v>
@@ -6241,7 +6317,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>89</v>
@@ -6255,7 +6331,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1008</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>89</v>
@@ -6264,326 +6340,326 @@
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1009</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B17" t="s">
         <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B18" t="s">
         <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1012</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B21" t="s">
         <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B31" t="s">
         <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="B33" t="s">
         <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="B34" t="s">
         <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="B35" t="s">
         <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>8</v>
+        <v>1026</v>
       </c>
       <c r="B36" t="s">
         <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>9</v>
+        <v>1027</v>
       </c>
       <c r="B37" t="s">
         <v>89</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>10</v>
+        <v>1028</v>
       </c>
       <c r="B38" t="s">
         <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D38" t="s">
         <v>134</v>
@@ -6591,7 +6667,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1029</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
         <v>89</v>
@@ -6600,200 +6676,200 @@
         <v>135</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1030</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
         <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1031</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1032</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>89</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1033</v>
+        <v>1029</v>
       </c>
       <c r="B43" t="s">
         <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="B44" t="s">
         <v>89</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1035</v>
+        <v>1031</v>
       </c>
       <c r="B45" t="s">
         <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1036</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
         <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1037</v>
+        <v>1032</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1038</v>
+        <v>1033</v>
       </c>
       <c r="B48" t="s">
         <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>13</v>
+        <v>1034</v>
       </c>
       <c r="B49" t="s">
         <v>89</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>14</v>
+        <v>1035</v>
       </c>
       <c r="B50" t="s">
         <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>15</v>
+        <v>1036</v>
       </c>
       <c r="B51" t="s">
         <v>89</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>16</v>
+        <v>1037</v>
       </c>
       <c r="B52" t="s">
         <v>89</v>
       </c>
       <c r="C52" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>17</v>
+        <v>1038</v>
       </c>
       <c r="B53" t="s">
         <v>89</v>
       </c>
       <c r="C53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D53" t="s">
         <v>154</v>
@@ -6801,7 +6877,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
         <v>89</v>
@@ -6815,7 +6891,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>89</v>
@@ -6829,7 +6905,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
         <v>89</v>
@@ -6839,6 +6915,76 @@
       </c>
       <c r="D56" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>17</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -7892,16 +8038,16 @@
         <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -7909,16 +8055,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" t="n">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3">
@@ -7926,16 +8072,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C3" t="n">
         <v>1001</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4">
@@ -7943,16 +8089,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C4" t="n">
         <v>1002</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5">
@@ -7960,16 +8106,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" t="n">
         <v>1003</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6">
@@ -7977,16 +8123,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C6" t="n">
         <v>1004</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7">
@@ -7994,16 +8140,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C7" t="n">
         <v>1005</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8">
@@ -8011,16 +8157,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C8" t="n">
         <v>1006</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9">
@@ -8028,16 +8174,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C9" t="n">
         <v>1007</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10">
@@ -8045,16 +8191,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C10" t="n">
         <v>1008</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11">
@@ -8062,16 +8208,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C11" t="n">
         <v>1009</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="E11" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12">
@@ -8079,16 +8225,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C12" t="n">
         <v>1010</v>
       </c>
       <c r="D12" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="E12" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13">
@@ -8096,16 +8242,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C13" t="n">
         <v>1011</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E13" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14">
@@ -8113,16 +8259,16 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C14" t="n">
         <v>1012</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15">
@@ -8130,16 +8276,16 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="C15" t="n">
         <v>1013</v>
       </c>
       <c r="D15" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16">
@@ -8147,16 +8293,16 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C16" t="n">
         <v>1014</v>
       </c>
       <c r="D16" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17">
@@ -8164,16 +8310,16 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C17" t="n">
         <v>1015</v>
       </c>
       <c r="D17" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="E17" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18">
@@ -8181,16 +8327,16 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C18" t="n">
         <v>1016</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E18" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19">
@@ -8198,16 +8344,16 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C19" t="n">
         <v>1017</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20">
@@ -8215,16 +8361,16 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C20" t="n">
         <v>1018</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21">
@@ -8232,16 +8378,16 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C21" t="n">
         <v>1019</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22">
@@ -8249,16 +8395,16 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C22" t="n">
         <v>1020</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="E22" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23">
@@ -8266,16 +8412,16 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C23" t="n">
         <v>1021</v>
       </c>
       <c r="D23" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E23" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24">
@@ -8283,16 +8429,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C24" t="n">
         <v>1022</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="E24" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25">
@@ -8300,16 +8446,16 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C25" t="n">
         <v>1023</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="E25" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26">
@@ -8317,16 +8463,16 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C26" t="n">
         <v>1024</v>
       </c>
       <c r="D26" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27">
@@ -8334,16 +8480,16 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C27" t="n">
         <v>1025</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E27" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28">
@@ -8351,16 +8497,16 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C28" t="n">
         <v>1026</v>
       </c>
       <c r="D28" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E28" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29">
@@ -8368,16 +8514,16 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C29" t="n">
         <v>1027</v>
       </c>
       <c r="D29" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="E29" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30">
@@ -8385,16 +8531,16 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C30" t="n">
         <v>1028</v>
       </c>
       <c r="D30" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="E30" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31">
@@ -8402,16 +8548,16 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C31" t="n">
         <v>1029</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="E31" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32">
@@ -8419,16 +8565,16 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C32" t="n">
         <v>1030</v>
       </c>
       <c r="D32" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E32" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33">
@@ -8436,16 +8582,16 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C33" t="n">
         <v>1031</v>
       </c>
       <c r="D33" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="E33" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34">
@@ -8453,16 +8599,16 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="C34" t="n">
         <v>1032</v>
       </c>
       <c r="D34" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="E34" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35">
@@ -8470,16 +8616,16 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C35" t="n">
         <v>1033</v>
       </c>
       <c r="D35" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="E35" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36">
@@ -8487,16 +8633,16 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="C36" t="n">
         <v>1034</v>
       </c>
       <c r="D36" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="E36" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37">
@@ -8504,16 +8650,16 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C37" t="n">
         <v>1035</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="E37" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38">
@@ -8521,16 +8667,16 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="C38" t="n">
         <v>1036</v>
       </c>
       <c r="D38" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39">
@@ -8538,16 +8684,16 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C39" t="n">
         <v>1037</v>
       </c>
       <c r="D39" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="E39" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="40">
@@ -8555,16 +8701,16 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C40" t="n">
         <v>1038</v>
       </c>
       <c r="D40" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="E40" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -11771,16 +11917,16 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -11794,10 +11940,10 @@
         <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
@@ -11811,10 +11957,10 @@
         <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4">
@@ -11828,10 +11974,10 @@
         <v>8766</v>
       </c>
       <c r="D4" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="E4" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -12890,10 +13036,10 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -12901,10 +13047,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3">
@@ -12912,10 +13058,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4">
@@ -12923,10 +13069,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5">
@@ -12934,10 +13080,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
@@ -12945,10 +13091,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -14022,16 +14168,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2">
@@ -14039,13 +14185,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3">
@@ -14053,13 +14199,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="D3" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
@@ -14067,13 +14213,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D4" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
@@ -14081,13 +14227,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D5" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="6">
@@ -14095,13 +14241,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="D6" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7">
@@ -14109,13 +14255,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C7" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="D7" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8">
@@ -14123,13 +14269,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C8" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="D8" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9">
@@ -14137,13 +14283,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C9" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D9" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10">
@@ -14151,13 +14297,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C10" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11">
@@ -14165,13 +14311,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12">
@@ -14179,13 +14325,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C12" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D12" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13">
@@ -14193,13 +14339,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C13" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="D13" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14">
@@ -14207,13 +14353,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="D14" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15">
@@ -14221,13 +14367,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C15" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="D15" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16">
@@ -14235,13 +14381,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C16" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="D16" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17">
@@ -14249,13 +14395,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="D17" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18">
@@ -14263,13 +14409,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C18" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="D18" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19">
@@ -14277,13 +14423,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C19" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="D19" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20">
@@ -14291,13 +14437,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C20" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="D20" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21">
@@ -14305,13 +14451,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="D21" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22">
@@ -14319,13 +14465,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="D22" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="23">
@@ -14333,13 +14479,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C23" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="D23" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24">
@@ -14347,13 +14493,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C24" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="D24" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25">
@@ -14361,13 +14507,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C25" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="D25" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26">
@@ -14375,13 +14521,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C26" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="D26" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="27">
@@ -14389,13 +14535,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C27" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="D27" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28">
@@ -14403,13 +14549,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C28" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="D28" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29">
@@ -14417,13 +14563,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C29" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="D29" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
     </row>
     <row r="30">
@@ -14431,13 +14577,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C30" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="D30" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
     </row>
     <row r="31">
@@ -14445,13 +14591,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C31" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="D31" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32">
@@ -14459,13 +14605,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C32" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D32" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
     </row>
     <row r="33">
@@ -14473,13 +14619,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C33" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="D33" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34">
@@ -14487,13 +14633,13 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C34" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="D34" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35">
@@ -14501,13 +14647,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C35" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="D35" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="36">
@@ -14515,13 +14661,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C36" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
     </row>
     <row r="37">
@@ -14529,13 +14675,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C37" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="D37" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38">
@@ -14543,13 +14689,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="D38" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
     </row>
     <row r="39">
@@ -14557,13 +14703,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C39" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="D39" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40">
@@ -14571,13 +14717,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C40" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="D40" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41">
@@ -14585,13 +14731,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C41" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="D41" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42">
@@ -14599,13 +14745,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C42" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="D42" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="43">
@@ -14613,13 +14759,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C43" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="D43" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44">
@@ -14627,13 +14773,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C44" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45">
@@ -14641,13 +14787,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C45" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="D45" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46">
@@ -14655,13 +14801,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C46" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="D46" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
     </row>
     <row r="47">
@@ -14669,13 +14815,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C47" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="D47" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
     </row>
     <row r="48">
@@ -14683,13 +14829,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C48" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="D48" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
     </row>
     <row r="49">
@@ -14697,13 +14843,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C49" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="D49" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50">
@@ -14711,13 +14857,13 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C50" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="D50" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
     </row>
     <row r="51">
@@ -14725,13 +14871,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C51" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="D51" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
     </row>
     <row r="52">
@@ -14739,13 +14885,13 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C52" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="D52" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53">
@@ -14753,13 +14899,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C53" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="D53" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
     </row>
     <row r="54">
@@ -14767,13 +14913,13 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C54" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="D54" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
     </row>
     <row r="55">
@@ -14781,13 +14927,13 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C55" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="D55" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
     </row>
     <row r="56">
@@ -14795,13 +14941,13 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C56" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="D56" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
     </row>
     <row r="57">
@@ -14809,13 +14955,13 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C57" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="D57" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
     </row>
     <row r="58">
@@ -14823,13 +14969,13 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C58" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="D58" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59">
@@ -14837,13 +14983,13 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C59" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="D59" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="60">
@@ -14851,13 +14997,13 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C60" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="D60" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61">
@@ -14865,13 +15011,13 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C61" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="D61" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
     </row>
     <row r="62">
@@ -14879,13 +15025,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C62" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="D62" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63">
@@ -14893,13 +15039,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C63" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="D63" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
     </row>
     <row r="64">
@@ -14907,13 +15053,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C64" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="D64" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
     </row>
     <row r="65">
@@ -14921,13 +15067,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C65" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="D65" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
     </row>
     <row r="66">
@@ -14935,13 +15081,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C66" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="D66" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
     </row>
     <row r="67">
@@ -14949,13 +15095,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C67" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="D67" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
     </row>
     <row r="68">
@@ -14963,13 +15109,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C68" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="D68" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="69">
@@ -14977,13 +15123,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C69" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="D69" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
     </row>
     <row r="70">
@@ -14991,13 +15137,13 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C70" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="D70" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
     </row>
     <row r="71">
@@ -15005,13 +15151,13 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C71" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="D71" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
     </row>
     <row r="72">
@@ -15019,13 +15165,13 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C72" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="D72" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
     </row>
     <row r="73">
@@ -15033,13 +15179,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C73" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="D73" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
     </row>
     <row r="74">
@@ -15047,13 +15193,13 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C74" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="D74" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row r="75">
@@ -15061,13 +15207,13 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C75" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="D75" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76">
@@ -15075,13 +15221,13 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C76" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="D76" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77">
@@ -15089,13 +15235,13 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C77" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="D77" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
     </row>
     <row r="78">
@@ -15103,13 +15249,13 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="C78" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="D78" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79">
@@ -15117,13 +15263,13 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="C79" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="D79" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
     </row>
     <row r="80">
@@ -15131,13 +15277,13 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="C80" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="D80" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
     </row>
     <row r="81">
@@ -15145,13 +15291,13 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C81" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="D81" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added regex to samply xlsx
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="449">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -851,6 +851,48 @@
     <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">max_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:alnum:]]){1,}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{5})$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">range_from</t>
   </si>
   <si>
@@ -920,7 +962,7 @@
     <t xml:space="preserve">p21csv</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_source"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["AUFNAHMEANLASS"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.admission_source"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["AUFNAHMEANLASS"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
@@ -929,7 +971,7 @@
     <t xml:space="preserve">i2b2</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNAN%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNAN%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
@@ -938,7 +980,7 @@
     <t xml:space="preserve">omop</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"E, Z, N, R, V, A, G, B\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
@@ -950,19 +992,19 @@
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_source"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_TAGEN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0]}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_source"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_TAGEN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AITAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AITAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 366, \"unit\": \"d\"}}"],"value_threshold":[0],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 8512"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 8512"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
@@ -974,19 +1016,19 @@
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_source"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_JAHREN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5]}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_source"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_JAHREN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AIJAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AIJAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 110, \"unit\": \"a\"}}"],"value_threshold":[5],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 9448"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 9448"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
@@ -998,19 +1040,19 @@
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_source"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["GEBURTSJAHR"],"source_table_name":["FALL.CSV"]}</t>
+    <t xml:space="preserve">{"key":["dt.birthdate_source"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["GEBURTSJAHR"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["birth_date"],"source_table_name":["patient_dimension"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["birth_date"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["year_of_birth"],"source_table_name":["person"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["year_of_birth"],"source_table_name":["person"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
@@ -1022,19 +1064,19 @@
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.condition_source"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["ICD_Kode"],"source_table_name":["ICD.CSV"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["ICD.CSV"],"fhir":["condition.encounter.identifier.value"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.condition_source"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["ICD_Kode"],"source_table_name":["ICD.CSV"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["ICD.CSV"],"fhir":["condition.encounter.identifier.value"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["condition_source_value"],"source_table_name":["condition_occurrence"],"data_map":[1],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["condition_source_value"],"source_table_name":["condition_occurrence"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"data_map":[1],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
@@ -1046,19 +1088,19 @@
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_source"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["Diagnoseart"],"source_table_name":["ICD.CSV"],"constraints":["{\"value_set\": \"HD, ND\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_source"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["Diagnoseart"],"source_table_name":["ICD.CSV"],"constraints":["{\"value_set\":[\"HD, ND\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["modifier_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"HD, ND\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["modifier_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"HD, ND\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A24;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["condition_type_concept_id"],"source_table_name":["condition_occurrence"],"constraints":["{\"value_set\": \"44786627, 44786629\"}"],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["condition_occurrence"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["condition_type_concept_id"],"source_table_name":["condition_occurrence"],"constraints":["{\"value_set\":[\"44786627, 44786629\"]}"],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["condition_occurrence"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A25;dataelements!A:G;7;FALSCH)</t>
@@ -1070,43 +1112,43 @@
     <t xml:space="preserve">=SVERWEIS($A26;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_source"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["ENTLASSUNGSGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_source"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["ENTLASSUNGSGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A27;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ENTLGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ENTLGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A28;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"}"],"sql_from":["observation"],"sql_where":["observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"],"sql_from":["observation"],"sql_where":["observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A29;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\": {\"patient_identifier_value\": {\"name\": \"Pl.uniqueness.Item02\", \"description\": \"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A30;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.encounter_source"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FALL.CSV"],"data_map":[1]}</t>
+    <t xml:space="preserve">{"key":["dt.encounter_source"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A31;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["encounter_num"],"source_table_name":["visit_dimension"],"data_map":[1],"sql_from":["visit_dimension"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["visit_dimension"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_dimension"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["encounter_num"],"source_table_name":["visit_dimension"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["visit_dimension"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["visit_dimension"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_dimension"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A32;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"data_map":[1],"sql_from":["visit_occurence"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["visit_occurence"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A33;dataelements!A:G;7;FALSCH)</t>
@@ -1160,25 +1202,25 @@
     <t xml:space="preserve">=SVERWEIS($A41;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\": {\"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item01\", \"description\": \"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"O[0-9]\", \"i2b2\": \"O[0-9]\", \"p21csv\": \"O[0-9]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\": {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item02\", \"description\": \"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C5[1-8]\", \"i2b2\": \"C5[1-8]\", \"p21csv\": \"C5[1-8]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}, \"condition_code_coding_code\": {\"name\": \"Pl.atemporal.Item03\", \"description\": \"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\", \"filter\": {\"omop\": \"C6[0-3]\", \"i2b2\": \"C6[0-3]\", \"p21csv\": \"C6[0-3]\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"m\", \"i2b2\": \"m\", \"p21csv\": \"m\"}}}, \"encounter_hospitalization_class\": {\"name\": \"Pl.atemporal.Item04\", \"description\": \"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\", \"filter\": {\"omop\": \"05xx\", \"i2b2\": \"05xx\", \"p21csv\": \"05xx\"}, \"join_crit\": \"encounter_identifier_value\", \"constraints\": {\"value_set\":  {\"omop\": \"w\", \"i2b2\": \"w\", \"p21csv\": \"w\"}}}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A42;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_source"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["GESCHLECHT"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"m, w, x\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.gender_source"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["GESCHLECHT"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"m, w, x\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A43;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["sex_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"value_set\": \"m, w, x\"}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["sex_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"value_set\":[\"m, w, x\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A44;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["gender_source_value"],"source_table_name":["person"],"constraints":["{\"value_set\": \"m, w, x\"}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["gender_source_value"],"source_table_name":["person"],"constraints":["{\"value_set\":[\"m, w, x\"]}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A45;dataelements!A:G;7;FALSCH)</t>
@@ -1190,43 +1232,43 @@
     <t xml:space="preserve">=SVERWEIS($A46;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_source"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["AUFNAHMEGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"]}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_source"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["AUFNAHMEGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A47;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A48;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\": \"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A49;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\": {\"patient_birthDate\": {\"name\": \"Pl.uniqueness.Item01\", \"description\": \"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"}}}"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A50;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.patient_source"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["PATIENTENNUMMER"],"source_table_name":["FALL.CSV"],"data_map":[1]}</t>
+    <t xml:space="preserve">{"key":["dt.patient_source"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["PATIENTENNUMMER"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A51;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"data_map":[1],"sql_from":["patient_dimension"]}</t>
+    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["patient_dimension"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A52;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["person_id"],"source_table_name":["person"],"data_map":[1],"sql_from":["observation"]}</t>
+    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["person_id"],"source_table_name":["person"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["observation"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A53;dataelements!A:G;7;FALSCH)</t>
@@ -1238,19 +1280,19 @@
     <t xml:space="preserve">=SVERWEIS($A54;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.procedure_source"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["OPS_Kode"],"source_table_name":["OPS.CSV"],"data_map":[1],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["OPS.CSV"],"fhir":["procedure.encounter.identifier.value"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.procedure_source"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["OPS_Kode"],"source_table_name":["OPS.CSV"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["OPS.CSV"],"fhir":["procedure.encounter.identifier.value"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A55;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'OPS%'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'OPS%'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A56;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["procedure_source_value"],"source_table_name":["procedure_occurrence"],"data_map":[1],"sql_from":["procedure_occurrence"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["procedure_occurrence"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["procedure_source_value"],"source_table_name":["procedure_occurrence"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"sql_from":["procedure_occurrence"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["procedure_occurrence"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A57;dataelements!A:G;7;FALSCH)</t>
@@ -1286,19 +1328,19 @@
     <t xml:space="preserve">=SVERWEIS($A62;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.provider_source"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["FAB"],"source_table_name":["FAB.CSV"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FAB.CSV"],"fhir":["encounter.identifier.value"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.provider_source"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["FAB"],"source_table_name":["FAB.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FAB.CSV"],"fhir":["encounter.identifier.value"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A63;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["tval_char"],"source_table_name":["observation_fact"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FACHABT%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["tval_char"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FACHABT%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A64;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["care_site_id"],"source_table_name":["visit_occurrence"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurrence"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["care_site_id"],"source_table_name":["visit_occurrence"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurrence"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A65;dataelements!A:G;7;FALSCH)</t>
@@ -1358,19 +1400,19 @@
     <t xml:space="preserve">=SVERWEIS($A74;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_source"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["BEATMUNGSSTUNDEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"]}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_source"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["BEATMUNGSSTUNDEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A75;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:BEATMST'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:BEATMST'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A76;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\": {\"min\": 0, \"max\": 8766, \"unit\": \"h\"}}"],"sql_from":["observation"],"sql_where":["observation_concept_id = 4108449"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"],"sql_from":["observation"],"sql_where":["observation_concept_id = 4108449"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A77;dataelements!A:G;7;FALSCH)</t>
@@ -1382,19 +1424,19 @@
     <t xml:space="preserve">=SVERWEIS($A78;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_source"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["PLZ"],"source_table_name":["FALL.CSV"]}</t>
+    <t xml:space="preserve">{"key":["dt.zipcode_source"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["PLZ"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"]}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A79;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip_cd"],"source_table_name":["patient_dimension"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A80;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip"],"source_table_name":["location"],"sql_from":["location"],"sql_join_on":["location_id"],"sql_join_type":["left outer"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
+    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip"],"source_table_name":["location"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"],"sql_from":["location"],"sql_join_on":["location_id"],"sql_join_type":["left outer"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A81;dataelements!A:G;7;FALSCH)</t>
@@ -1586,6 +1628,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D81"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="dataelement_id"/>
+    <tableColumn id="2" name="key"/>
+    <tableColumn id="3" name="value"/>
+    <tableColumn id="4" name="Designation of date element (first defined language)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B2" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:B2"/>
@@ -1641,7 +1696,20 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="max_length"/>
+    <tableColumn id="3" name="regex"/>
+    <tableColumn id="4" name="Designation of data element (in first defined language)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
@@ -1654,26 +1722,13 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="format"/>
     <tableColumn id="3" name="Designation of data element (in first defined language)"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D81"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="dataelement_id"/>
-    <tableColumn id="2" name="key"/>
-    <tableColumn id="3" name="value"/>
-    <tableColumn id="4" name="Designation of date element (first defined language)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4309,7 +4364,9 @@
       <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="F6"/>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>67</v>
       </c>
@@ -4330,7 +4387,9 @@
       <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="F7"/>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>68</v>
       </c>
@@ -4397,7 +4456,9 @@
       <c r="E10" t="s">
         <v>66</v>
       </c>
-      <c r="F10"/>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>71</v>
       </c>
@@ -4510,7 +4571,9 @@
       <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="F15"/>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>77</v>
       </c>
@@ -4531,7 +4594,9 @@
       <c r="E16" t="s">
         <v>66</v>
       </c>
-      <c r="F16"/>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>78</v>
       </c>
@@ -4575,7 +4640,9 @@
       <c r="E18" t="s">
         <v>66</v>
       </c>
-      <c r="F18"/>
+      <c r="F18" t="n">
+        <v>6</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>80</v>
       </c>
@@ -4665,7 +4732,9 @@
       <c r="E22" t="s">
         <v>66</v>
       </c>
-      <c r="F22"/>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
       <c r="G22" s="1" t="s">
         <v>84</v>
       </c>
@@ -9766,23 +9835,101 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>252</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="D2" t="e">
-        <f t="array" ref="D2">VLOOKUP(validations_string!$A2,IF(dataelements!$E:$E="string",dataelements!$F:$G),2,FALSE)</f>
-        <v>#N/A</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -9798,6 +9945,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11917,13 +12067,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>172</v>
@@ -11940,10 +12090,10 @@
         <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3">
@@ -11957,10 +12107,10 @@
         <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
@@ -11974,10 +12124,10 @@
         <v>8766</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="E4" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -11989,7 +12139,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
@@ -13036,7 +13186,7 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>172</v>
@@ -13047,10 +13197,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3">
@@ -13058,10 +13208,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4">
@@ -13069,10 +13219,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5">
@@ -13080,10 +13230,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6">
@@ -13091,10 +13241,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -13106,7 +13256,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -14168,16 +14318,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>171</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
@@ -14185,13 +14335,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="D2" t="s">
-        <v>273</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3">
@@ -14199,13 +14349,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4">
@@ -14213,13 +14363,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C4" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5">
@@ -14227,13 +14377,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="D5" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6">
@@ -14241,13 +14391,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="D6" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7">
@@ -14255,13 +14405,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="D7" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8">
@@ -14269,13 +14419,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="D8" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9">
@@ -14283,13 +14433,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10">
@@ -14297,13 +14447,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="D10" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11">
@@ -14311,13 +14461,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12">
@@ -14325,13 +14475,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C12" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="D12" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
     <row r="13">
@@ -14339,13 +14489,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C13" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="D13" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14">
@@ -14353,13 +14503,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C14" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="D14" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15">
@@ -14367,13 +14517,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C15" t="s">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="D15" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16">
@@ -14381,13 +14531,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C16" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="D16" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
     </row>
     <row r="17">
@@ -14395,13 +14545,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C17" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="D17" t="s">
-        <v>306</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18">
@@ -14409,13 +14559,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="D18" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
     </row>
     <row r="19">
@@ -14423,13 +14573,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C19" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="D19" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
     </row>
     <row r="20">
@@ -14437,13 +14587,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C20" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="D20" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21">
@@ -14451,13 +14601,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C21" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="D21" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22">
@@ -14465,13 +14615,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C22" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="D22" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
     </row>
     <row r="23">
@@ -14479,13 +14629,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C23" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="D23" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24">
@@ -14493,13 +14643,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C24" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="D24" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
     </row>
     <row r="25">
@@ -14507,13 +14657,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C25" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="D25" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26">
@@ -14521,13 +14671,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C26" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="D26" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27">
@@ -14535,13 +14685,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C27" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="D27" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28">
@@ -14549,13 +14699,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C28" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="D28" t="s">
-        <v>328</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29">
@@ -14563,13 +14713,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C29" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="D29" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
     </row>
     <row r="30">
@@ -14577,13 +14727,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C30" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="D30" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31">
@@ -14591,13 +14741,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C31" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="D31" t="s">
-        <v>334</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32">
@@ -14605,13 +14755,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C32" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="D32" t="s">
-        <v>336</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33">
@@ -14619,13 +14769,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C33" t="s">
-        <v>337</v>
+        <v>351</v>
       </c>
       <c r="D33" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
     </row>
     <row r="34">
@@ -14633,13 +14783,13 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C34" t="s">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="D34" t="s">
-        <v>340</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35">
@@ -14647,13 +14797,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C35" t="s">
-        <v>341</v>
+        <v>355</v>
       </c>
       <c r="D35" t="s">
-        <v>342</v>
+        <v>356</v>
       </c>
     </row>
     <row r="36">
@@ -14661,13 +14811,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C36" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="D36" t="s">
-        <v>344</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37">
@@ -14675,13 +14825,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C37" t="s">
-        <v>345</v>
+        <v>359</v>
       </c>
       <c r="D37" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38">
@@ -14689,13 +14839,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C38" t="s">
-        <v>347</v>
+        <v>361</v>
       </c>
       <c r="D38" t="s">
-        <v>348</v>
+        <v>362</v>
       </c>
     </row>
     <row r="39">
@@ -14703,13 +14853,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C39" t="s">
-        <v>349</v>
+        <v>363</v>
       </c>
       <c r="D39" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40">
@@ -14717,13 +14867,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C40" t="s">
-        <v>351</v>
+        <v>365</v>
       </c>
       <c r="D40" t="s">
-        <v>352</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41">
@@ -14731,13 +14881,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C41" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="D41" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42">
@@ -14745,13 +14895,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C42" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
       <c r="D42" t="s">
-        <v>356</v>
+        <v>370</v>
       </c>
     </row>
     <row r="43">
@@ -14759,13 +14909,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C43" t="s">
-        <v>357</v>
+        <v>371</v>
       </c>
       <c r="D43" t="s">
-        <v>358</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44">
@@ -14773,13 +14923,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C44" t="s">
-        <v>359</v>
+        <v>373</v>
       </c>
       <c r="D44" t="s">
-        <v>360</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45">
@@ -14787,13 +14937,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C45" t="s">
-        <v>361</v>
+        <v>375</v>
       </c>
       <c r="D45" t="s">
-        <v>362</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46">
@@ -14801,13 +14951,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C46" t="s">
-        <v>363</v>
+        <v>377</v>
       </c>
       <c r="D46" t="s">
-        <v>364</v>
+        <v>378</v>
       </c>
     </row>
     <row r="47">
@@ -14815,13 +14965,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C47" t="s">
-        <v>365</v>
+        <v>379</v>
       </c>
       <c r="D47" t="s">
-        <v>366</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48">
@@ -14829,13 +14979,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C48" t="s">
-        <v>367</v>
+        <v>381</v>
       </c>
       <c r="D48" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49">
@@ -14843,13 +14993,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C49" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="D49" t="s">
-        <v>370</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50">
@@ -14857,13 +15007,13 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C50" t="s">
-        <v>371</v>
+        <v>385</v>
       </c>
       <c r="D50" t="s">
-        <v>372</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51">
@@ -14871,13 +15021,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C51" t="s">
-        <v>373</v>
+        <v>387</v>
       </c>
       <c r="D51" t="s">
-        <v>374</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52">
@@ -14885,13 +15035,13 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C52" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="D52" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53">
@@ -14899,13 +15049,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C53" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="D53" t="s">
-        <v>378</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54">
@@ -14913,13 +15063,13 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C54" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="D54" t="s">
-        <v>380</v>
+        <v>394</v>
       </c>
     </row>
     <row r="55">
@@ -14927,13 +15077,13 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C55" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="D55" t="s">
-        <v>382</v>
+        <v>396</v>
       </c>
     </row>
     <row r="56">
@@ -14941,13 +15091,13 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C56" t="s">
-        <v>383</v>
+        <v>397</v>
       </c>
       <c r="D56" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
     </row>
     <row r="57">
@@ -14955,13 +15105,13 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C57" t="s">
-        <v>385</v>
+        <v>399</v>
       </c>
       <c r="D57" t="s">
-        <v>386</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58">
@@ -14969,13 +15119,13 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C58" t="s">
-        <v>387</v>
+        <v>401</v>
       </c>
       <c r="D58" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
     </row>
     <row r="59">
@@ -14983,13 +15133,13 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C59" t="s">
-        <v>389</v>
+        <v>403</v>
       </c>
       <c r="D59" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
     </row>
     <row r="60">
@@ -14997,13 +15147,13 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C60" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="D60" t="s">
-        <v>392</v>
+        <v>406</v>
       </c>
     </row>
     <row r="61">
@@ -15011,13 +15161,13 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C61" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="D61" t="s">
-        <v>394</v>
+        <v>408</v>
       </c>
     </row>
     <row r="62">
@@ -15025,13 +15175,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C62" t="s">
-        <v>395</v>
+        <v>409</v>
       </c>
       <c r="D62" t="s">
-        <v>396</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63">
@@ -15039,13 +15189,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C63" t="s">
-        <v>397</v>
+        <v>411</v>
       </c>
       <c r="D63" t="s">
-        <v>398</v>
+        <v>412</v>
       </c>
     </row>
     <row r="64">
@@ -15053,13 +15203,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C64" t="s">
-        <v>399</v>
+        <v>413</v>
       </c>
       <c r="D64" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65">
@@ -15067,13 +15217,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C65" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="D65" t="s">
-        <v>402</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66">
@@ -15081,13 +15231,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C66" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="D66" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
     </row>
     <row r="67">
@@ -15095,13 +15245,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C67" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="D67" t="s">
-        <v>406</v>
+        <v>420</v>
       </c>
     </row>
     <row r="68">
@@ -15109,13 +15259,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C68" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="D68" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
     </row>
     <row r="69">
@@ -15123,13 +15273,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C69" t="s">
-        <v>409</v>
+        <v>423</v>
       </c>
       <c r="D69" t="s">
-        <v>410</v>
+        <v>424</v>
       </c>
     </row>
     <row r="70">
@@ -15137,13 +15287,13 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C70" t="s">
-        <v>411</v>
+        <v>425</v>
       </c>
       <c r="D70" t="s">
-        <v>412</v>
+        <v>426</v>
       </c>
     </row>
     <row r="71">
@@ -15151,13 +15301,13 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C71" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="D71" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
     </row>
     <row r="72">
@@ -15165,13 +15315,13 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C72" t="s">
-        <v>415</v>
+        <v>429</v>
       </c>
       <c r="D72" t="s">
-        <v>416</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73">
@@ -15179,13 +15329,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C73" t="s">
-        <v>417</v>
+        <v>431</v>
       </c>
       <c r="D73" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
     </row>
     <row r="74">
@@ -15193,13 +15343,13 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C74" t="s">
-        <v>419</v>
+        <v>433</v>
       </c>
       <c r="D74" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75">
@@ -15207,13 +15357,13 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C75" t="s">
-        <v>421</v>
+        <v>435</v>
       </c>
       <c r="D75" t="s">
-        <v>422</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76">
@@ -15221,13 +15371,13 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C76" t="s">
-        <v>423</v>
+        <v>437</v>
       </c>
       <c r="D76" t="s">
-        <v>424</v>
+        <v>438</v>
       </c>
     </row>
     <row r="77">
@@ -15235,13 +15385,13 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C77" t="s">
-        <v>425</v>
+        <v>439</v>
       </c>
       <c r="D77" t="s">
-        <v>426</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78">
@@ -15249,13 +15399,13 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="C78" t="s">
-        <v>427</v>
+        <v>441</v>
       </c>
       <c r="D78" t="s">
-        <v>428</v>
+        <v>442</v>
       </c>
     </row>
     <row r="79">
@@ -15263,13 +15413,13 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="C79" t="s">
-        <v>429</v>
+        <v>443</v>
       </c>
       <c r="D79" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
     </row>
     <row r="80">
@@ -15277,13 +15427,13 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="C80" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="D80" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
     </row>
     <row r="81">
@@ -15291,13 +15441,13 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="C81" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="D81" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -15319,7 +15469,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated string representation in xlsx
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="450">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -855,6 +855,9 @@
   </si>
   <si>
     <t xml:space="preserve">regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
     <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
@@ -9852,84 +9855,98 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2"/>
+      <c r="B2" t="s">
+        <v>254</v>
+      </c>
       <c r="C2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3"/>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
       <c r="C3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
       <c r="C5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
       <c r="C6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7"/>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
       <c r="C7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8"/>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -12067,13 +12084,13 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>172</v>
@@ -12090,10 +12107,10 @@
         <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
@@ -12107,10 +12124,10 @@
         <v>110</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4">
@@ -12124,10 +12141,10 @@
         <v>8766</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -13186,7 +13203,7 @@
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>172</v>
@@ -13197,10 +13214,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3">
@@ -13208,10 +13225,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4">
@@ -13219,10 +13236,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5">
@@ -13230,10 +13247,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6">
@@ -13241,10 +13258,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C6" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -14318,16 +14335,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>171</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
@@ -14335,13 +14352,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3">
@@ -14349,13 +14366,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4">
@@ -14363,13 +14380,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5">
@@ -14377,13 +14394,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="6">
@@ -14391,13 +14408,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7">
@@ -14405,13 +14422,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D7" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8">
@@ -14419,13 +14436,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9">
@@ -14433,13 +14450,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D9" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10">
@@ -14447,13 +14464,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C10" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11">
@@ -14461,13 +14478,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12">
@@ -14475,13 +14492,13 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C12" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D12" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13">
@@ -14489,13 +14506,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14">
@@ -14503,13 +14520,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15">
@@ -14517,13 +14534,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D15" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16">
@@ -14531,13 +14548,13 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C16" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="17">
@@ -14545,13 +14562,13 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C17" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D17" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="18">
@@ -14559,13 +14576,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D18" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19">
@@ -14573,13 +14590,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D19" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20">
@@ -14587,13 +14604,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C20" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D20" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21">
@@ -14601,13 +14618,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C21" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D21" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22">
@@ -14615,13 +14632,13 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C22" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D22" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23">
@@ -14629,13 +14646,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C23" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D23" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24">
@@ -14643,13 +14660,13 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C24" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D24" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25">
@@ -14657,13 +14674,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C25" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D25" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26">
@@ -14671,13 +14688,13 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C26" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D26" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27">
@@ -14685,13 +14702,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D27" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28">
@@ -14699,13 +14716,13 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C28" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D28" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29">
@@ -14713,13 +14730,13 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C29" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D29" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30">
@@ -14727,13 +14744,13 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C30" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D30" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="31">
@@ -14741,13 +14758,13 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C31" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D31" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32">
@@ -14755,13 +14772,13 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C32" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="33">
@@ -14769,13 +14786,13 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C33" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D33" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="34">
@@ -14783,13 +14800,13 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C34" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D34" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35">
@@ -14797,13 +14814,13 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C35" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D35" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36">
@@ -14811,13 +14828,13 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C36" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D36" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37">
@@ -14825,13 +14842,13 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C37" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D37" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38">
@@ -14839,13 +14856,13 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C38" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D38" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39">
@@ -14853,13 +14870,13 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C39" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D39" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40">
@@ -14867,13 +14884,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C40" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D40" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="41">
@@ -14881,13 +14898,13 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C41" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D41" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="42">
@@ -14895,13 +14912,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D42" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43">
@@ -14909,13 +14926,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C43" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D43" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44">
@@ -14923,13 +14940,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C44" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D44" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="45">
@@ -14937,13 +14954,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C45" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D45" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46">
@@ -14951,13 +14968,13 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D46" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47">
@@ -14965,13 +14982,13 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C47" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D47" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48">
@@ -14979,13 +14996,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C48" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D48" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49">
@@ -14993,13 +15010,13 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C49" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D49" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="50">
@@ -15007,13 +15024,13 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C50" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D50" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="51">
@@ -15021,13 +15038,13 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C51" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D51" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="52">
@@ -15035,13 +15052,13 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C52" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D52" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="53">
@@ -15049,13 +15066,13 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C53" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D53" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54">
@@ -15063,13 +15080,13 @@
         <v>14</v>
       </c>
       <c r="B54" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C54" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D54" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="55">
@@ -15077,13 +15094,13 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C55" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D55" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56">
@@ -15091,13 +15108,13 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C56" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D56" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57">
@@ -15105,13 +15122,13 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C57" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D57" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="58">
@@ -15119,13 +15136,13 @@
         <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C58" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D58" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="59">
@@ -15133,13 +15150,13 @@
         <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D59" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="60">
@@ -15147,13 +15164,13 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C60" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D60" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61">
@@ -15161,13 +15178,13 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C61" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D61" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62">
@@ -15175,13 +15192,13 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C62" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D62" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="63">
@@ -15189,13 +15206,13 @@
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C63" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D63" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="64">
@@ -15203,13 +15220,13 @@
         <v>16</v>
       </c>
       <c r="B64" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C64" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D64" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="65">
@@ -15217,13 +15234,13 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C65" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D65" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="66">
@@ -15231,13 +15248,13 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C66" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D66" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67">
@@ -15245,13 +15262,13 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C67" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D67" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="68">
@@ -15259,13 +15276,13 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C68" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D68" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="69">
@@ -15273,13 +15290,13 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C69" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D69" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="70">
@@ -15287,13 +15304,13 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C70" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D70" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="71">
@@ -15301,13 +15318,13 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C71" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D71" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="72">
@@ -15315,13 +15332,13 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C72" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D72" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="73">
@@ -15329,13 +15346,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C73" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D73" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="74">
@@ -15343,13 +15360,13 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C74" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D74" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75">
@@ -15357,13 +15374,13 @@
         <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C75" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D75" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="76">
@@ -15371,13 +15388,13 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C76" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D76" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="77">
@@ -15385,13 +15402,13 @@
         <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C77" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D77" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="78">
@@ -15399,13 +15416,13 @@
         <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C78" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D78" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="79">
@@ -15413,13 +15430,13 @@
         <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C79" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D79" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="80">
@@ -15427,13 +15444,13 @@
         <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C80" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="D80" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="81">
@@ -15441,13 +15458,13 @@
         <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C81" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D81" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed representation of dqa slot in all data elements
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -219,72 +219,6 @@
     <t xml:space="preserve">=SVERWEIS(dataelements!$D3;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D4;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D5;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D6;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D7;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D8;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D9;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D10;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D12;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D13;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D14;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D15;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D16;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D17;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D18;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D19;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D20;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D21;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D22;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -325,289 +259,6 @@
 Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter (in Tagen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Angabe erfolgt nur bei Kindern bis zur Vollendung des 1. Lebensjahrs. Sie wird für die DRG-Zuordnung benötigt. Bei Neugeborenen mit Aufnahmetag=Geburtsdatum ist „1“ anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter (in Jahren)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Altersangabe wird für die DRG-Zuordnung benötigt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geburtsjahr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das Geburtsjahr ist im Format JJJJ anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICD Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnoseschlüssel sind in der gültigen ICD-10GM-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. mit Sonderzeichen.  
-Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnoseart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsgrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01x Behandlung regulär beendet 
-- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
-- 03x Behandlung aus sonstigen Gründen beendet 
-- 04x Behandlung gegen ärztlichen Rat beendet 
-- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
-- 069 Verlegung in ein anderes Krankenhaus 
-- 079 Tod 
-- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
-- 099 Entlassung in eine Rehabilitationseinrichtung 
-- 109 Entlassung in eine Pflegeeinrichtung 
-- 119 Entlassung in ein Hospiz 
-- 139 externe Verlegung zur psychiatrischen Behandlung 
-- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
-- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
-- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
-- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
-- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
-- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
-- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
-Hinweise:  
-Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
-Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
-Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">01x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fallnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das KH-interne Kennzeichen des Behandlungsfalls dient der eindeutigen Identifikation des Behandlungs-falls (Primärschlüssel). 
-Das KH-interne Kennzeichen darf von der Datenstelle nicht weiter übermittelt werden. 
-Wurden für einen Behandlungsfall im Verfahren nach § 301 SGB V unter identischem krankenhausinter-nen Kennzeichen des Behandlungsfalls mehrere Rechnungen in einem Entgeltbereich gestellt (z.B. quar-talsweise Abrechnung), ist bei der Datenlieferung nach § 21 KHEntgG nur ein Fall mit den Angaben des Gesamtaufenthalts im entsprechenden Entgeltbereich zu übermitteln.   
-Besondere Behandlungsfälle/Konstellationen:  
-Neugeborene sind stets als eigenständige Fälle mit allen zugehörigen fallbezogenen Daten getrennt von der Mutter zu dokumentieren. 
-Für gesunde Neugeborene ist ‚0601’ (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G’ anzuge-ben. 
-Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..’ (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G’ anzugeben. 
-Zur Kodierung der Diagnosen bei Neugeborenen siehe DKR.   
-Begleitpersonen und mitaufgenommene Pflegekräfte, die im § 301-Verfahren kein KH-internes Kennzeichen erhalten, sind mit einem eindeutigen Kennzeichen und mit dem Aufnahmeanlass „B“ zu dokumentieren. Die Angabe von Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmegrund, Entlassungs-/Verlegungsgrund, Alter, Fachabteilungs-, Diagnosen- und Prozedurenangaben entfällt.   
-Nur vorstationär behandelte Fälle:  
-Für nur vorstationär behandelte Fälle werden von den Falldaten der entlassende Standort, das KH-interne Kennzeichen, Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmeanlass, Aufnahmegrund, Fachabteilung und ggf. Diagnose- und Prozedurenangaben übermittelt. Für das Aufnahmedatum ist der erste, für das Entlassungsdatum der letzte vorstationäre Behandlungstag anzugeben.    
-Teilstationäre Fälle:  
-Im § 301-Verfahren werden teilstationäre Fälle mit tagesbezogenen Entgelten quartalsbezogen abgerechnet, dabei sind die Prozeduren jeweils mit dem jeweiligen Kalenderdatum der Leistungserbringung anzugeben. Fehlerhafte Angaben zu Prozeduren und zum Prozedurendatum werden im Datenannahmeverfahren als Fehler gewertet!  
-Krankenhäuser, die an der Kalkulationserhebung teilnehmen, dokumentieren die teilstationären Fälle mit fallbezogenen Angaben in den Dateien „Fall“, „FAB“, „ICD“, „OPS“ und „Entgelte“. Die Datei „Kosten“ enthält die tagesbezogenen Angaben der teilstationären Behandlungskosten und die Datumsangabe des je-weiligen Behandlungstags im Datenfeld „Pflegetag“. Es gibt keine kontaktbezogene Übermittlung von teilstationären Fällen im KHEntgG-Entgeltbereich.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsdatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist das Entlassungs-/Verlegungsdatum (Tag und Uhrzeit) aus der vollstationären oder teilstationären Behandlung anzugeben. (Bei interner Verlegung in einen anderen Entgeltbereich ohne nachfolgende Rückverlegung wird das Verlegungsdatum angegeben; die Behandlungsepisode in dem anderen Entgeltbereich wird als gesonderter Fall dokumentiert.) Bei nur vorstationär behandelten Fällen ist das Entlassungsdatum der letzte vorstationäre Behandlungstag.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmedatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist das Aufnahmedatum (Aufnahmetag und Aufnahmeuhrzeit) zur vollstationären oder teilstationären Behandlung anzugeben.  
-Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geschlecht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- m männlich  
-- w weiblich  
-- x unbestimmt  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmegrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
-- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
-- 03xx Krankenhausbehandlung, teilstationär 
-- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
-- 05xx stationäre Entbindung 
-- 06xx Geburt 
-- 08xx Stationäre Aufnahme zur Organentnahme  
-Hinweise:  
-Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
-Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">01xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patientennummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Patientennummer dient im Rahmen der Kalkulation der Zusammenführung von Fällen (mit unter-schiedlichen KH-internen Kennzeichen), bei denen die Patientennummer angegeben werden muss, zu einem Behandlungsblock. Bei Patienten, die im Datenjahr sowohl im Entgeltbereich „PSY“ als auch im Entgeltbereich „PIA“ behandelt wurden, muss in den jeweiligen Falldaten die Patientennummer angegeben werden. Die Patientennummer ist eine eindeutige und über die Zeit stabile Patienten-Identifikationsnummer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPS Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prozedurenschlüssel sind in der gültigen OPS-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. ohne Sonderzeichen.  
-Zur Reihenfolge der Prozedurenschlüssel für Fälle im KHEntgG-Entgeltbereich siehe DKR.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPS Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000’ angegeben werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fachabteilung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001’ (Rückverlegung) oder ‚0002’ (Wiederaufnahme) oder‚0003‘ (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
-Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA’ (Hauptabteilung) oder ‚BA’ (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE’ voranzustellen.  
-Bei Angabe der Pseudofachabteilungen ‚0001’, ‚0002’ und ‚0003‘ ist als Präfix ‚HA’ anzugeben.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsdatum (Fachabteilung)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bei nachstationärer Behandlung ist der letzte vollstationäre Behandlungstag (Entlassungsdatum) anzugeben. Der Wechsel von vollstationär zu nachstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden. Die nachstationären Behandlungstage sind bei den Falldaten gesondert anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmedatum (Fachabteilung)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bei vorstationärer Behandlung ist der erste vollstationäre Behandlungstag (Aufnahmedatum) anzugeben. Der Wechsel von vorstationär zu vollstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatmungsstunden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Beatmungsstunden sind als Gesamtbeatmungszeit für den Krankenhausfall entsprechend DKR anzugeben. Der Wert entspricht der Angabe „Beatmungsstunden“ in der Entlassungsanzeige (Segment DAU).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postleitzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Postleitzahl der Anschrift des Versicherten ist vollständig mit 5 Ziffern anzugeben.  
-Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
-  </si>
-  <si>
     <t xml:space="preserve">value</t>
   </si>
   <si>
@@ -617,283 +268,13 @@
     <t xml:space="preserve">Designation of value (in first defined language)</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C2;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C3;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C4;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C5;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C6;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C7;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C8;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C9;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C10;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C11;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C12;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C13;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">max_length</t>
   </si>
   <si>
     <t xml:space="preserve">regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:alnum:]]){1,}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:digit:]]{5})$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">range_from</t>
@@ -905,43 +286,7 @@
     <t xml:space="preserve">unit_of_measure</t>
   </si>
   <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A2;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A3;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A4;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A2;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A3;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A4;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A5;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A6;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
   </si>
   <si>
     <t xml:space="preserve">dataelement_id</t>
@@ -956,493 +301,10 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"]}</t>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"key\":[\"dt.admission_source\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.admission_target\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.admission_target\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p21csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.admission_source"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["AUFNAHMEANLASS"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i2b2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNAN%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">omop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.admission_target"],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"E, Z, N, R, V, A, G, B\"]}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_source"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_TAGEN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AITAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageindays_target"],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[366],\"unit\":[\"d\"]}}"],"value_threshold":[0],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 8512"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_source"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["ALTER_IN_JAHREN_AM_AUFNAHMETAG"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:AIJAA'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ageinyears_target"],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[110],\"unit\":[\"a\"]}}"],"value_threshold":[5],"sql_from":["observation"],"sql_where":["observation_concept_id = 4265453 AND unit_concept_id = 9448"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_source"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["GEBURTSJAHR"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["birth_date"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.birthdate_target"],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"source_variable_name":["year_of_birth"],"source_table_name":["person"],"constraints":["{\"regex\":[\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\"]}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.condition_source"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["ICD_Kode"],"source_table_name":["ICD.CSV"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["ICD.CSV"],"fhir":["condition.encounter.identifier.value"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.condition_target"],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"source_variable_name":["condition_source_value"],"source_table_name":["condition_occurrence"],"constraints":["{\"regex\":[\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\.)([[:digit:]]{1,2}))?$\"]}"],"data_map":[1],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_source"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["Diagnoseart"],"source_table_name":["ICD.CSV"],"constraints":["{\"value_set\":[\"HD, ND\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["modifier_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"HD, ND\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ICD%'"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["condition.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A24;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.conditioncategory_target"],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"source_variable_name":["condition_type_concept_id"],"source_table_name":["condition_occurrence"],"constraints":["{\"value_set\":[\"44786627, 44786629\"]}"],"sql_from":["condition_occurrence"],"helper_vars":{"condition_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["condition_occurrence"],"fhir":["condition.encounter.identifier.value"],"sql_from":["condition_occurrence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A25;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A26;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.discharge_source"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["ENTLASSUNGSGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A27;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'ENTLGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A28;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.discharge_target"],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\"]}"],"sql_from":["observation"],"sql_where":["observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A29;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A30;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounter_source"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A31;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["encounter_num"],"source_table_name":["visit_dimension"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["visit_dimension"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["visit_dimension"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A32;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounter_target"],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["visit_occurence"],"helper_vars":{"encounter_subject_patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.subject.patient.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A33;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A34;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterend_source"],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"source_variable_name":["ENTLASSUNGSDATUM"],"source_table_name":["FALL.CSV"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A35;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterend_target"],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"source_variable_name":["end_date"],"source_table_name":["visit_dimension"],"sql_from":["visit_dimension"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["visit_dimension"],"fhir":["encounter.identifier.value"],"sql_from":["visit_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A36;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterend_target"],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"source_variable_name":["visit_end_date"],"source_table_name":["visit_occurrence"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A37;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A38;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterstart_source"],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"source_variable_name":["AUFNAHMEDATUM"],"source_table_name":["FALL.CSV"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A39;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterstart_target"],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"source_variable_name":["start_date"],"source_table_name":["visit_dimension"],"sql_from":["visit_dimension"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["visit_dimension"],"fhir":["encounter.identifier.value"],"sql_from":["visit_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A40;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.encounterstart_target"],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"source_variable_name":["visit_start_date"],"source_table_name":["visit_occurrence"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurence"],"sql_where":["gender_concept_id IN ('8507', '8532', '8551')"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A41;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A42;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.gender_source"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["GESCHLECHT"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"m, w, x\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A43;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["sex_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"value_set\":[\"m, w, x\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A44;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.gender_target"],"variable_name":["patient_gender"],"fhir":["patient.gender"],"source_variable_name":["gender_source_value"],"source_table_name":["person"],"constraints":["{\"value_set\":[\"m, w, x\"]}"],"sql_from":["person"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A45;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A46;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_source"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["AUFNAHMEGRUND"],"source_table_name":["FALL.CSV"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A47;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'AUFNGR%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A48;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.hospitalization_target"],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"value_set\":[\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\"]}"],"sql_from":["observation"],"sql_where":["observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A49;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A50;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.patient_source"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["PATIENTENNUMMER"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A51;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["patient_dimension"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A52;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.patient_target"],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"source_variable_name":["person_id"],"source_table_name":["person"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"data_map":[1],"sql_from":["observation"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A53;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A54;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.procedure_source"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["OPS_Kode"],"source_table_name":["OPS.CSV"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_internes_Kennzeichen"],"source_table_name":["OPS.CSV"],"fhir":["procedure.encounter.identifier.value"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A55;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["concept_cd"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'OPS%'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A56;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.procedure_target"],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"source_variable_name":["procedure_source_value"],"source_table_name":["procedure_occurrence"],"constraints":["{\"regex\":[\"^([[:digit:]]{1})(\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\.)([[:alnum:]]){1,2})?$\"]}"],"data_map":[1],"sql_from":["procedure_occurrence"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["procedure_occurrence"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A57;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A58;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.proceduredate_source"],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"source_variable_name":["OPS_Datum"],"source_table_name":["OPS.CSV"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A59;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.proceduredate_target"],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"source_variable_name":["start_date"],"source_table_name":["observation_fact"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'OPS%'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A60;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.proceduredate_target"],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"source_variable_name":["procedure_date"],"source_table_name":["procedure_occurrence"],"sql_from":["procedure_occurrence"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["procedure_occurrence"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["procedure_occurrence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A61;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A62;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.provider_source"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["FAB"],"source_table_name":["FAB.CSV"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["KH_INTERNES_KENNZEICHEN"],"source_table_name":["FAB.CSV"],"fhir":["encounter.identifier.value"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A63;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["tval_char"],"source_table_name":["observation_fact"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FACHABT%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A64;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.provider_target"],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"source_variable_name":["care_site_id"],"source_table_name":["visit_occurrence"],"constraints":["{\"regex\":[\"^([[:alnum:]]){1,}\"]}"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurrence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A65;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A66;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerend_source"],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"source_variable_name":["FAB_ENTLASSUNGSDATUM"],"source_table_name":["FAB.CSV"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A67;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerend_target"],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"source_variable_name":["end_date"],"source_table_name":["observation_fact"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FACHABT%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A68;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerend_target"],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"source_variable_name":["visit_end_date"],"source_table_name":["visit_occurrence"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A69;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A70;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerstart_source"],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"source_variable_name":["FAB_AUFNAHMEDATUM"],"source_table_name":["FAB.CSV"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A71;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerstart_target"],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"source_variable_name":["start_date"],"source_table_name":["observation_fact"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FACHABT%'"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A72;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.providerstart_target"],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"source_variable_name":["visit_start_date"],"source_table_name":["visit_occurrence"],"sql_from":["visit_occurence"],"helper_vars":{"encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["visit_occurrence"],"fhir":["encounter.identifier.value"],"sql_from":["visit_occurence"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A73;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A74;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_source"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["BEATMUNGSSTUNDEN"],"source_table_name":["FALL.CSV"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A75;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["nval_num"],"source_table_name":["observation_fact"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"],"sql_from":["observation_fact"],"sql_where":["concept_cd LIKE 'FALL:BEATMST'"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["encounter_num"],"source_table_name":["observation_fact"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation_fact"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A76;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.ventilation_target"],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"source_variable_name":["observation_source_value"],"source_table_name":["observation"],"constraints":["{\"range\":{\"min\":[0],\"max\":[8766],\"unit\":[\"h\"]}}"],"sql_from":["observation"],"sql_where":["observation_concept_id = 4108449"],"helper_vars":{"procedure_encounter_identifier_value":{"designation":["Fallnummer"],"source_variable_name":["visit_occurrence_id"],"source_table_name":["observation"],"fhir":["procedure.encounter.identifier.value"],"sql_from":["observation"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A77;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A78;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_source"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["PLZ"],"source_table_name":["FALL.CSV"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A79;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip_cd"],"source_table_name":["patient_dimension"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"],"sql_from":["patient_dimension"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["patient_num"],"source_table_name":["patient_dimension"],"fhir":["patient.identifier.value"],"sql_from":["patient_dimension"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A80;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"key":["dt.zipcode_target"],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"source_variable_name":["zip"],"source_table_name":["location"],"constraints":["{\"regex\":[\"^([[:digit:]]{5})$\"]}"],"sql_from":["location"],"sql_join_on":["location_id"],"sql_join_type":["left outer"],"helper_vars":{"patient_identifier_value":{"designation":["Patientennummer"],"source_variable_name":["person_id"],"source_table_name":["person"],"fhir":["patient.identifier.value"],"sql_from":["person"]}}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A81;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -1632,8 +494,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D81" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -1656,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G3"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -1672,8 +534,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D3" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1685,8 +547,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="value"/>
@@ -1699,8 +561,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -1712,8 +574,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="range_from"/>
@@ -1726,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="format"/>
@@ -4306,441 +3168,61 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="n">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" t="n">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="n">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="n">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="n">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="n">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="n">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="G17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" t="n">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" t="n">
-        <v>6</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="G18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="n">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" t="n">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="n">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" t="n">
-        <v>5</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="n">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" t="n">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="n">
-        <v>7</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23">
       <c r="G23" s="1"/>
@@ -6207,16 +4689,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
@@ -6224,13 +4706,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
@@ -6238,825 +4720,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1004</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1005</v>
-      </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1006</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1008</v>
-      </c>
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>1009</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>1010</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>1011</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>1012</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>1013</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>1014</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>1017</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>1020</v>
-      </c>
-      <c r="B30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>1021</v>
-      </c>
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>1022</v>
-      </c>
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>1023</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>1024</v>
-      </c>
-      <c r="B34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>1025</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>1026</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>1027</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>1028</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>9</v>
-      </c>
-      <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>1029</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>1030</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>1031</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>1032</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>1033</v>
-      </c>
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>1034</v>
-      </c>
-      <c r="B49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>1035</v>
-      </c>
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>1036</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>1037</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>1038</v>
-      </c>
-      <c r="B53" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" t="s">
-        <v>157</v>
-      </c>
-      <c r="D55" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>15</v>
-      </c>
-      <c r="B56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>161</v>
-      </c>
-      <c r="D57" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>17</v>
-      </c>
-      <c r="B58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" t="s">
-        <v>163</v>
-      </c>
-      <c r="D58" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D59" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>20</v>
-      </c>
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" t="s">
-        <v>170</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -8107,683 +5777,40 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
-      <c r="C2" t="n">
-        <v>1000</v>
+      <c r="C2" t="s">
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1002</v>
-      </c>
-      <c r="D4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1003</v>
-      </c>
-      <c r="D5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1004</v>
-      </c>
-      <c r="D6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1005</v>
-      </c>
-      <c r="D7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1006</v>
-      </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1007</v>
-      </c>
-      <c r="D9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1008</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1009</v>
-      </c>
-      <c r="D11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1010</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1011</v>
-      </c>
-      <c r="D13" t="s">
-        <v>196</v>
-      </c>
-      <c r="E13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1012</v>
-      </c>
-      <c r="D14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1013</v>
-      </c>
-      <c r="D15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1014</v>
-      </c>
-      <c r="D16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1015</v>
-      </c>
-      <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1016</v>
-      </c>
-      <c r="D18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" t="s">
-        <v>207</v>
-      </c>
-    </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1017</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1018</v>
-      </c>
-      <c r="D20" t="s">
-        <v>210</v>
-      </c>
-      <c r="E20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1019</v>
-      </c>
-      <c r="D21" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1020</v>
-      </c>
-      <c r="D22" t="s">
-        <v>214</v>
-      </c>
-      <c r="E22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1021</v>
-      </c>
-      <c r="D23" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1022</v>
-      </c>
-      <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1023</v>
-      </c>
-      <c r="D25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1024</v>
-      </c>
-      <c r="D26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1025</v>
-      </c>
-      <c r="D27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1026</v>
-      </c>
-      <c r="D28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1027</v>
-      </c>
-      <c r="D29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1028</v>
-      </c>
-      <c r="D30" t="s">
-        <v>230</v>
-      </c>
-      <c r="E30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1029</v>
-      </c>
-      <c r="D31" t="s">
-        <v>232</v>
-      </c>
-      <c r="E31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1030</v>
-      </c>
-      <c r="D32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1031</v>
-      </c>
-      <c r="D33" t="s">
-        <v>236</v>
-      </c>
-      <c r="E33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1032</v>
-      </c>
-      <c r="D34" t="s">
-        <v>238</v>
-      </c>
-      <c r="E34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1033</v>
-      </c>
-      <c r="D35" t="s">
-        <v>240</v>
-      </c>
-      <c r="E35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1034</v>
-      </c>
-      <c r="D36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1035</v>
-      </c>
-      <c r="D37" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1036</v>
-      </c>
-      <c r="D38" t="s">
-        <v>246</v>
-      </c>
-      <c r="E38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1037</v>
-      </c>
-      <c r="D39" t="s">
-        <v>248</v>
-      </c>
-      <c r="E39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1038</v>
-      </c>
-      <c r="D40" t="s">
-        <v>250</v>
-      </c>
-      <c r="E40" t="s">
-        <v>251</v>
-      </c>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -9838,115 +6865,31 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>252</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>253</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>254</v>
-      </c>
-      <c r="C8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -12081,70 +9024,36 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>267</v>
+        <v>78</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>268</v>
+        <v>79</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>75</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>75</v>
       </c>
-      <c r="C2" t="n">
-        <v>366</v>
+      <c r="C2" t="s">
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8766</v>
-      </c>
-      <c r="D4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" t="s">
-        <v>275</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -13200,68 +10109,24 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>276</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C5" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C6" t="s">
-        <v>282</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -14335,16 +11200,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>283</v>
+        <v>82</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>284</v>
+        <v>83</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>171</v>
+        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>285</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
@@ -14352,1119 +11217,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>289</v>
-      </c>
-      <c r="C3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C4" t="s">
-        <v>293</v>
-      </c>
-      <c r="D4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>295</v>
-      </c>
-      <c r="C5" t="s">
-        <v>296</v>
-      </c>
-      <c r="D5" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D6" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>289</v>
-      </c>
-      <c r="C7" t="s">
-        <v>300</v>
-      </c>
-      <c r="D7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C8" t="s">
-        <v>302</v>
-      </c>
-      <c r="D8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>295</v>
-      </c>
-      <c r="C9" t="s">
-        <v>304</v>
-      </c>
-      <c r="D9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>286</v>
-      </c>
-      <c r="C10" t="s">
-        <v>306</v>
-      </c>
-      <c r="D10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>289</v>
-      </c>
-      <c r="C11" t="s">
-        <v>308</v>
-      </c>
-      <c r="D11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>292</v>
-      </c>
-      <c r="C12" t="s">
-        <v>310</v>
-      </c>
-      <c r="D12" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>295</v>
-      </c>
-      <c r="C13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>286</v>
-      </c>
-      <c r="C14" t="s">
-        <v>314</v>
-      </c>
-      <c r="D14" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>289</v>
-      </c>
-      <c r="C15" t="s">
-        <v>316</v>
-      </c>
-      <c r="D15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>292</v>
-      </c>
-      <c r="C16" t="s">
-        <v>318</v>
-      </c>
-      <c r="D16" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>295</v>
-      </c>
-      <c r="C17" t="s">
-        <v>320</v>
-      </c>
-      <c r="D17" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C18" t="s">
-        <v>322</v>
-      </c>
-      <c r="D18" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>289</v>
-      </c>
-      <c r="C19" t="s">
-        <v>324</v>
-      </c>
-      <c r="D19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" t="s">
-        <v>326</v>
-      </c>
-      <c r="D20" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>295</v>
-      </c>
-      <c r="C21" t="s">
-        <v>328</v>
-      </c>
-      <c r="D21" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>286</v>
-      </c>
-      <c r="C22" t="s">
-        <v>330</v>
-      </c>
-      <c r="D22" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>289</v>
-      </c>
-      <c r="C23" t="s">
-        <v>332</v>
-      </c>
-      <c r="D23" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" t="s">
-        <v>334</v>
-      </c>
-      <c r="D24" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>295</v>
-      </c>
-      <c r="C25" t="s">
-        <v>336</v>
-      </c>
-      <c r="D25" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>286</v>
-      </c>
-      <c r="C26" t="s">
-        <v>338</v>
-      </c>
-      <c r="D26" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>289</v>
-      </c>
-      <c r="C27" t="s">
-        <v>340</v>
-      </c>
-      <c r="D27" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>292</v>
-      </c>
-      <c r="C28" t="s">
-        <v>342</v>
-      </c>
-      <c r="D28" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>295</v>
-      </c>
-      <c r="C29" t="s">
-        <v>344</v>
-      </c>
-      <c r="D29" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>8</v>
-      </c>
-      <c r="B30" t="s">
-        <v>286</v>
-      </c>
-      <c r="C30" t="s">
-        <v>346</v>
-      </c>
-      <c r="D30" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>8</v>
-      </c>
-      <c r="B31" t="s">
-        <v>289</v>
-      </c>
-      <c r="C31" t="s">
-        <v>348</v>
-      </c>
-      <c r="D31" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>8</v>
-      </c>
-      <c r="B32" t="s">
-        <v>292</v>
-      </c>
-      <c r="C32" t="s">
-        <v>350</v>
-      </c>
-      <c r="D32" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>8</v>
-      </c>
-      <c r="B33" t="s">
-        <v>295</v>
-      </c>
-      <c r="C33" t="s">
-        <v>352</v>
-      </c>
-      <c r="D33" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>9</v>
-      </c>
-      <c r="B34" t="s">
-        <v>286</v>
-      </c>
-      <c r="C34" t="s">
-        <v>354</v>
-      </c>
-      <c r="D34" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>9</v>
-      </c>
-      <c r="B35" t="s">
-        <v>289</v>
-      </c>
-      <c r="C35" t="s">
-        <v>356</v>
-      </c>
-      <c r="D35" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>9</v>
-      </c>
-      <c r="B36" t="s">
-        <v>292</v>
-      </c>
-      <c r="C36" t="s">
-        <v>358</v>
-      </c>
-      <c r="D36" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>295</v>
-      </c>
-      <c r="C37" t="s">
-        <v>360</v>
-      </c>
-      <c r="D37" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>10</v>
-      </c>
-      <c r="B38" t="s">
-        <v>286</v>
-      </c>
-      <c r="C38" t="s">
-        <v>362</v>
-      </c>
-      <c r="D38" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
-        <v>289</v>
-      </c>
-      <c r="C39" t="s">
-        <v>364</v>
-      </c>
-      <c r="D39" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>10</v>
-      </c>
-      <c r="B40" t="s">
-        <v>292</v>
-      </c>
-      <c r="C40" t="s">
-        <v>366</v>
-      </c>
-      <c r="D40" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>295</v>
-      </c>
-      <c r="C41" t="s">
-        <v>368</v>
-      </c>
-      <c r="D41" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>286</v>
-      </c>
-      <c r="C42" t="s">
-        <v>370</v>
-      </c>
-      <c r="D42" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>11</v>
-      </c>
-      <c r="B43" t="s">
-        <v>289</v>
-      </c>
-      <c r="C43" t="s">
-        <v>372</v>
-      </c>
-      <c r="D43" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>292</v>
-      </c>
-      <c r="C44" t="s">
-        <v>374</v>
-      </c>
-      <c r="D44" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>11</v>
-      </c>
-      <c r="B45" t="s">
-        <v>295</v>
-      </c>
-      <c r="C45" t="s">
-        <v>376</v>
-      </c>
-      <c r="D45" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>286</v>
-      </c>
-      <c r="C46" t="s">
-        <v>378</v>
-      </c>
-      <c r="D46" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>289</v>
-      </c>
-      <c r="C47" t="s">
-        <v>380</v>
-      </c>
-      <c r="D47" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
-        <v>292</v>
-      </c>
-      <c r="C48" t="s">
-        <v>382</v>
-      </c>
-      <c r="D48" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>12</v>
-      </c>
-      <c r="B49" t="s">
-        <v>295</v>
-      </c>
-      <c r="C49" t="s">
-        <v>384</v>
-      </c>
-      <c r="D49" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>13</v>
-      </c>
-      <c r="B50" t="s">
-        <v>286</v>
-      </c>
-      <c r="C50" t="s">
-        <v>386</v>
-      </c>
-      <c r="D50" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>13</v>
-      </c>
-      <c r="B51" t="s">
-        <v>289</v>
-      </c>
-      <c r="C51" t="s">
-        <v>388</v>
-      </c>
-      <c r="D51" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>13</v>
-      </c>
-      <c r="B52" t="s">
-        <v>292</v>
-      </c>
-      <c r="C52" t="s">
-        <v>390</v>
-      </c>
-      <c r="D52" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>13</v>
-      </c>
-      <c r="B53" t="s">
-        <v>295</v>
-      </c>
-      <c r="C53" t="s">
-        <v>392</v>
-      </c>
-      <c r="D53" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>286</v>
-      </c>
-      <c r="C54" t="s">
-        <v>394</v>
-      </c>
-      <c r="D54" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>289</v>
-      </c>
-      <c r="C55" t="s">
-        <v>396</v>
-      </c>
-      <c r="D55" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>14</v>
-      </c>
-      <c r="B56" t="s">
-        <v>292</v>
-      </c>
-      <c r="C56" t="s">
-        <v>398</v>
-      </c>
-      <c r="D56" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>14</v>
-      </c>
-      <c r="B57" t="s">
-        <v>295</v>
-      </c>
-      <c r="C57" t="s">
-        <v>400</v>
-      </c>
-      <c r="D57" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>15</v>
-      </c>
-      <c r="B58" t="s">
-        <v>286</v>
-      </c>
-      <c r="C58" t="s">
-        <v>402</v>
-      </c>
-      <c r="D58" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>15</v>
-      </c>
-      <c r="B59" t="s">
-        <v>289</v>
-      </c>
-      <c r="C59" t="s">
-        <v>404</v>
-      </c>
-      <c r="D59" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>15</v>
-      </c>
-      <c r="B60" t="s">
-        <v>292</v>
-      </c>
-      <c r="C60" t="s">
-        <v>406</v>
-      </c>
-      <c r="D60" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>15</v>
-      </c>
-      <c r="B61" t="s">
-        <v>295</v>
-      </c>
-      <c r="C61" t="s">
-        <v>408</v>
-      </c>
-      <c r="D61" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>16</v>
-      </c>
-      <c r="B62" t="s">
-        <v>286</v>
-      </c>
-      <c r="C62" t="s">
-        <v>410</v>
-      </c>
-      <c r="D62" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>16</v>
-      </c>
-      <c r="B63" t="s">
-        <v>289</v>
-      </c>
-      <c r="C63" t="s">
-        <v>412</v>
-      </c>
-      <c r="D63" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>16</v>
-      </c>
-      <c r="B64" t="s">
-        <v>292</v>
-      </c>
-      <c r="C64" t="s">
-        <v>414</v>
-      </c>
-      <c r="D64" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>16</v>
-      </c>
-      <c r="B65" t="s">
-        <v>295</v>
-      </c>
-      <c r="C65" t="s">
-        <v>416</v>
-      </c>
-      <c r="D65" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>17</v>
-      </c>
-      <c r="B66" t="s">
-        <v>286</v>
-      </c>
-      <c r="C66" t="s">
-        <v>418</v>
-      </c>
-      <c r="D66" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>17</v>
-      </c>
-      <c r="B67" t="s">
-        <v>289</v>
-      </c>
-      <c r="C67" t="s">
-        <v>420</v>
-      </c>
-      <c r="D67" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>17</v>
-      </c>
-      <c r="B68" t="s">
-        <v>292</v>
-      </c>
-      <c r="C68" t="s">
-        <v>422</v>
-      </c>
-      <c r="D68" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>17</v>
-      </c>
-      <c r="B69" t="s">
-        <v>295</v>
-      </c>
-      <c r="C69" t="s">
-        <v>424</v>
-      </c>
-      <c r="D69" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>18</v>
-      </c>
-      <c r="B70" t="s">
-        <v>286</v>
-      </c>
-      <c r="C70" t="s">
-        <v>426</v>
-      </c>
-      <c r="D70" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>18</v>
-      </c>
-      <c r="B71" t="s">
-        <v>289</v>
-      </c>
-      <c r="C71" t="s">
-        <v>428</v>
-      </c>
-      <c r="D71" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>18</v>
-      </c>
-      <c r="B72" t="s">
-        <v>292</v>
-      </c>
-      <c r="C72" t="s">
-        <v>430</v>
-      </c>
-      <c r="D72" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>18</v>
-      </c>
-      <c r="B73" t="s">
-        <v>295</v>
-      </c>
-      <c r="C73" t="s">
-        <v>432</v>
-      </c>
-      <c r="D73" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>19</v>
-      </c>
-      <c r="B74" t="s">
-        <v>286</v>
-      </c>
-      <c r="C74" t="s">
-        <v>434</v>
-      </c>
-      <c r="D74" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>19</v>
-      </c>
-      <c r="B75" t="s">
-        <v>289</v>
-      </c>
-      <c r="C75" t="s">
-        <v>436</v>
-      </c>
-      <c r="D75" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>19</v>
-      </c>
-      <c r="B76" t="s">
-        <v>292</v>
-      </c>
-      <c r="C76" t="s">
-        <v>438</v>
-      </c>
-      <c r="D76" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>19</v>
-      </c>
-      <c r="B77" t="s">
-        <v>295</v>
-      </c>
-      <c r="C77" t="s">
-        <v>440</v>
-      </c>
-      <c r="D77" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>20</v>
-      </c>
-      <c r="B78" t="s">
-        <v>286</v>
-      </c>
-      <c r="C78" t="s">
-        <v>442</v>
-      </c>
-      <c r="D78" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>20</v>
-      </c>
-      <c r="B79" t="s">
-        <v>289</v>
-      </c>
-      <c r="C79" t="s">
-        <v>444</v>
-      </c>
-      <c r="D79" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>20</v>
-      </c>
-      <c r="B80" t="s">
-        <v>292</v>
-      </c>
-      <c r="C80" t="s">
-        <v>446</v>
-      </c>
-      <c r="D80" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>20</v>
-      </c>
-      <c r="B81" t="s">
-        <v>295</v>
-      </c>
-      <c r="C81" t="s">
-        <v>448</v>
-      </c>
-      <c r="D81" t="s">
-        <v>449</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dqa import file
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="327">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -217,6 +217,72 @@
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(dataelements!$D3;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D4;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D5;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D6;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D7;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D8;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D9;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D10;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D12;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D13;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D14;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D15;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D16;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D17;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D18;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D19;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D20;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D21;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D22;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -259,6 +325,289 @@
 Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
   </si>
   <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter (in Tagen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Angabe erfolgt nur bei Kindern bis zur Vollendung des 1. Lebensjahrs. Sie wird für die DRG-Zuordnung benötigt. Bei Neugeborenen mit Aufnahmetag=Geburtsdatum ist „1“ anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter (in Jahren)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Altersangabe wird für die DRG-Zuordnung benötigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geburtsjahr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Geburtsjahr ist im Format JJJJ anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICD Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnoseschlüssel sind in der gültigen ICD-10GM-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. mit Sonderzeichen.  
+Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnoseart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsgrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01x Behandlung regulär beendet 
+- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
+- 03x Behandlung aus sonstigen Gründen beendet 
+- 04x Behandlung gegen ärztlichen Rat beendet 
+- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
+- 069 Verlegung in ein anderes Krankenhaus 
+- 079 Tod 
+- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
+- 099 Entlassung in eine Rehabilitationseinrichtung 
+- 109 Entlassung in eine Pflegeeinrichtung 
+- 119 Entlassung in ein Hospiz 
+- 139 externe Verlegung zur psychiatrischen Behandlung 
+- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
+- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
+- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
+- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
+- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
+- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
+- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
+Hinweise:  
+Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
+Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
+Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das KH-interne Kennzeichen des Behandlungsfalls dient der eindeutigen Identifikation des Behandlungs-falls (Primärschlüssel). 
+Das KH-interne Kennzeichen darf von der Datenstelle nicht weiter übermittelt werden. 
+Wurden für einen Behandlungsfall im Verfahren nach § 301 SGB V unter identischem krankenhausinter-nen Kennzeichen des Behandlungsfalls mehrere Rechnungen in einem Entgeltbereich gestellt (z.B. quar-talsweise Abrechnung), ist bei der Datenlieferung nach § 21 KHEntgG nur ein Fall mit den Angaben des Gesamtaufenthalts im entsprechenden Entgeltbereich zu übermitteln.   
+Besondere Behandlungsfälle/Konstellationen:  
+Neugeborene sind stets als eigenständige Fälle mit allen zugehörigen fallbezogenen Daten getrennt von der Mutter zu dokumentieren. 
+Für gesunde Neugeborene ist ‚0601’ (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G’ anzuge-ben. 
+Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..’ (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G’ anzugeben. 
+Zur Kodierung der Diagnosen bei Neugeborenen siehe DKR.   
+Begleitpersonen und mitaufgenommene Pflegekräfte, die im § 301-Verfahren kein KH-internes Kennzeichen erhalten, sind mit einem eindeutigen Kennzeichen und mit dem Aufnahmeanlass „B“ zu dokumentieren. Die Angabe von Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmegrund, Entlassungs-/Verlegungsgrund, Alter, Fachabteilungs-, Diagnosen- und Prozedurenangaben entfällt.   
+Nur vorstationär behandelte Fälle:  
+Für nur vorstationär behandelte Fälle werden von den Falldaten der entlassende Standort, das KH-interne Kennzeichen, Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmeanlass, Aufnahmegrund, Fachabteilung und ggf. Diagnose- und Prozedurenangaben übermittelt. Für das Aufnahmedatum ist der erste, für das Entlassungsdatum der letzte vorstationäre Behandlungstag anzugeben.    
+Teilstationäre Fälle:  
+Im § 301-Verfahren werden teilstationäre Fälle mit tagesbezogenen Entgelten quartalsbezogen abgerechnet, dabei sind die Prozeduren jeweils mit dem jeweiligen Kalenderdatum der Leistungserbringung anzugeben. Fehlerhafte Angaben zu Prozeduren und zum Prozedurendatum werden im Datenannahmeverfahren als Fehler gewertet!  
+Krankenhäuser, die an der Kalkulationserhebung teilnehmen, dokumentieren die teilstationären Fälle mit fallbezogenen Angaben in den Dateien „Fall“, „FAB“, „ICD“, „OPS“ und „Entgelte“. Die Datei „Kosten“ enthält die tagesbezogenen Angaben der teilstationären Behandlungskosten und die Datumsangabe des je-weiligen Behandlungstags im Datenfeld „Pflegetag“. Es gibt keine kontaktbezogene Übermittlung von teilstationären Fällen im KHEntgG-Entgeltbereich.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsdatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist das Entlassungs-/Verlegungsdatum (Tag und Uhrzeit) aus der vollstationären oder teilstationären Behandlung anzugeben. (Bei interner Verlegung in einen anderen Entgeltbereich ohne nachfolgende Rückverlegung wird das Verlegungsdatum angegeben; die Behandlungsepisode in dem anderen Entgeltbereich wird als gesonderter Fall dokumentiert.) Bei nur vorstationär behandelten Fällen ist das Entlassungsdatum der letzte vorstationäre Behandlungstag.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmedatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist das Aufnahmedatum (Aufnahmetag und Aufnahmeuhrzeit) zur vollstationären oder teilstationären Behandlung anzugeben.  
+Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geschlecht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- m männlich  
+- w weiblich  
+- x unbestimmt  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmegrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
+- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
+- 03xx Krankenhausbehandlung, teilstationär 
+- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
+- 05xx stationäre Entbindung 
+- 06xx Geburt 
+- 08xx Stationäre Aufnahme zur Organentnahme  
+Hinweise:  
+Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
+Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patientennummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Patientennummer dient im Rahmen der Kalkulation der Zusammenführung von Fällen (mit unter-schiedlichen KH-internen Kennzeichen), bei denen die Patientennummer angegeben werden muss, zu einem Behandlungsblock. Bei Patienten, die im Datenjahr sowohl im Entgeltbereich „PSY“ als auch im Entgeltbereich „PIA“ behandelt wurden, muss in den jeweiligen Falldaten die Patientennummer angegeben werden. Die Patientennummer ist eine eindeutige und über die Zeit stabile Patienten-Identifikationsnummer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPS Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prozedurenschlüssel sind in der gültigen OPS-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. ohne Sonderzeichen.  
+Zur Reihenfolge der Prozedurenschlüssel für Fälle im KHEntgG-Entgeltbereich siehe DKR.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPS Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000’ angegeben werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachabteilung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001’ (Rückverlegung) oder ‚0002’ (Wiederaufnahme) oder‚0003‘ (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
+Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA’ (Hauptabteilung) oder ‚BA’ (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE’ voranzustellen.  
+Bei Angabe der Pseudofachabteilungen ‚0001’, ‚0002’ und ‚0003‘ ist als Präfix ‚HA’ anzugeben.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsdatum (Fachabteilung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei nachstationärer Behandlung ist der letzte vollstationäre Behandlungstag (Entlassungsdatum) anzugeben. Der Wechsel von vollstationär zu nachstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden. Die nachstationären Behandlungstage sind bei den Falldaten gesondert anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmedatum (Fachabteilung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei vorstationärer Behandlung ist der erste vollstationäre Behandlungstag (Aufnahmedatum) anzugeben. Der Wechsel von vorstationär zu vollstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatmungsstunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Beatmungsstunden sind als Gesamtbeatmungszeit für den Krankenhausfall entsprechend DKR anzugeben. Der Wert entspricht der Angabe „Beatmungsstunden“ in der Entlassungsanzeige (Segment DAU).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postleitzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Postleitzahl der Anschrift des Versicherten ist vollständig mit 5 Ziffern anzugeben.  
+Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
+  </si>
+  <si>
     <t xml:space="preserve">value</t>
   </si>
   <si>
@@ -268,7 +617,238 @@
     <t xml:space="preserve">Designation of value (in first defined language)</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C2;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C3;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C4;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C5;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C6;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C7;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C8;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C9;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C10;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C11;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C12;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C13;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">max_length</t>
@@ -277,6 +857,45 @@
     <t xml:space="preserve">regex</t>
   </si>
   <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:alnum:]]){1,}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{5})$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">range_from</t>
   </si>
   <si>
@@ -286,9 +905,45 @@
     <t xml:space="preserve">unit_of_measure</t>
   </si>
   <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A2;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A3;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A4;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">format</t>
   </si>
   <si>
+    <t xml:space="preserve">yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A2;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A3;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A4;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A5;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A6;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataelement_id</t>
   </si>
   <si>
@@ -305,6 +960,120 @@
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"key\":[\"dt.ageindays_source\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ageindays_target\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ageindays_target\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"key\":[\"dt.ageinyears_source\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ageinyears_target\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ageinyears_target\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"key\":[\"dt.birthdate_source\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.birthdate_target\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.birthdate_target\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"key\":[\"dt.condition_source\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.condition_target\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.condition_target\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"key\":[\"dt.conditioncategory_source\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.conditioncategory_target\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.conditioncategory_target\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"key\":[\"dt.discharge_source\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.discharge_target\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.discharge_target\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"key\":[\"dt.encounter_source\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounter_target\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounter_target\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"key\":[\"dt.encounterend_source\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounterend_target\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounterend_target\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"key\":[\"dt.encounterstart_source\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounterstart_target\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounterstart_target\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"key\":[\"dt.gender_source\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.gender_target\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.gender_target\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"key\":[\"dt.hospitalization_source\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.hospitalization_target\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.hospitalization_target\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"key\":[\"dt.patient_source\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.patient_target\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}"],"omop":["{\"key\":[\"dt.patient_target\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"key\":[\"dt.procedure_source\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.procedure_target\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.procedure_target\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"key\":[\"dt.proceduredate_source\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.proceduredate_target\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.proceduredate_target\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"key\":[\"dt.provider_source\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.provider_target\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.provider_target\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"key\":[\"dt.providerend_source\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.providerend_target\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.providerend_target\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"key\":[\"dt.providerstart_source\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.providerstart_target\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.providerstart_target\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"key\":[\"dt.ventilation_source\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ventilation_target\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ventilation_target\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"key\":[\"dt.zipcode_source\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.zipcode_target\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.zipcode_target\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -494,8 +1263,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D21" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -518,8 +1287,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G22" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -534,8 +1303,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D3" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -547,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E40"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="value"/>
@@ -561,8 +1330,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -574,8 +1343,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="range_from"/>
@@ -588,8 +1357,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="format"/>
@@ -3168,61 +3937,441 @@
       </c>
     </row>
     <row r="4">
-      <c r="G4" s="1"/>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5">
-      <c r="G5" s="1"/>
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6">
-      <c r="G6" s="1"/>
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7">
-      <c r="G7" s="1"/>
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8">
-      <c r="G8" s="1"/>
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9">
-      <c r="G9" s="1"/>
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10">
-      <c r="G10" s="1"/>
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11">
-      <c r="G11" s="1"/>
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12">
-      <c r="G12" s="1"/>
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13">
-      <c r="G13" s="1"/>
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14">
-      <c r="G14" s="1"/>
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15">
-      <c r="G15" s="1"/>
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16">
-      <c r="G16" s="1"/>
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17">
-      <c r="G17" s="1"/>
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18">
-      <c r="G18" s="1"/>
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="n">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19">
-      <c r="G19" s="1"/>
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20">
-      <c r="G20" s="1"/>
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="21">
-      <c r="G21" s="1"/>
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22">
-      <c r="G22" s="1"/>
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23">
       <c r="G23" s="1"/>
@@ -4689,16 +5838,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -4706,13 +5855,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
@@ -4720,13 +5869,825 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1005</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1006</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1008</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1009</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1021</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1022</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1023</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1026</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1027</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1028</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1029</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1031</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1032</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1033</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1034</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1035</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1036</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1037</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1038</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>17</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5777,40 +7738,683 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>75</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
+        <v>94</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1005</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1006</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1009</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1011</v>
+      </c>
+      <c r="D13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1012</v>
+      </c>
+      <c r="D14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="19">
-      <c r="D19" s="1"/>
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1017</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1018</v>
+      </c>
+      <c r="D20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D21" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1020</v>
+      </c>
+      <c r="D22" t="s">
+        <v>214</v>
+      </c>
+      <c r="E22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1021</v>
+      </c>
+      <c r="D23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1022</v>
+      </c>
+      <c r="D24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1025</v>
+      </c>
+      <c r="D27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1026</v>
+      </c>
+      <c r="D28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1027</v>
+      </c>
+      <c r="D29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1028</v>
+      </c>
+      <c r="D30" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D31" t="s">
+        <v>232</v>
+      </c>
+      <c r="E31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1030</v>
+      </c>
+      <c r="D32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D33" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1032</v>
+      </c>
+      <c r="D34" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D35" t="s">
+        <v>240</v>
+      </c>
+      <c r="E35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1034</v>
+      </c>
+      <c r="D36" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1035</v>
+      </c>
+      <c r="D37" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1036</v>
+      </c>
+      <c r="D38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1037</v>
+      </c>
+      <c r="D39" t="s">
+        <v>248</v>
+      </c>
+      <c r="E39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1038</v>
+      </c>
+      <c r="D40" t="s">
+        <v>250</v>
+      </c>
+      <c r="E40" t="s">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -6865,31 +9469,115 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>252</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>253</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>75</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -9024,36 +11712,70 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>78</v>
+        <v>267</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>79</v>
+        <v>268</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>80</v>
+        <v>269</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8766</v>
+      </c>
+      <c r="D4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -10109,24 +12831,68 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>81</v>
+        <v>276</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>75</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -11200,16 +13966,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>82</v>
+        <v>283</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>284</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>72</v>
+        <v>171</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>84</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
@@ -11217,13 +13983,279 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" t="s">
+        <v>317</v>
+      </c>
+      <c r="D17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C19" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D21" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mdr_to_samply and mdr_from_samply; not yet working
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -956,121 +956,121 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"key\":[\"dt.admission_source\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.admission_target\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.admission_target\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"key\":[\"dt.ageindays_source\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ageindays_target\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ageindays_target\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"key\":[\"dt.ageinyears_source\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ageinyears_target\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ageinyears_target\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"key\":[\"dt.birthdate_source\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.birthdate_target\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.birthdate_target\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"key\":[\"dt.condition_source\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.condition_target\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.condition_target\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"key\":[\"dt.conditioncategory_source\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.conditioncategory_target\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.conditioncategory_target\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"key\":[\"dt.discharge_source\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.discharge_target\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.discharge_target\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"key\":[\"dt.encounter_source\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounter_target\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounter_target\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"key\":[\"dt.encounterend_source\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounterend_target\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounterend_target\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"key\":[\"dt.encounterstart_source\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.encounterstart_target\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"key\":[\"dt.encounterstart_target\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"key\":[\"dt.gender_source\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.gender_target\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.gender_target\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"key\":[\"dt.hospitalization_source\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.hospitalization_target\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.hospitalization_target\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"key\":[\"dt.patient_source\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.patient_target\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}"],"omop":["{\"key\":[\"dt.patient_target\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"key\":[\"dt.procedure_source\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.procedure_target\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.procedure_target\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"key\":[\"dt.proceduredate_source\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.proceduredate_target\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.proceduredate_target\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"key\":[\"dt.provider_source\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"key\":[\"dt.provider_target\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.provider_target\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"key\":[\"dt.providerend_source\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.providerend_target\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.providerend_target\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"key\":[\"dt.providerstart_source\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.providerstart_target\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.providerstart_target\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"key\":[\"dt.ventilation_source\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.ventilation_target\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"key\":[\"dt.ventilation_target\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4108449\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"dqa_assessment":[1],"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"key\":[\"dt.zipcode_source\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}"]},"postgres":{"i2b2":["{\"key\":[\"dt.zipcode_target\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"key\":[\"dt.zipcode_target\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
updated mdr_to_samply; still not working
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -210,81 +210,6 @@
     <t xml:space="preserve">=SVERWEIS(dataelements!$D2;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">dataelement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">permittedValues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D3;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D4;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D5;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D6;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D7;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D8;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D9;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D10;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calendar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D12;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D13;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D14;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D15;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D16;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D17;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D18;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D19;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D20;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D21;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D22;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -306,308 +231,6 @@
     <t xml:space="preserve">Diese Gruppe enthält die Datenelemente des Paragraph 21, die im Rahmen der DQ-Analyse geprüft werden.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aufnahmeanlass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- E Einweisung durch einen Arzt 
-- Z Einweisung durch einen Zahnarzt 
-- N Notfall 
-- R Aufnahme nach vorausgehender Behandlung in einer Rehabilitationseinrichtung 
-- V Verlegung mit Behandlungsdauer im verlegenden Krankenhaus länger als 24 Stunden 
-- A Verlegung mit Behandlungsdauer im verlegenden Krankenhaus bis zu 24 Stunden  
-Zusatzschlüssel für besondere Kalkulationsanforderungen: 
-    - G Geburt (siehe Hinweis Neugeborene) 
-    - B Begleitperson oder mitaufgenommene Pflegekraft  
-Hinweise:  
-Einweisung durch einen Arzt ist im § 301-Aufnahmesatz im Segment Aufnahme durch die Arztnummer des einweisenden Arztes, Einweisung durch einen Zahnarzt durch die Zahnarztnummer des einweisenden Zahnarztes dokumentiert.  
-Verlegung ist im § 301-Aufnahmesatz durch das IK des die Aufnahme veranlassenden Krankenhauses dokumentiert. Wenn die Behandlungsdauer im verlegenden Krankenhaus nicht länger als 24 Stunden betrug ist als Aufnahmeanlass ‚A’, wenn sie länger als 24 Stunden betrug, ist ‚V’ anzugeben. Der Aufnahmeanlass ‚R’ wird in der § 301-Datenübermittlung nicht abgebildet, er soll übermittelt werden, wenn die Patientendatenhaltung dieses Zusatzmerkmal enthält.  
-Interne Verlegung mit Wechsel aus einem Entgeltbereich in einen anderen Entgeltbereich wird durch das eigene IK als IK des veranlassenden Krankenhauses dokumentiert.  
-Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter (in Tagen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Angabe erfolgt nur bei Kindern bis zur Vollendung des 1. Lebensjahrs. Sie wird für die DRG-Zuordnung benötigt. Bei Neugeborenen mit Aufnahmetag=Geburtsdatum ist „1“ anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alter (in Jahren)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Altersangabe wird für die DRG-Zuordnung benötigt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geburtsjahr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das Geburtsjahr ist im Format JJJJ anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICD Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnoseschlüssel sind in der gültigen ICD-10GM-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. mit Sonderzeichen.  
-Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnoseart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsgrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01x Behandlung regulär beendet 
-- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
-- 03x Behandlung aus sonstigen Gründen beendet 
-- 04x Behandlung gegen ärztlichen Rat beendet 
-- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
-- 069 Verlegung in ein anderes Krankenhaus 
-- 079 Tod 
-- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
-- 099 Entlassung in eine Rehabilitationseinrichtung 
-- 109 Entlassung in eine Pflegeeinrichtung 
-- 119 Entlassung in ein Hospiz 
-- 139 externe Verlegung zur psychiatrischen Behandlung 
-- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
-- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
-- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
-- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
-- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
-- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
-- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
-Hinweise:  
-Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
-Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
-Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">01x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fallnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Das KH-interne Kennzeichen des Behandlungsfalls dient der eindeutigen Identifikation des Behandlungs-falls (Primärschlüssel). 
-Das KH-interne Kennzeichen darf von der Datenstelle nicht weiter übermittelt werden. 
-Wurden für einen Behandlungsfall im Verfahren nach § 301 SGB V unter identischem krankenhausinter-nen Kennzeichen des Behandlungsfalls mehrere Rechnungen in einem Entgeltbereich gestellt (z.B. quar-talsweise Abrechnung), ist bei der Datenlieferung nach § 21 KHEntgG nur ein Fall mit den Angaben des Gesamtaufenthalts im entsprechenden Entgeltbereich zu übermitteln.   
-Besondere Behandlungsfälle/Konstellationen:  
-Neugeborene sind stets als eigenständige Fälle mit allen zugehörigen fallbezogenen Daten getrennt von der Mutter zu dokumentieren. 
-Für gesunde Neugeborene ist ‚0601’ (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G’ anzuge-ben. 
-Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..’ (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G’ anzugeben. 
-Zur Kodierung der Diagnosen bei Neugeborenen siehe DKR.   
-Begleitpersonen und mitaufgenommene Pflegekräfte, die im § 301-Verfahren kein KH-internes Kennzeichen erhalten, sind mit einem eindeutigen Kennzeichen und mit dem Aufnahmeanlass „B“ zu dokumentieren. Die Angabe von Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmegrund, Entlassungs-/Verlegungsgrund, Alter, Fachabteilungs-, Diagnosen- und Prozedurenangaben entfällt.   
-Nur vorstationär behandelte Fälle:  
-Für nur vorstationär behandelte Fälle werden von den Falldaten der entlassende Standort, das KH-interne Kennzeichen, Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmeanlass, Aufnahmegrund, Fachabteilung und ggf. Diagnose- und Prozedurenangaben übermittelt. Für das Aufnahmedatum ist der erste, für das Entlassungsdatum der letzte vorstationäre Behandlungstag anzugeben.    
-Teilstationäre Fälle:  
-Im § 301-Verfahren werden teilstationäre Fälle mit tagesbezogenen Entgelten quartalsbezogen abgerechnet, dabei sind die Prozeduren jeweils mit dem jeweiligen Kalenderdatum der Leistungserbringung anzugeben. Fehlerhafte Angaben zu Prozeduren und zum Prozedurendatum werden im Datenannahmeverfahren als Fehler gewertet!  
-Krankenhäuser, die an der Kalkulationserhebung teilnehmen, dokumentieren die teilstationären Fälle mit fallbezogenen Angaben in den Dateien „Fall“, „FAB“, „ICD“, „OPS“ und „Entgelte“. Die Datei „Kosten“ enthält die tagesbezogenen Angaben der teilstationären Behandlungskosten und die Datumsangabe des je-weiligen Behandlungstags im Datenfeld „Pflegetag“. Es gibt keine kontaktbezogene Übermittlung von teilstationären Fällen im KHEntgG-Entgeltbereich.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsdatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist das Entlassungs-/Verlegungsdatum (Tag und Uhrzeit) aus der vollstationären oder teilstationären Behandlung anzugeben. (Bei interner Verlegung in einen anderen Entgeltbereich ohne nachfolgende Rückverlegung wird das Verlegungsdatum angegeben; die Behandlungsepisode in dem anderen Entgeltbereich wird als gesonderter Fall dokumentiert.) Bei nur vorstationär behandelten Fällen ist das Entlassungsdatum der letzte vorstationäre Behandlungstag.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmedatum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist das Aufnahmedatum (Aufnahmetag und Aufnahmeuhrzeit) zur vollstationären oder teilstationären Behandlung anzugeben.  
-Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geschlecht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- m männlich  
-- w weiblich  
-- x unbestimmt  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmegrund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
-- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
-- 03xx Krankenhausbehandlung, teilstationär 
-- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
-- 05xx stationäre Entbindung 
-- 06xx Geburt 
-- 08xx Stationäre Aufnahme zur Organentnahme  
-Hinweise:  
-Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
-Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">01xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patientennummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Patientennummer dient im Rahmen der Kalkulation der Zusammenführung von Fällen (mit unter-schiedlichen KH-internen Kennzeichen), bei denen die Patientennummer angegeben werden muss, zu einem Behandlungsblock. Bei Patienten, die im Datenjahr sowohl im Entgeltbereich „PSY“ als auch im Entgeltbereich „PIA“ behandelt wurden, muss in den jeweiligen Falldaten die Patientennummer angegeben werden. Die Patientennummer ist eine eindeutige und über die Zeit stabile Patienten-Identifikationsnummer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPS Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prozedurenschlüssel sind in der gültigen OPS-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. ohne Sonderzeichen.  
-Zur Reihenfolge der Prozedurenschlüssel für Fälle im KHEntgG-Entgeltbereich siehe DKR.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPS Datum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000’ angegeben werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fachabteilung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001’ (Rückverlegung) oder ‚0002’ (Wiederaufnahme) oder‚0003‘ (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
-Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA’ (Hauptabteilung) oder ‚BA’ (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE’ voranzustellen.  
-Bei Angabe der Pseudofachabteilungen ‚0001’, ‚0002’ und ‚0003‘ ist als Präfix ‚HA’ anzugeben.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entlassungsdatum (Fachabteilung)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bei nachstationärer Behandlung ist der letzte vollstationäre Behandlungstag (Entlassungsdatum) anzugeben. Der Wechsel von vollstationär zu nachstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden. Die nachstationären Behandlungstage sind bei den Falldaten gesondert anzugeben.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aufnahmedatum (Fachabteilung)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bei vorstationärer Behandlung ist der erste vollstationäre Behandlungstag (Aufnahmedatum) anzugeben. Der Wechsel von vorstationär zu vollstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatmungsstunden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Beatmungsstunden sind als Gesamtbeatmungszeit für den Krankenhausfall entsprechend DKR anzugeben. Der Wert entspricht der Angabe „Beatmungsstunden“ in der Entlassungsanzeige (Segment DAU).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postleitzahl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die Postleitzahl der Anschrift des Versicherten ist vollständig mit 5 Ziffern anzugeben.  
-Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
-  </si>
-  <si>
     <t xml:space="preserve">value</t>
   </si>
   <si>
@@ -617,283 +240,13 @@
     <t xml:space="preserve">Designation of value (in first defined language)</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C2;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C3;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C4;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C5;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C6;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C7;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C8;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C9;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C10;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C11;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C12;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C13;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">max_length</t>
   </si>
   <si>
     <t xml:space="preserve">regex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:alnum:]]){1,}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^([[:digit:]]{5})$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">range_from</t>
@@ -905,43 +258,7 @@
     <t xml:space="preserve">unit_of_measure</t>
   </si>
   <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A2;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A3;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_integer!$A4;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yyyy-MM-dd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A2;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A3;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A4;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A5;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A6;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
   </si>
   <si>
     <t xml:space="preserve">dataelement_id</t>
@@ -951,129 +268,6 @@
   </si>
   <si>
     <t xml:space="preserve">Designation of date element (first defined language)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dqa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"condition_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"observation_concept_id = 4108449\"],\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}"]},"postgres":{"i2b2":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"],"omop":["{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"],\"sql_where\":[\"\"],\"helper_vars\":{\"patient_identifier_value\":{\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"],\"sql_join_on\":[\"\"],\"sql_join_type\":[\"\"],\"sql_where\":[\"\"]}}}"]}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +457,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D21" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -1287,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G2"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -1303,8 +497,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1316,8 +510,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="value"/>
@@ -1330,8 +524,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D2"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -1343,8 +537,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="range_from"/>
@@ -1357,8 +551,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C2"/>
   <tableColumns count="3">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="format"/>
@@ -3914,464 +3108,64 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="n">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="n">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="n">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="G11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" t="n">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" t="n">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="G13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="n">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="n">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="G14" s="1"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="n">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="G15" s="1"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="n">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="n">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" t="n">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="G17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" t="n">
-        <v>16</v>
-      </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" t="n">
-        <v>6</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="G18" s="1"/>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="n">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" t="n">
-        <v>4</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="G19" s="1"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" t="n">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" t="n">
-        <v>5</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="n">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" t="n">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="n">
-        <v>20</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" t="n">
-        <v>7</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23">
       <c r="G23" s="1"/>
@@ -5838,16 +4632,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -5855,839 +4649,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1004</v>
-      </c>
-      <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1005</v>
-      </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>1006</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>1007</v>
-      </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1008</v>
-      </c>
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>1009</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>1010</v>
-      </c>
-      <c r="B20" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>1011</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>1012</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>1013</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>1014</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>1015</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>1016</v>
-      </c>
-      <c r="B26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>1017</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>1018</v>
-      </c>
-      <c r="B28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>1019</v>
-      </c>
-      <c r="B29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>1020</v>
-      </c>
-      <c r="B30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C30" t="s">
-        <v>126</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>1021</v>
-      </c>
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>1022</v>
-      </c>
-      <c r="B32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>128</v>
-      </c>
-      <c r="D32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>1023</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>129</v>
-      </c>
-      <c r="D33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>1024</v>
-      </c>
-      <c r="B34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>1025</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" t="s">
-        <v>131</v>
-      </c>
-      <c r="D35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>1026</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>1027</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>1028</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>9</v>
-      </c>
-      <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>1029</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>1030</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>1031</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>1032</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>1033</v>
-      </c>
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>1034</v>
-      </c>
-      <c r="B49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>1035</v>
-      </c>
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>1036</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>1037</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>1038</v>
-      </c>
-      <c r="B53" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" t="s">
-        <v>157</v>
-      </c>
-      <c r="D55" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>15</v>
-      </c>
-      <c r="B56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>161</v>
-      </c>
-      <c r="D57" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>17</v>
-      </c>
-      <c r="B58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" t="s">
-        <v>163</v>
-      </c>
-      <c r="D58" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D59" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>20</v>
-      </c>
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" t="s">
-        <v>170</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -7738,683 +5706,40 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>173</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
-      <c r="C2" t="n">
-        <v>1000</v>
+      <c r="C2" t="s">
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>70</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1001</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1002</v>
-      </c>
-      <c r="D4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1003</v>
-      </c>
-      <c r="D5" t="s">
-        <v>180</v>
-      </c>
-      <c r="E5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1004</v>
-      </c>
-      <c r="D6" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1005</v>
-      </c>
-      <c r="D7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1006</v>
-      </c>
-      <c r="D8" t="s">
-        <v>186</v>
-      </c>
-      <c r="E8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1007</v>
-      </c>
-      <c r="D9" t="s">
-        <v>188</v>
-      </c>
-      <c r="E9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1008</v>
-      </c>
-      <c r="D10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E10" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1009</v>
-      </c>
-      <c r="D11" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1010</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1011</v>
-      </c>
-      <c r="D13" t="s">
-        <v>196</v>
-      </c>
-      <c r="E13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1012</v>
-      </c>
-      <c r="D14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1013</v>
-      </c>
-      <c r="D15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1014</v>
-      </c>
-      <c r="D16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1015</v>
-      </c>
-      <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1016</v>
-      </c>
-      <c r="D18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" t="s">
-        <v>207</v>
-      </c>
-    </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1017</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1018</v>
-      </c>
-      <c r="D20" t="s">
-        <v>210</v>
-      </c>
-      <c r="E20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1019</v>
-      </c>
-      <c r="D21" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1020</v>
-      </c>
-      <c r="D22" t="s">
-        <v>214</v>
-      </c>
-      <c r="E22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1021</v>
-      </c>
-      <c r="D23" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1022</v>
-      </c>
-      <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1023</v>
-      </c>
-      <c r="D25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1024</v>
-      </c>
-      <c r="D26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1025</v>
-      </c>
-      <c r="D27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1026</v>
-      </c>
-      <c r="D28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1027</v>
-      </c>
-      <c r="D29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1028</v>
-      </c>
-      <c r="D30" t="s">
-        <v>230</v>
-      </c>
-      <c r="E30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1029</v>
-      </c>
-      <c r="D31" t="s">
-        <v>232</v>
-      </c>
-      <c r="E31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1030</v>
-      </c>
-      <c r="D32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1031</v>
-      </c>
-      <c r="D33" t="s">
-        <v>236</v>
-      </c>
-      <c r="E33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1032</v>
-      </c>
-      <c r="D34" t="s">
-        <v>238</v>
-      </c>
-      <c r="E34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1033</v>
-      </c>
-      <c r="D35" t="s">
-        <v>240</v>
-      </c>
-      <c r="E35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1034</v>
-      </c>
-      <c r="D36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1035</v>
-      </c>
-      <c r="D37" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1036</v>
-      </c>
-      <c r="D38" t="s">
-        <v>246</v>
-      </c>
-      <c r="E38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1037</v>
-      </c>
-      <c r="D39" t="s">
-        <v>248</v>
-      </c>
-      <c r="E39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1038</v>
-      </c>
-      <c r="D40" t="s">
-        <v>250</v>
-      </c>
-      <c r="E40" t="s">
-        <v>251</v>
-      </c>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -9469,115 +6794,31 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>252</v>
+        <v>71</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>253</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3" t="s">
-        <v>257</v>
-      </c>
-      <c r="D3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>254</v>
-      </c>
-      <c r="C8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" t="s">
-        <v>266</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -11712,70 +8953,36 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>267</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>268</v>
+        <v>74</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>75</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>70</v>
       </c>
-      <c r="C2" t="n">
-        <v>366</v>
+      <c r="C2" t="s">
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8766</v>
-      </c>
-      <c r="D4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" t="s">
-        <v>275</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -12831,68 +10038,24 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>276</v>
+        <v>76</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>277</v>
-      </c>
-      <c r="C5" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C6" t="s">
-        <v>282</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -13966,296 +11129,30 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>283</v>
+        <v>77</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>284</v>
+        <v>78</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>285</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C3" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C5" t="s">
-        <v>293</v>
-      </c>
-      <c r="D5" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C6" t="s">
-        <v>295</v>
-      </c>
-      <c r="D6" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C7" t="s">
-        <v>297</v>
-      </c>
-      <c r="D7" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>286</v>
-      </c>
-      <c r="C9" t="s">
-        <v>301</v>
-      </c>
-      <c r="D9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>286</v>
-      </c>
-      <c r="C10" t="s">
-        <v>303</v>
-      </c>
-      <c r="D10" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>286</v>
-      </c>
-      <c r="C11" t="s">
-        <v>305</v>
-      </c>
-      <c r="D11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" t="s">
-        <v>307</v>
-      </c>
-      <c r="D12" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>286</v>
-      </c>
-      <c r="C13" t="s">
-        <v>309</v>
-      </c>
-      <c r="D13" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>286</v>
-      </c>
-      <c r="C14" t="s">
-        <v>311</v>
-      </c>
-      <c r="D14" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>286</v>
-      </c>
-      <c r="C15" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C16" t="s">
-        <v>315</v>
-      </c>
-      <c r="D16" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>286</v>
-      </c>
-      <c r="C17" t="s">
-        <v>317</v>
-      </c>
-      <c r="D17" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>286</v>
-      </c>
-      <c r="C18" t="s">
-        <v>319</v>
-      </c>
-      <c r="D18" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>286</v>
-      </c>
-      <c r="C19" t="s">
-        <v>321</v>
-      </c>
-      <c r="D19" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>286</v>
-      </c>
-      <c r="C20" t="s">
-        <v>323</v>
-      </c>
-      <c r="D20" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>286</v>
-      </c>
-      <c r="C21" t="s">
-        <v>325</v>
-      </c>
-      <c r="D21" t="s">
-        <v>326</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress; extraction of plausibilities yet missing
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="327">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -210,6 +210,81 @@
     <t xml:space="preserve">=SVERWEIS(dataelements!$D2;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">dataelement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">permittedValues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D3;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D4;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D5;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D6;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D7;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D8;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D9;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D10;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D12;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D13;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D14;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D15;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D16;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D17;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D18;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D19;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D20;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D21;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D22;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -231,6 +306,308 @@
     <t xml:space="preserve">Diese Gruppe enthält die Datenelemente des Paragraph 21, die im Rahmen der DQ-Analyse geprüft werden.</t>
   </si>
   <si>
+    <t xml:space="preserve">Aufnahmeanlass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- E Einweisung durch einen Arzt 
+- Z Einweisung durch einen Zahnarzt 
+- N Notfall 
+- R Aufnahme nach vorausgehender Behandlung in einer Rehabilitationseinrichtung 
+- V Verlegung mit Behandlungsdauer im verlegenden Krankenhaus länger als 24 Stunden 
+- A Verlegung mit Behandlungsdauer im verlegenden Krankenhaus bis zu 24 Stunden  
+Zusatzschlüssel für besondere Kalkulationsanforderungen: 
+    - G Geburt (siehe Hinweis Neugeborene) 
+    - B Begleitperson oder mitaufgenommene Pflegekraft  
+Hinweise:  
+Einweisung durch einen Arzt ist im § 301-Aufnahmesatz im Segment Aufnahme durch die Arztnummer des einweisenden Arztes, Einweisung durch einen Zahnarzt durch die Zahnarztnummer des einweisenden Zahnarztes dokumentiert.  
+Verlegung ist im § 301-Aufnahmesatz durch das IK des die Aufnahme veranlassenden Krankenhauses dokumentiert. Wenn die Behandlungsdauer im verlegenden Krankenhaus nicht länger als 24 Stunden betrug ist als Aufnahmeanlass ‚A’, wenn sie länger als 24 Stunden betrug, ist ‚V’ anzugeben. Der Aufnahmeanlass ‚R’ wird in der § 301-Datenübermittlung nicht abgebildet, er soll übermittelt werden, wenn die Patientendatenhaltung dieses Zusatzmerkmal enthält.  
+Interne Verlegung mit Wechsel aus einem Entgeltbereich in einen anderen Entgeltbereich wird durch das eigene IK als IK des veranlassenden Krankenhauses dokumentiert.  
+Für DRG-Fälle, bei denen nach Rückverlegung eine Neueinstufung anhand der Daten beider Krankenhausaufenthalte durchgeführt wird, ist der Aufnahmeanlass bei Behandlungsbeginn in einer Fachabteilung, die zu dem Entgeltbereich der DRG-Fallpauschalen zählt, anzugeben.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter (in Tagen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Angabe erfolgt nur bei Kindern bis zur Vollendung des 1. Lebensjahrs. Sie wird für die DRG-Zuordnung benötigt. Bei Neugeborenen mit Aufnahmetag=Geburtsdatum ist „1“ anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alter (in Jahren)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Altersangabe wird für die DRG-Zuordnung benötigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geburtsjahr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das Geburtsjahr ist im Format JJJJ anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICD Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnoseschlüssel sind in der gültigen ICD-10GM-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. mit Sonderzeichen.  
+Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnoseart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsgrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01x Behandlung regulär beendet 
+- 02x Behandlung regulär beendet, nachstationäre Behandlung vorgesehen 
+- 03x Behandlung aus sonstigen Gründen beendet 
+- 04x Behandlung gegen ärztlichen Rat beendet 
+- 059 Zuständigkeitswechsel des Kostenträgers (bei tagesbezogenen Entgelten) 
+- 069 Verlegung in ein anderes Krankenhaus 
+- 079 Tod 
+- 089 Verlegung in ein anderes Krankenhaus im Rahmen einer Kooperation 
+- 099 Entlassung in eine Rehabilitationseinrichtung 
+- 109 Entlassung in eine Pflegeeinrichtung 
+- 119 Entlassung in ein Hospiz 
+- 139 externe Verlegung zur psychiatrischen Behandlung 
+- 14x Behandlung aus sonstigen Gründen beendet, nachstationäre Behandlung vorgesehen 
+- 15x Behandlung gegen ärztlichen Rat beendet, nachstationäre Behandlung vorgesehen 
+- 179 interne Verlegung mit Wechsel zwischen den Entgeltbereichen der DRG-Fallpauschalen, nach der BPflV oder für besondere Einrichtungen nach § 17b Abs. 1 Satz 15 KHG 
+- 229 Fallabschluss (interne Verlegung) bei Wechsel zwischen voll- und teilstationärer Behandlung 
+- 239 Beginn eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für verlegende Fachabteilung) 
+- 249 Beendigung eines externen Aufenthalts mit Abwesenheit über Mitternacht (BPflV-Bereich, für Pseudo-Fachabteilung 0003) 
+- 259 Entlassung zum Jahresende bei Aufnahme im Vorjahr (für Zwecke der Abrechnung, § 4 PEPPV)  
+Hinweise:  
+Es ist der Entlassungs-/Verlegungsgrund entsprechend Schlüssel 5 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. Stelle (‚x’) sind die nach Schlüssel 5 möglichen Werte (‚1’, ‚2’ oder ‚9’) anzugeben.  
+Der Entlassungs-/Verlegungsgrund kann entfallen bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass ‚B’). In allen anderen Fällen ist der Entlassungs-/Verlegungsgrund eine Muss-Angabe (bei Neugeborenen mit Aufnahmeanlass ‚G’ ist z.B. ‚019’ anzugeben).  
+Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">059</t>
+  </si>
+  <si>
+    <t xml:space="preserve">069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallnummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Das KH-interne Kennzeichen des Behandlungsfalls dient der eindeutigen Identifikation des Behandlungs-falls (Primärschlüssel). 
+Das KH-interne Kennzeichen darf von der Datenstelle nicht weiter übermittelt werden. 
+Wurden für einen Behandlungsfall im Verfahren nach § 301 SGB V unter identischem krankenhausinter-nen Kennzeichen des Behandlungsfalls mehrere Rechnungen in einem Entgeltbereich gestellt (z.B. quar-talsweise Abrechnung), ist bei der Datenlieferung nach § 21 KHEntgG nur ein Fall mit den Angaben des Gesamtaufenthalts im entsprechenden Entgeltbereich zu übermitteln.   
+Besondere Behandlungsfälle/Konstellationen:  
+Neugeborene sind stets als eigenständige Fälle mit allen zugehörigen fallbezogenen Daten getrennt von der Mutter zu dokumentieren. 
+Für gesunde Neugeborene ist ‚0601’ (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G’ anzuge-ben. 
+Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..’ (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G’ anzugeben. 
+Zur Kodierung der Diagnosen bei Neugeborenen siehe DKR.   
+Begleitpersonen und mitaufgenommene Pflegekräfte, die im § 301-Verfahren kein KH-internes Kennzeichen erhalten, sind mit einem eindeutigen Kennzeichen und mit dem Aufnahmeanlass „B“ zu dokumentieren. Die Angabe von Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmegrund, Entlassungs-/Verlegungsgrund, Alter, Fachabteilungs-, Diagnosen- und Prozedurenangaben entfällt.   
+Nur vorstationär behandelte Fälle:  
+Für nur vorstationär behandelte Fälle werden von den Falldaten der entlassende Standort, das KH-interne Kennzeichen, Geburtsjahr, Geschlecht, PLZ, Wohnort, Aufnahmeanlass, Aufnahmegrund, Fachabteilung und ggf. Diagnose- und Prozedurenangaben übermittelt. Für das Aufnahmedatum ist der erste, für das Entlassungsdatum der letzte vorstationäre Behandlungstag anzugeben.    
+Teilstationäre Fälle:  
+Im § 301-Verfahren werden teilstationäre Fälle mit tagesbezogenen Entgelten quartalsbezogen abgerechnet, dabei sind die Prozeduren jeweils mit dem jeweiligen Kalenderdatum der Leistungserbringung anzugeben. Fehlerhafte Angaben zu Prozeduren und zum Prozedurendatum werden im Datenannahmeverfahren als Fehler gewertet!  
+Krankenhäuser, die an der Kalkulationserhebung teilnehmen, dokumentieren die teilstationären Fälle mit fallbezogenen Angaben in den Dateien „Fall“, „FAB“, „ICD“, „OPS“ und „Entgelte“. Die Datei „Kosten“ enthält die tagesbezogenen Angaben der teilstationären Behandlungskosten und die Datumsangabe des je-weiligen Behandlungstags im Datenfeld „Pflegetag“. Es gibt keine kontaktbezogene Übermittlung von teilstationären Fällen im KHEntgG-Entgeltbereich.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsdatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist das Entlassungs-/Verlegungsdatum (Tag und Uhrzeit) aus der vollstationären oder teilstationären Behandlung anzugeben. (Bei interner Verlegung in einen anderen Entgeltbereich ohne nachfolgende Rückverlegung wird das Verlegungsdatum angegeben; die Behandlungsepisode in dem anderen Entgeltbereich wird als gesonderter Fall dokumentiert.) Bei nur vorstationär behandelten Fällen ist das Entlassungsdatum der letzte vorstationäre Behandlungstag.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmedatum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist das Aufnahmedatum (Aufnahmetag und Aufnahmeuhrzeit) zur vollstationären oder teilstationären Behandlung anzugeben.  
+Bei nur vorstationär behandelten Fällen ist das Aufnahmedatum der erste vorstationäre Behandlungstag.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geschlecht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- m männlich  
+- w weiblich  
+- x unbestimmt  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmegrund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 01xx Krankenhausbehandlung, vollstationär 
+- 02xx Krankenhausbehandlung, vollstationär mit vorausgegangener vorstationärer Behandlung 
+- 03xx Krankenhausbehandlung, teilstationär 
+- 04xx vorstationäre Behandlung ohne anschließende vollstationäre Behandlung 
+- 05xx stationäre Entbindung 
+- 06xx Geburt 
+- 08xx Stationäre Aufnahme zur Organentnahme  
+Hinweise:  
+Es ist der Aufnahmegrund entsprechend Schlüssel 1 der Anlage 2 zur § 301-Vereinbarung anzugeben. Als 3. und 4. Stelle (xx) sind die nach Schlüssel 1 möglichen Werte (01 bis 07, bei tagesbezogenen Entgelten auch 21 bis 27) anzugeben. Fälle mit den Werten „41“ bis „47“ in der 3. und 4. Stelle (Behandlungen im Rahmen von Verträgen zur integrierten Versorgung) können übermittelt werden.  
+Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patientennummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Patientennummer dient im Rahmen der Kalkulation der Zusammenführung von Fällen (mit unter-schiedlichen KH-internen Kennzeichen), bei denen die Patientennummer angegeben werden muss, zu einem Behandlungsblock. Bei Patienten, die im Datenjahr sowohl im Entgeltbereich „PSY“ als auch im Entgeltbereich „PIA“ behandelt wurden, muss in den jeweiligen Falldaten die Patientennummer angegeben werden. Die Patientennummer ist eine eindeutige und über die Zeit stabile Patienten-Identifikationsnummer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPS Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prozedurenschlüssel sind in der gültigen OPS-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. ohne Sonderzeichen.  
+Zur Reihenfolge der Prozedurenschlüssel für Fälle im KHEntgG-Entgeltbereich siehe DKR.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPS Datum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000’ angegeben werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachabteilung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001’ (Rückverlegung) oder ‚0002’ (Wiederaufnahme) oder‚0003‘ (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
+Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA’ (Hauptabteilung) oder ‚BA’ (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE’ voranzustellen.  
+Bei Angabe der Pseudofachabteilungen ‚0001’, ‚0002’ und ‚0003‘ ist als Präfix ‚HA’ anzugeben.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entlassungsdatum (Fachabteilung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei nachstationärer Behandlung ist der letzte vollstationäre Behandlungstag (Entlassungsdatum) anzugeben. Der Wechsel von vollstationär zu nachstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden. Die nachstationären Behandlungstage sind bei den Falldaten gesondert anzugeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufnahmedatum (Fachabteilung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei vorstationärer Behandlung ist der erste vollstationäre Behandlungstag (Aufnahmedatum) anzugeben. Der Wechsel von vorstationär zu vollstationär innerhalb der gleichen Fachabteilung muss nicht durch eine gesonderte Wiederholung der Fachabteilungsangabe dokumentiert werden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beatmungsstunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Beatmungsstunden sind als Gesamtbeatmungszeit für den Krankenhausfall entsprechend DKR anzugeben. Der Wert entspricht der Angabe „Beatmungsstunden“ in der Entlassungsanzeige (Segment DAU).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postleitzahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die Postleitzahl der Anschrift des Versicherten ist vollständig mit 5 Ziffern anzugeben.  
+Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
+  </si>
+  <si>
     <t xml:space="preserve">value</t>
   </si>
   <si>
@@ -240,7 +617,238 @@
     <t xml:space="preserve">Designation of value (in first defined language)</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A2; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C2;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A3; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C3;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A4; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C4;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A5; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C5;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A6; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C6;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A7; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C7;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A8; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C8;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A9; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C9;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A10; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C10;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A11; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C11;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A12; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C12;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A13; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C13;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A14; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">max_length</t>
@@ -249,6 +857,45 @@
     <t xml:space="preserve">regex</t>
   </si>
   <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:alnum:]]){1,}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^([[:digit:]]{5})$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">range_from</t>
   </si>
   <si>
@@ -258,9 +905,45 @@
     <t xml:space="preserve">unit_of_measure</t>
   </si>
   <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A2;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A3;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_integer!$A4;WENN(dataelements!$E:$E="integer";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">format</t>
   </si>
   <si>
+    <t xml:space="preserve">yyyy-MM-dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A2;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A3;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A4;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A5;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_calendar!$A6;WENN(dataelements!$E:$E="calendar";dataelements!$F:$G);2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">dataelement_id</t>
   </si>
   <si>
@@ -268,6 +951,129 @@
   </si>
   <si>
     <t xml:space="preserve">Designation of date element (first defined language)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dqa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -457,8 +1263,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D21" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D21"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -481,8 +1287,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G22" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -497,8 +1303,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D61"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -510,8 +1316,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E40"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="value"/>
@@ -524,8 +1330,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D8"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -537,8 +1343,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:E4" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="range_from"/>
@@ -551,8 +1357,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C2" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="format"/>
@@ -3108,64 +3914,464 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="G3" s="1"/>
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4">
-      <c r="G4" s="1"/>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="5">
-      <c r="G5" s="1"/>
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6">
-      <c r="G6" s="1"/>
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7">
-      <c r="G7" s="1"/>
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8">
-      <c r="G8" s="1"/>
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9">
-      <c r="G9" s="1"/>
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10">
-      <c r="G10" s="1"/>
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11">
-      <c r="G11" s="1"/>
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12">
-      <c r="G12" s="1"/>
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13">
-      <c r="G13" s="1"/>
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14">
-      <c r="G14" s="1"/>
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15">
-      <c r="G15" s="1"/>
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" t="n">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16">
-      <c r="G16" s="1"/>
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17">
-      <c r="G17" s="1"/>
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="18">
-      <c r="G18" s="1"/>
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="n">
+        <v>6</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19">
-      <c r="G19" s="1"/>
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="n">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="n">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20">
-      <c r="G20" s="1"/>
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="n">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="21">
-      <c r="G21" s="1"/>
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="n">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22">
-      <c r="G22" s="1"/>
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="23">
       <c r="G23" s="1"/>
@@ -4632,16 +5838,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -4649,13 +5855,839 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1001</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1002</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1005</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1006</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1007</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1008</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>1009</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>1010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1011</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1012</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1014</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1015</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>1016</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>1017</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>1018</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>1019</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>1021</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>1022</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1023</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>1024</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>1026</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>1027</v>
+      </c>
+      <c r="B37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>1028</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>139</v>
+      </c>
+      <c r="D41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>1029</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>1031</v>
+      </c>
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>1032</v>
+      </c>
+      <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>1033</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>1034</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>1035</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>1036</v>
+      </c>
+      <c r="B51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>1037</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>1038</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>15</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" t="s">
+        <v>159</v>
+      </c>
+      <c r="D56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>17</v>
+      </c>
+      <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" t="s">
+        <v>163</v>
+      </c>
+      <c r="D58" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5706,40 +7738,683 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>172</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>70</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
+        <v>94</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1005</v>
+      </c>
+      <c r="D7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1006</v>
+      </c>
+      <c r="D8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1007</v>
+      </c>
+      <c r="D9" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1009</v>
+      </c>
+      <c r="D11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1010</v>
+      </c>
+      <c r="D12" t="s">
+        <v>194</v>
+      </c>
+      <c r="E12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1011</v>
+      </c>
+      <c r="D13" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1012</v>
+      </c>
+      <c r="D14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1013</v>
+      </c>
+      <c r="D15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1014</v>
+      </c>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="19">
-      <c r="D19" s="1"/>
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1017</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1018</v>
+      </c>
+      <c r="D20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1019</v>
+      </c>
+      <c r="D21" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1020</v>
+      </c>
+      <c r="D22" t="s">
+        <v>214</v>
+      </c>
+      <c r="E22" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1021</v>
+      </c>
+      <c r="D23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1022</v>
+      </c>
+      <c r="D24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1025</v>
+      </c>
+      <c r="D27" t="s">
+        <v>224</v>
+      </c>
+      <c r="E27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1026</v>
+      </c>
+      <c r="D28" t="s">
+        <v>226</v>
+      </c>
+      <c r="E28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1027</v>
+      </c>
+      <c r="D29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1028</v>
+      </c>
+      <c r="D30" t="s">
+        <v>230</v>
+      </c>
+      <c r="E30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D31" t="s">
+        <v>232</v>
+      </c>
+      <c r="E31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1030</v>
+      </c>
+      <c r="D32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1031</v>
+      </c>
+      <c r="D33" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1032</v>
+      </c>
+      <c r="D34" t="s">
+        <v>238</v>
+      </c>
+      <c r="E34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1033</v>
+      </c>
+      <c r="D35" t="s">
+        <v>240</v>
+      </c>
+      <c r="E35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1034</v>
+      </c>
+      <c r="D36" t="s">
+        <v>242</v>
+      </c>
+      <c r="E36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1035</v>
+      </c>
+      <c r="D37" t="s">
+        <v>244</v>
+      </c>
+      <c r="E37" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1036</v>
+      </c>
+      <c r="D38" t="s">
+        <v>246</v>
+      </c>
+      <c r="E38" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1037</v>
+      </c>
+      <c r="D39" t="s">
+        <v>248</v>
+      </c>
+      <c r="E39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1038</v>
+      </c>
+      <c r="D40" t="s">
+        <v>250</v>
+      </c>
+      <c r="E40" t="s">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -6794,31 +9469,115 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>71</v>
+        <v>252</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>253</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>172</v>
       </c>
       <c r="E1"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>70</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -8953,36 +11712,70 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>73</v>
+        <v>267</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>268</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>75</v>
+        <v>269</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>68</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>270</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8766</v>
+      </c>
+      <c r="D4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -10038,24 +12831,68 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>76</v>
+        <v>276</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" t="s">
-        <v>70</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -11129,30 +13966,296 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>283</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>78</v>
+        <v>284</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>79</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
-        <v>70</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>287</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C8" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C12" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" t="s">
+        <v>311</v>
+      </c>
+      <c r="D14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>286</v>
+      </c>
+      <c r="C16" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" t="s">
+        <v>317</v>
+      </c>
+      <c r="D17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" t="s">
+        <v>319</v>
+      </c>
+      <c r="D18" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C19" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" t="s">
+        <v>323</v>
+      </c>
+      <c r="D20" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D21" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalized samply rest export to dqa-mdr conversion; not tested yet, but looks good :)
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -956,73 +956,73 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"fhir\":[\"condition.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
@@ -1034,43 +1034,43 @@
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
samply export/import now working
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -956,73 +956,73 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
@@ -1034,43 +1034,43 @@
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
@@ -4780,19 +4780,23 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>validationTypes!$A$1:$A$15</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1 E16:E176</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>validationTypes!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E15</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+          <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+              <x14:formula1>
+                <xm:f>validationTypes!$A$1:$A$15</xm:f>
+              </x14:formula1>
+              <xm:sqref>E1 E16:E176</xm:sqref>
+            </x14:dataValidation>
+            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+              <x14:formula1>
+                <xm:f>validationTypes!#REF!</xm:f>
+              </x14:formula1>
+              <xm:sqref>E2:E15</xm:sqref>
+            </x14:dataValidation>
+          </x14:dataValidations>
+        </ext>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -12908,19 +12912,23 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>calendarFormats!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>calendarFormats!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+          <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+              <x14:formula1>
+                <xm:f>calendarFormats!$A:$A</xm:f>
+              </x14:formula1>
+              <xm:sqref>B7:B1048576</xm:sqref>
+            </x14:dataValidation>
+            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+              <x14:formula1>
+                <xm:f>calendarFormats!#REF!</xm:f>
+              </x14:formula1>
+              <xm:sqref>B2:B5</xm:sqref>
+            </x14:dataValidation>
+          </x14:dataValidations>
+        </ext>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
added filter to import/export
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="260">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(dataelements!$D22;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D23;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -414,63 +417,6 @@
 Der Entlassungsgrund ‚179’ (interne Verlegung mit Wechsel …) dokumentiert, dass der Krankenhausfall als DRG-Fall abgeschlossen ist.  </t>
   </si>
   <si>
-    <t xml:space="preserve">01x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">059</t>
-  </si>
-  <si>
-    <t xml:space="preserve">069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">079</t>
-  </si>
-  <si>
-    <t xml:space="preserve">089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">099</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">179</t>
-  </si>
-  <si>
-    <t xml:space="preserve">229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">249</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fallnummer</t>
   </si>
   <si>
@@ -535,31 +481,16 @@
 Der Aufnahmegrund kann bei Begleitpersonen und mitaufgenommenen Pflegekräften (Aufnahmeanlass „B“) entfallen. In allen anderen Fällen ist der Aufnahmegrund eine Muss-Angabe.  </t>
   </si>
   <si>
-    <t xml:space="preserve">01xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08xx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Patientennummer</t>
   </si>
   <si>
     <t xml:space="preserve">Die Patientennummer dient im Rahmen der Kalkulation der Zusammenführung von Fällen (mit unter-schiedlichen KH-internen Kennzeichen), bei denen die Patientennummer angegeben werden muss, zu einem Behandlungsblock. Bei Patienten, die im Datenjahr sowohl im Entgeltbereich „PSY“ als auch im Entgeltbereich „PIA“ behandelt wurden, muss in den jeweiligen Falldaten die Patientennummer angegeben werden. Die Patientennummer ist eine eindeutige und über die Zeit stabile Patienten-Identifikationsnummer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medikation (OPS Code)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die aus den Prozedurenschlüsseln abgeleiteten Informationen bzgl. Medikation.</t>
   </si>
   <si>
     <t xml:space="preserve">OPS Code</t>
@@ -695,162 +626,6 @@
     <t xml:space="preserve">=SVERWEIS($C14;definitions!$A:$C;3;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A15; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C15;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A16; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C16;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A17; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C17;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A18; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C18;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A19; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C19;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A20; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C20;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A21; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C21;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A22; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C22;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A23; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C23;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A24; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C24;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A25; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C25;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A26; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C26;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A27; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C27;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A28; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C28;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A29; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C29;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A30; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C30;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A31; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C31;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A32; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C32;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A33; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C33;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A34; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C34;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A35; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C35;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A36; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C36;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A37; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C37;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A38; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C38;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A39; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C39;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_permittedValues!$A40; WENN(dataelements!$E:$E="permittedValues"; dataelements!$F:$G);2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS($C40;definitions!$A:$C;3;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">max_length</t>
   </si>
   <si>
@@ -866,34 +641,52 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?$</t>
+    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?(\+|\*)?$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">^([[:digit:]]{1,3})$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">^([[:alnum:]]){1,}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">^([[:digit:]]{1,4})$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(6\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A9;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A10;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">^([[:digit:]]{5})$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A11;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">range_from</t>
@@ -956,124 +749,130 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[110],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786629\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01x, 02x, 03x, 04x, 059, 069, 079, 089, 099, 109, 119, 139, 14x, 15x, 179, 229, 239, 249, 259\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"05xx\"],\"i2b2\":[\"05xx\"],\"p21csv\":[\"05xx\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"01xx, 02xx, 03xx, 04xx, 05xx, 06xx, 08xx\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1062,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D21" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D22" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D22"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -1287,8 +1086,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G22" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G23" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G23"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -1303,8 +1102,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D61" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D36" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D36"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1316,8 +1115,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E40" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:E40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:E14" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:E14"/>
   <tableColumns count="5">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="value"/>
@@ -1330,8 +1129,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D11" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D11"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -4065,7 +3864,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F9" t="n">
         <v>3</v>
@@ -4091,7 +3890,7 @@
         <v>66</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>71</v>
@@ -4160,7 +3959,7 @@
         <v>61</v>
       </c>
       <c r="F13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>75</v>
@@ -4180,7 +3979,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F14" t="n">
         <v>5</v>
@@ -4206,7 +4005,7 @@
         <v>66</v>
       </c>
       <c r="F15" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>77</v>
@@ -4229,7 +4028,7 @@
         <v>66</v>
       </c>
       <c r="F16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>78</v>
@@ -4249,10 +4048,10 @@
         <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F17" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>79</v>
@@ -4272,10 +4071,10 @@
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F18" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>80</v>
@@ -4295,10 +4094,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F19" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>81</v>
@@ -4321,7 +4120,7 @@
         <v>72</v>
       </c>
       <c r="F20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>82</v>
@@ -4341,10 +4140,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>83</v>
@@ -4364,17 +4163,37 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F22" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="23">
-      <c r="G23" s="1"/>
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24">
       <c r="G24" s="1"/>
@@ -5842,16 +5661,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
@@ -5859,13 +5678,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
@@ -5873,13 +5692,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
@@ -5887,13 +5706,13 @@
         <v>1000</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -5901,13 +5720,13 @@
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6">
@@ -5915,13 +5734,13 @@
         <v>1002</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -5929,13 +5748,13 @@
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8">
@@ -5943,13 +5762,13 @@
         <v>1004</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9">
@@ -5957,13 +5776,13 @@
         <v>1005</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
@@ -5971,13 +5790,13 @@
         <v>1006</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11">
@@ -5985,13 +5804,13 @@
         <v>1007</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
@@ -5999,13 +5818,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13">
@@ -6013,13 +5832,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
@@ -6027,13 +5846,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
@@ -6041,13 +5860,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16">
@@ -6055,13 +5874,13 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17">
@@ -6069,13 +5888,13 @@
         <v>1008</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18">
@@ -6083,13 +5902,13 @@
         <v>1009</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19">
@@ -6097,601 +5916,251 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1010</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1011</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1012</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1013</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1017</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1018</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1019</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1020</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1021</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1022</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1023</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1024</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1025</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1026</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>1027</v>
-      </c>
-      <c r="B37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>1028</v>
-      </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>8</v>
-      </c>
-      <c r="B39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>9</v>
-      </c>
-      <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>139</v>
-      </c>
-      <c r="D41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="D42" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>1029</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>1030</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>144</v>
-      </c>
-      <c r="D44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>1031</v>
-      </c>
-      <c r="B45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>1032</v>
-      </c>
-      <c r="B47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D47" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>1033</v>
-      </c>
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>1034</v>
-      </c>
-      <c r="B49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>1035</v>
-      </c>
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>1036</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>1037</v>
-      </c>
-      <c r="B52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>1038</v>
-      </c>
-      <c r="B53" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" t="s">
-        <v>157</v>
-      </c>
-      <c r="D55" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>15</v>
-      </c>
-      <c r="B56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>16</v>
-      </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>161</v>
-      </c>
-      <c r="D57" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>17</v>
-      </c>
-      <c r="B58" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" t="s">
-        <v>163</v>
-      </c>
-      <c r="D58" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D59" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>19</v>
-      </c>
-      <c r="B60" t="s">
-        <v>89</v>
-      </c>
-      <c r="C60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>20</v>
-      </c>
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -7742,19 +7211,19 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -7762,16 +7231,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" t="n">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">
@@ -7779,16 +7248,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C3" t="n">
         <v>1001</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4">
@@ -7796,16 +7265,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" t="n">
         <v>1002</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5">
@@ -7813,16 +7282,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C5" t="n">
         <v>1003</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6">
@@ -7830,16 +7299,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" t="n">
         <v>1004</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7">
@@ -7847,16 +7316,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C7" t="n">
         <v>1005</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
@@ -7864,16 +7333,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C8" t="n">
         <v>1006</v>
       </c>
       <c r="D8" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9">
@@ -7881,16 +7350,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C9" t="n">
         <v>1007</v>
       </c>
       <c r="D9" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10">
@@ -7898,16 +7367,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" t="n">
         <v>1008</v>
       </c>
       <c r="D10" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11">
@@ -7915,16 +7384,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" t="n">
         <v>1009</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="E11" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
@@ -7932,16 +7401,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C12" t="n">
         <v>1010</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="E12" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13">
@@ -7949,16 +7418,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C13" t="n">
         <v>1011</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14">
@@ -7966,459 +7435,20 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C14" t="n">
         <v>1012</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>3</v>
-      </c>
-      <c r="B15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1013</v>
-      </c>
-      <c r="D15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1014</v>
-      </c>
-      <c r="D16" t="s">
-        <v>202</v>
-      </c>
-      <c r="E16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1015</v>
-      </c>
-      <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>3</v>
-      </c>
-      <c r="B18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1016</v>
-      </c>
-      <c r="D18" t="s">
-        <v>206</v>
-      </c>
-      <c r="E18" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1017</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1018</v>
-      </c>
-      <c r="D20" t="s">
-        <v>210</v>
-      </c>
-      <c r="E20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1019</v>
-      </c>
-      <c r="D21" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1020</v>
-      </c>
-      <c r="D22" t="s">
-        <v>214</v>
-      </c>
-      <c r="E22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1021</v>
-      </c>
-      <c r="D23" t="s">
-        <v>216</v>
-      </c>
-      <c r="E23" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1022</v>
-      </c>
-      <c r="D24" t="s">
-        <v>218</v>
-      </c>
-      <c r="E24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1023</v>
-      </c>
-      <c r="D25" t="s">
-        <v>220</v>
-      </c>
-      <c r="E25" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1024</v>
-      </c>
-      <c r="D26" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1025</v>
-      </c>
-      <c r="D27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E27" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1026</v>
-      </c>
-      <c r="D28" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1027</v>
-      </c>
-      <c r="D29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1028</v>
-      </c>
-      <c r="D30" t="s">
-        <v>230</v>
-      </c>
-      <c r="E30" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1029</v>
-      </c>
-      <c r="D31" t="s">
-        <v>232</v>
-      </c>
-      <c r="E31" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>144</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1030</v>
-      </c>
-      <c r="D32" t="s">
-        <v>234</v>
-      </c>
-      <c r="E32" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1031</v>
-      </c>
-      <c r="D33" t="s">
-        <v>236</v>
-      </c>
-      <c r="E33" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>148</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1032</v>
-      </c>
-      <c r="D34" t="s">
-        <v>238</v>
-      </c>
-      <c r="E34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1033</v>
-      </c>
-      <c r="D35" t="s">
-        <v>240</v>
-      </c>
-      <c r="E35" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1034</v>
-      </c>
-      <c r="D36" t="s">
-        <v>242</v>
-      </c>
-      <c r="E36" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1035</v>
-      </c>
-      <c r="D37" t="s">
-        <v>244</v>
-      </c>
-      <c r="E37" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s">
-        <v>152</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1036</v>
-      </c>
-      <c r="D38" t="s">
-        <v>246</v>
-      </c>
-      <c r="E38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1037</v>
-      </c>
-      <c r="D39" t="s">
-        <v>248</v>
-      </c>
-      <c r="E39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1038</v>
-      </c>
-      <c r="D40" t="s">
-        <v>250</v>
-      </c>
-      <c r="E40" t="s">
-        <v>251</v>
-      </c>
+      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:E1048576">
@@ -9473,16 +8503,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>252</v>
+        <v>177</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>253</v>
+        <v>178</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="E1"/>
     </row>
@@ -9491,13 +8521,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>180</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3">
@@ -9505,13 +8535,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>257</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4">
@@ -9519,13 +8549,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5">
@@ -9533,13 +8563,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6">
@@ -9547,13 +8577,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7">
@@ -9561,13 +8591,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8">
@@ -9575,13 +8605,55 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>265</v>
+        <v>191</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -11716,19 +10788,19 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>267</v>
+        <v>198</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>268</v>
+        <v>199</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>200</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -11736,16 +10808,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>270</v>
+        <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3">
@@ -11753,16 +10825,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>272</v>
+        <v>203</v>
       </c>
       <c r="E3" t="s">
-        <v>273</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4">
@@ -11776,10 +10848,10 @@
         <v>8766</v>
       </c>
       <c r="D4" t="s">
-        <v>274</v>
+        <v>205</v>
       </c>
       <c r="E4" t="s">
-        <v>275</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -12835,13 +11907,13 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>276</v>
+        <v>207</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -12849,10 +11921,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
@@ -12860,10 +11932,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>279</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4">
@@ -12871,10 +11943,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5">
@@ -12882,10 +11954,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6">
@@ -12893,10 +11965,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -13974,16 +13046,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>283</v>
+        <v>214</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>284</v>
+        <v>215</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>285</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2">
@@ -13991,13 +13063,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>218</v>
       </c>
       <c r="D2" t="s">
-        <v>288</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3">
@@ -14005,13 +13077,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>290</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4">
@@ -14019,13 +13091,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>222</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5">
@@ -14033,13 +13105,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C5" t="s">
-        <v>293</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>294</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
@@ -14047,13 +13119,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
-        <v>295</v>
+        <v>226</v>
       </c>
       <c r="D6" t="s">
-        <v>296</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7">
@@ -14061,13 +13133,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>228</v>
       </c>
       <c r="D7" t="s">
-        <v>298</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8">
@@ -14075,13 +13147,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C8" t="s">
-        <v>299</v>
+        <v>230</v>
       </c>
       <c r="D8" t="s">
-        <v>300</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9">
@@ -14089,13 +13161,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>301</v>
+        <v>232</v>
       </c>
       <c r="D9" t="s">
-        <v>302</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10">
@@ -14103,13 +13175,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>234</v>
       </c>
       <c r="D10" t="s">
-        <v>304</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11">
@@ -14117,13 +13189,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
-        <v>305</v>
+        <v>236</v>
       </c>
       <c r="D11" t="s">
-        <v>306</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12">
@@ -14131,13 +13203,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C12" t="s">
-        <v>307</v>
+        <v>238</v>
       </c>
       <c r="D12" t="s">
-        <v>308</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13">
@@ -14145,13 +13217,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>240</v>
       </c>
       <c r="D13" t="s">
-        <v>310</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14">
@@ -14159,13 +13231,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C14" t="s">
-        <v>311</v>
+        <v>242</v>
       </c>
       <c r="D14" t="s">
-        <v>312</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15">
@@ -14173,13 +13245,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
-        <v>313</v>
+        <v>244</v>
       </c>
       <c r="D15" t="s">
-        <v>314</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16">
@@ -14187,13 +13259,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C16" t="s">
-        <v>315</v>
+        <v>246</v>
       </c>
       <c r="D16" t="s">
-        <v>316</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17">
@@ -14201,13 +13273,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>317</v>
+        <v>248</v>
       </c>
       <c r="D17" t="s">
-        <v>318</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18">
@@ -14215,13 +13287,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
-        <v>319</v>
+        <v>250</v>
       </c>
       <c r="D18" t="s">
-        <v>320</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19">
@@ -14229,13 +13301,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C19" t="s">
-        <v>321</v>
+        <v>252</v>
       </c>
       <c r="D19" t="s">
-        <v>322</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20">
@@ -14243,13 +13315,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C20" t="s">
-        <v>323</v>
+        <v>254</v>
       </c>
       <c r="D20" t="s">
-        <v>324</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21">
@@ -14257,13 +13329,27 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="C21" t="s">
-        <v>325</v>
+        <v>256</v>
       </c>
       <c r="D21" t="s">
-        <v>326</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added p21staging sql unit tests; updated fhir mapping according to current version from confluence; updated all sqls according to new fhir mapping; updated samply import file
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -641,7 +641,7 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A2;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?(\+|\*)?$</t>
+    <t xml:space="preserve">^([[:upper:]]){1}([[:digit:]]{1,2})((\.)([[:digit:]]{1,2}))?(\+|\*|\!)?$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
@@ -749,127 +749,127 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"condition_category_encounter_diagnosis\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_category_encounter_diagnosis"],"fhir":["condition.category.encounter.diagnosis"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"condition_category_encounter_diagnosis\"],\"fhir\":[\"condition.category.encounter.diagnosis\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_diagnosis_rank"],"fhir":["encounter.diagnosis.rank"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_end"],"fhir":["EpisodeOfCare.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"EpisodeOfCare_period_end\"],\"fhir\":[\"EpisodeOfCare.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["EpisodeOfCare_period_start"],"fhir":["EpisodeOfCare.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"EpisodeOfCare_period_start\"],\"fhir\":[\"EpisodeOfCare.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"]}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_where\":[\"procedure_source_value LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_where\":[\"procedure_source_value LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"],\"sql_where\":[\"OPS-Kode LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS-Datum\"],\"source_table_name\":[\"ops\"],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_serviceProvider_type_Organization_name"],"fhir":["encounter.serviceProvider.type.Organization.name"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"encounter_serviceProvider_type_Organization_name\"],\"fhir\":[\"encounter.serviceProvider.type.Organization.name\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["location_identifier_value"],"fhir":["location.identifier.value"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"fab\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_location_period_end"],"fhir":["encounter.location.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB-Entlassungsdatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_location_period_start"],"fhir":["encounter.location.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB-Aufnahmedatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
updated mdr with new i2b2 modelling (gender w=f, x=u)
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -698,7 +698,7 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A11;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^[[:digit:]]{1,6}\-[[:digit:]]{1}$</t>
+    <t xml:space="preserve">^[[:digit:]]{2,5}\-[[:digit:]]{1}$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A12;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
@@ -824,7 +824,7 @@
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
@@ -890,7 +890,7 @@
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{1,6}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{1,6}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
changed ops constraints for p21 to inek conformity
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -677,7 +677,7 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^([[:digit:]]{1})(\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+    <t xml:space="preserve">^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
@@ -842,7 +842,7 @@
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
fixed ops regex for p21; added chaperone exclusion in staging sqls; updated tests; updated version
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -677,7 +677,7 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$</t>
+    <t xml:space="preserve">^([[:digit:]]{1})(\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)?([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
@@ -764,25 +764,25 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AITAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:AIJAA'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
@@ -800,49 +800,49 @@
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_ide\"],\"source_table_name\":[\"encounter_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"encounter_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_ide\"],\"source_table_name\":[\"encounter_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"encounter_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"]}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))(([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
@@ -878,13 +878,13 @@
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
updated ops-medi constraints; updated mdr
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -683,7 +683,7 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^(6\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\.)([[:alnum:]]){1,2})?$</t>
+    <t xml:space="preserve">^(6(\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\.)?([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A9;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
@@ -848,7 +848,7 @@
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_where\":[\"procedure_source_value LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"],\"sql_where\":[\"OPS-Kode LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6(\\\\\\\\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_where\":[\"procedure_source_value LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6(\\\\\\\\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"],\"sql_where\":[\"OPS-Kode LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
updated mdr to now support also uniqueness logic from dqastats
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -788,7 +788,7 @@
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
@@ -824,7 +824,7 @@
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"O[0-9]\"],\"p21staging\":[\"O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"C5[1-8]\"],\"p21staging\":[\"C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"C6[0-3]\"],\"p21staging\":[\"C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
added support for analysis of 14 dataelements in total via fhirgw
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -764,13 +764,13 @@
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birthDate\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Condition'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"resources\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
@@ -782,49 +782,49 @@
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ENTLGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"hospitalization.dischargeDisposition.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(aadvice|exp|home|hosp|oth|other\\\\\\\\-hcf|rehab|snf|alt\\\\\\\\-home|long|psy)$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_ide\"],\"source_table_name\":[\"encounter_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"encounter_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_ide\"],\"source_table_name\":[\"encounter_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"encounter_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"subject.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"period.end\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"period.start\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, f, u\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, d, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"male, female, unknown, other\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"extension.valueCodeableConcept.coding.code\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
@@ -836,7 +836,7 @@
     <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS-Datum\"],\"source_table_name\":[\"ops\"],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS-Datum\"],\"source_table_name\":[\"ops\"],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"performedDateTime\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
@@ -860,19 +860,19 @@
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code_40617009"],"fhir":["procedure.code.coding.code.40617009"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"procedure_code_coding_code_40617009\"],\"fhir\":[\"procedure.code.coding.code.40617009\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#p21' AND DATA -&gt; 'code' -&gt; 'coding' -&gt; 0 -&gt;&gt; 'code' = '74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"address.postalCode\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#laboratory'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
fixed fhir adaption; fixed tests; adaption to new i2b2 modelling
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -770,7 +770,7 @@
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Condition'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"resources\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Condition'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
@@ -806,13 +806,13 @@
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, d, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"male, female, unknown, other\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_gender"],"fhir":["patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"],\"fhirgw\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"],\"fhirgw\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"],\"fhirgw\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"],\"fhirgw\":[\"male\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"],\"fhirgw\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"f\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"sex_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, d, x\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"patient_gender\"],\"fhir\":[\"patient.gender\"],\"source_variable_name\":[\"gender\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"male, female, unknown, other\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"extension.valueCodeableConcept.coding.code\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNGR%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"extension.valueCodeableConcept.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
@@ -824,7 +824,7 @@
     <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
@@ -860,7 +860,7 @@
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#p21' AND DATA -&gt; 'code' -&gt; 'coding' -&gt; 0 -&gt;&gt; 'code' = '74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#p21' AND DATA -&gt; 'code' -&gt; 'coding' -&gt; 0 -&gt;&gt; 'code' = '74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
@@ -872,7 +872,7 @@
     <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#laboratory'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#laboratory'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>

</xml_diff>

<commit_message>
updated i2b2 sqls, staging sqls, MDR
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="272">
   <si>
     <t>This Excel sheet was automatically generated from a CSV export</t>
   </si>
@@ -246,12 +246,12 @@
     <t xml:space="preserve">=SVERWEIS(dataelements!$D10;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">calendar</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(dataelements!$D11;definitions!$A:$D;3;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(dataelements!$D12;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS(dataelements!$D24;definitions!$A:$D;3;FALSCH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(dataelements!$D25;definitions!$A:$D;3;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -368,17 +371,20 @@
     <t xml:space="preserve">Das Geburtsjahr ist im Format JJJJ anzugeben.</t>
   </si>
   <si>
-    <t xml:space="preserve">Diagnosen (ICD)</t>
+    <t xml:space="preserve">Hauptdiagnosen (ICD)</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnoseschlüssel sind in der gültigen ICD-10GM-Version analog zur § 301-Vereinbarung zu übermitteln: d.h. mit Sonderzeichen.  
-Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD’) übermittelt werden.  </t>
+Als erste Diagnose soll die Hauptdiagnose (Diagnoseart: ‚HD') übermittelt werden.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nebendiagnosen (ICD)</t>
   </si>
   <si>
     <t xml:space="preserve">Diagnoseart</t>
   </si>
   <si>
-    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND’ übermittelt.</t>
+    <t xml:space="preserve">Die Diagnosen sind im KHEntgG-Entgeltbereich entsprechend den Deutschen Kodierrichtlinien (DKR) anzugeben. Bei nur vorstationär behandelten Fällen sind die Begriffe Haupt- und Nebendiagnose nicht definiert und die Aufnahmediagnosen können mit einer beliebigen Diagnoseart übermittelt werden. Bei PIA-Fällen wird für alle Diagnosen immer die Diagnoseart ‚ND' übermittelt.</t>
   </si>
   <si>
     <t xml:space="preserve">HD</t>
@@ -419,8 +425,8 @@
 Wurden für einen Behandlungsfall im Verfahren nach § 301 SGB V unter identischem krankenhausinter-nen Kennzeichen des Behandlungsfalls mehrere Rechnungen in einem Entgeltbereich gestellt (z.B. quar-talsweise Abrechnung), ist bei der Datenlieferung nach § 21 KHEntgG nur ein Fall mit den Angaben des Gesamtaufenthalts im entsprechenden Entgeltbereich zu übermitteln.   
 Besondere Behandlungsfälle/Konstellationen:  
 Neugeborene sind stets als eigenständige Fälle mit allen zugehörigen fallbezogenen Daten getrennt von der Mutter zu dokumentieren. 
-Für gesunde Neugeborene ist ‚0601’ (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G’ anzuge-ben. 
-Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..’ (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G’ anzugeben. 
+Für gesunde Neugeborene ist ‚0601' (Geburt) als Aufnahmegrund und der Aufnahmeanlass ‚G' anzuge-ben. 
+Für krankheitsbedingt behandlungsbedürftige Neugeborene ist der Aufnahmegrund ‚01..' (siehe Aufnahmegrund) und der Aufnahmeanlass ‚G' anzugeben. 
 Zur Kodierung der Diagnosen bei Neugeborenen siehe DKR.   </t>
   </si>
   <si>
@@ -488,15 +494,15 @@
     <t xml:space="preserve">OPS Datum</t>
   </si>
   <si>
-    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000’ angegeben werden.</t>
+    <t xml:space="preserve">Es ist der Beginn der Prozedur anzugeben. Bei Prozeduren, für die keine Startzeit (HHMM) erfasst ist, kann ‚JJJJMMTT0000' angegeben werden.</t>
   </si>
   <si>
     <t xml:space="preserve">Fachabteilung</t>
   </si>
   <si>
-    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001’ (Rückverlegung) oder ‚0002’ (Wiederaufnahme) oder‚0003‘ (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
-Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA’ (Hauptabteilung) oder ‚BA’ (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE’ voranzustellen.  
-Bei Angabe der Pseudofachabteilungen ‚0001’, ‚0002’ und ‚0003‘ ist als Präfix ‚HA’ anzugeben.  </t>
+    <t xml:space="preserve">Die Fachabteilung ist an dieser Stelle analog der Übermittlung nach § 301 SGB V einschließlich der Pseudofachabteilungen ‚0001' (Rückverlegung) oder ‚0002' (Wiederaufnahme) oder‚0003' (externer Aufenthalt mit Abwesenheit über Mitternacht im BPflV-Bereich) anzugeben.  
+Dem Fachabteilungsschlüssel ist bei Fachabteilungen das Präfix ‚HA' (Hauptabteilung) oder ‚BA' (Belegabteilung), bei Besonderen Einrichtungen das Präfix ‚BE' voranzustellen.  
+Bei Angabe der Pseudofachabteilungen ‚0001', ‚0002' und ‚0003' ist als Präfix ‚HA' anzugeben.  </t>
   </si>
   <si>
     <t xml:space="preserve">Entlassungsdatum (Fachabteilung)</t>
@@ -521,7 +527,7 @@
   </si>
   <si>
     <t xml:space="preserve">Die Postleitzahl der Anschrift des Versicherten ist vollständig mit 5 Ziffern anzugeben.  
-Bei ausländischen oder wohnsitzlosen Patienten: ‚00000’.   </t>
+Bei ausländischen oder wohnsitzlosen Patienten: ‚00000'.   </t>
   </si>
   <si>
     <t xml:space="preserve">Laborwerte (LOINC)</t>
@@ -638,52 +644,55 @@
     <t xml:space="preserve">=SVERWEIS(validations_string!$A3;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">^([[:digit:]]{1,3})$</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A4;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">^[0-2](\d){1,2}$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">^([[:alnum:]]){1,}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A5;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">^([[:digit:]]{1,4})$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A6;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A7;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">^([[:digit:]]{1})(\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\.)?([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A8;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A9;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">^(6(\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\.)?([[:alnum:]]){1,2})?$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A9;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS(validations_string!$A10;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A11;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">^([[:digit:]]{5})$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A11;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A12;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">^[[:digit:]]{2,5}\-[[:digit:]]{1}$</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS(validations_string!$A12;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS(validations_string!$A13;WENN(dataelements!$E:$E="string";dataelements!$F:$G);2;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">range_from</t>
@@ -746,19 +755,19 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'AUFNAN%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"FALL|AUFNAHMEANLASS:E\\\",\\\"FALL|AUFNAHMEANLASS:Z\\\",\\\"FALL|AUFNAHMEANLASS:N\\\",\\\"FALL|AUFNAHMEANLASS:R\\\",\\\"FALL|AUFNAHMEANLASS:V\\\",\\\"FALL|AUFNAHMEANLASS:A\\\",\\\"FALL|AUFNAHMEANLASS:G\\\",\\\"FALL|AUFNAHMEANLASS:B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|AUFNAHMEANLASS%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERTAGE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERTAGE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERJAHRE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[115],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERJAHRE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
@@ -770,112 +779,118 @@
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"ICD.CSV\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"condition_source_value\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Condition'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"HD\\\"]}\"],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:HD' AND observation_blob NOT LIKE 'Code 2 from%'\\n\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'HD'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_diagnosis_rank"],"fhir":["encounter.diagnosis.rank"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code_rank2"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"ND\\\"]}\"],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code.rank2\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:ND' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'ND'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^DISCHARGEDISPOSITION\\\\\\\\:(AADVICE|EXP|HOME|HOSP|OTH|OTHER\\\\\\\\-HCF|REHAB|SNF|ALT\\\\\\\\-HOME|LONG|PSY)$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DISCHARGEDISPOSITION%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,3})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"hospitalization.dischargeDisposition.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(aadvice|exp|home|hosp|oth|other\\\\\\\\-hcf|rehab|snf|alt\\\\\\\\-home|long|psy)$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_diagnosis_rank"],"fhir":["encounter.diagnosis.rank"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_ide\"],\"source_table_name\":[\"encounter_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"encounter_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"subject.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^FALL\\\\\\\\|ENTLASSGRUND\\\\\\\\:[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|ENTLASSGRUND%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"hospitalization.dischargeDisposition.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(aadvice|exp|home|hosp|oth|other\\\\\\\\-hcf|rehab|snf|alt\\\\\\\\-home|long|psy)$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"patient_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"subject.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"period.end\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"period.start\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_gender"],"fhir":["encounter.subject.patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"],\"fhirgw\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"],\"fhirgw\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"],\"fhirgw\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"DEM|GESCHLECHT:m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"],\"fhirgw\":[\"male\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"],\"fhirgw\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DEM|GESCHLECHT:m, DEM|GESCHLECHT:w, DEM|GESCHLECHT:d, DEM|GESCHLECHT:x\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|GESCHLECHT%'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"gender\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"male, female, unknown, other\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_gender"],"fhir":["encounter.subject.patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"],\"fhirgw\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.1\":{\"name\":[\"Pl.atemporal.Item02\"],\"description\":[\"Nur bei weiblichen Patientinnen sind bösartige Neubildungen der weiblichen Genitalorgane (ICD C51-C58) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C5[1-8]\"],\"i2b2\":[\"^(ICD10\\\\:)C5[1-8]\"],\"p21csv\":[\"^C5[1-8]\"],\"p21staging\":[\"^C5[1-8]\"],\"fhirgw\":[\"^C5[1-8]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}},\"condition_code_coding_code.2\":{\"name\":[\"Pl.atemporal.Item03\"],\"description\":[\"Nur bei männlichen Patienten sind bösartige Neubildungen der männlichen Genitalorgane (ICD C60-C63) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^C6[0-3]\"],\"i2b2\":[\"^(ICD10\\\\:)C6[0-3]\"],\"p21csv\":[\"^C6[0-3]\"],\"p21staging\":[\"^C6[0-3]\"],\"fhirgw\":[\"^C6[0-3]\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"m\"],\"i2b2\":[\"DEM|GESCHLECHT:m\"],\"p21csv\":[\"m\"],\"p21staging\":[\"m\"],\"fhirgw\":[\"male\"]}}},\"encounter_hospitalization_class\":{\"name\":[\"Pl.atemporal.Item04\"],\"description\":[\"Nur bei weiblichen Patientinnen ist 'stationäre Entbindung' als Aufnahmegrund (05) erlaubt.\"],\"filter\":{\"omop\":[\"^05\"],\"i2b2\":[\"^FALL\\\\|AUFNAHMEGRUND\\\\:05\"],\"p21csv\":[\"^05\"],\"p21staging\":[\"^05\"],\"fhirgw\":[\"^05\"]},\"join_crit\":[\"encounter_identifier_value\"],\"constraints\":{\"value_set\":{\"omop\":[\"w\"],\"i2b2\":[\"DEM|GESCHLECHT:w\"],\"p21csv\":[\"w\"],\"p21staging\":[\"w\"],\"fhirgw\":[\"female\"]}}}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"GESCHLECHT\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DEM|GESCHLECHT:m, DEM|GESCHLECHT:w, DEM|GESCHLECHT:d, DEM|GESCHLECHT:x\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|GESCHLECHT%'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"gender_source_value\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"Geschlecht\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"m, w, x\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.gender\"],\"variable_name\":[\"encounter_subject_patient_gender\"],\"fhir\":[\"encounter.subject.patient.gender\"],\"source_variable_name\":[\"gender\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"male, female, unknown, other\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.gender\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">{"variable_name":["encounter_hospitalization_class"],"fhir":["encounter.hospitalization.class"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"AUFNAHMEGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^FALL\\\\\\\\|AUFNAHMEGRUND\\\\\\\\:([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|AUFNAHMEGRUND%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id NOT IN (4164916, 4194310, 4138807, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"Aufnahmegrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.hospitalization\"],\"variable_name\":[\"encounter_hospitalization_class\"],\"fhir\":[\"encounter.hospitalization.class\"],\"source_variable_name\":[\"extension.valueCodeableConcept.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1,4})$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.hospitalization\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A13;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["patient_identifier_value"],"fhir":["patient.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_birthDate\":{\"name\":[\"Pl.uniqueness.Item01\"],\"description\":[\"Mit jeder Patienten-ID darf nur ein Geburtsjahr assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"PATIENTENNUMMER\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"patient_dimension\"]}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation\"]}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.patient\"],\"variable_name\":[\"patient_identifier_value\"],\"fhir\":[\"patient.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A14;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_internes_Kennzeichen\"],\"source_table_name\":[\"OPS.CSV\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:)([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{1})(\\\\\\\\-)?([[:digit:]]{2})([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A15;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["procedure_code_coding_code"],"fhir":["procedure.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"procedure_code_coding_code\\\"],\\\"filter_logic\\\":[\\\"6\\\\\\\\-00\\\"]}\"],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS_Kode\"],\"source_table_name\":[\"OPS.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6(\\\\\\\\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(OPS\\\\\\\\:6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS:6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"procedure_source_value\"],\"source_table_name\":[\"procedure_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6\\\\\\\\-00)([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"procedure_occurrence\"],\"sql_where\":[\"procedure_source_value LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.procedure_medication\"],\"variable_name\":[\"procedure_code_coding_code\"],\"fhir\":[\"procedure.code.coding.code\"],\"source_variable_name\":[\"OPS-Kode\"],\"source_table_name\":[\"ops\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(6(\\\\\\\\-)?(00))([[:lower:]]{1}|([[:digit:]]{1}))((\\\\\\\\.)?([[:alnum:]]){1,2})?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"ops\"],\"sql_where\":[\"OPS-Kode LIKE '6-00%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.procedure_medication\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A16;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["procedure_performedDateTime"],"fhir":["procedure.performedDateTime"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS_Datum\"],\"source_table_name\":[\"OPS.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'OPS%'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"procedure_date\"],\"source_table_name\":[\"procedure_occurrence\"],\"sql_from\":[\"procedure_occurrence\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"procedure_occurrence\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"procedure_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"OPS-Datum\"],\"source_table_name\":[\"ops\"],\"sql_from\":[\"ops\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"ops\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"ops\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.proceduredate\"],\"variable_name\":[\"procedure_performedDateTime\"],\"fhir\":[\"procedure.performedDateTime\"],\"source_variable_name\":[\"performedDateTime\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Procedure'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.proceduredate\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A17;dataelements!A:G;7;FALSCH)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{"variable_name":["location_identifier_value"],"fhir":["location.identifier.value"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"tval_char\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"fab\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">=SVERWEIS($A18;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_location_period_end"],"fhir":["encounter.location.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB-Entlassungsdatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["location_identifier_value"],"fhir":["location.identifier.value"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"FAB.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FAB.CSV\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"]}}}"]},"postgres":{"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"care_site_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.provider\"],\"variable_name\":[\"location_identifier_value\"],\"fhir\":[\"location.identifier.value\"],\"source_variable_name\":[\"FAB\"],\"source_table_name\":[\"fab\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.provider\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A19;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_location_period_start"],"fhir":["encounter.location.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"observation_fact\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FACHABT%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB-Aufnahmedatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_location_period_end"],"fhir":["encounter.location.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB_ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerend\"],\"variable_name\":[\"encounter_location_period_end\"],\"fhir\":[\"encounter.location.period.end\"],\"source_variable_name\":[\"FAB-Entlassungsdatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A20;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL:BEATMST'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"undefined\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#p21' AND DATA -&gt; 'code' -&gt; 'coding' -&gt; 0 -&gt;&gt; 'code' = '74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"undefined\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_location_period_start"],"fhir":["encounter.location.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB_AUFNAHMEDATUM\"],\"source_table_name\":[\"FAB.CSV\"]}}"]},"postgres":{"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.providerstart\"],\"variable_name\":[\"encounter_location_period_start\"],\"fhir\":[\"encounter.location.period.start\"],\"source_variable_name\":[\"FAB-Aufnahmedatum\"],\"source_table_name\":[\"fab\"],\"sql_from\":[\"fab\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fab\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.providerstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fab\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A21;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
+    <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"BEATMUNGSSTUNDEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC:74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4108449\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ventilation\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"Beatmungsstunden\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ventilation\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"undefined\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[8766],\\\"unit\\\":[\\\"h\\\"]}}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#p21' AND DATA -&gt; 'code' -&gt; 'coding' -&gt; 0 -&gt;&gt; 'code' = '74201-5'\"]},\"helper_vars\":{\"procedure_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"procedure_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"undefined\"],\"fhir\":[\"procedure.encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
+  </si>
+  <si>
     <t xml:space="preserve">{"variable_name":["patient_address_postalCode"],"fhir":["patient.address.postalCode"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip_cd\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"zip\"],\"source_table_name\":[\"location\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"location\"],\"sql_join_on\":[\"location_id\"],\"sql_join_type\":[\"left outer\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"person\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"PLZ\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.zipcode\"],\"variable_name\":[\"patient_address_postalCode\"],\"fhir\":[\"patient.address.postalCode\"],\"source_variable_name\":[\"address.postalCode\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:digit:]]{5})$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.zipcode\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A22;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
     <t xml:space="preserve">{"variable_name":["observation_code_coding_code"],"fhir":["observation.code.coding.code"],"csv":[],"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(LOINC\\\\\\\\:)[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'LOINC%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"loinc_code\"],\"source_table_name\":[\"laboratory_p21\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"laboratory_p21\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"case_id\"],\"source_table_name\":[\"laboratory_p21\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"laboratory_p21\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.laboratory\"],\"variable_name\":[\"observation_code_coding_code\"],\"fhir\":[\"observation.code.coding.code\"],\"source_variable_name\":[\"code.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[[:digit:]]{2,5}\\\\\\\\-[[:digit:]]{1}$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Observation' AND DATA -&gt; 'meta' -&gt;&gt; 'source' = '#laboratory'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.laboratory\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
-    <t xml:space="preserve">=SVERWEIS($A23;dataelements!A:G;7;FALSCH)</t>
+    <t xml:space="preserve">=SVERWEIS($A24;dataelements!A:G;7;FALSCH)</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1080,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D23" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A1:D24" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D24"/>
   <tableColumns count="4">
     <tableColumn id="1" name="dataelement_id"/>
     <tableColumn id="2" name="key"/>
@@ -1089,8 +1104,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G24" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:G25" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:G25"/>
   <tableColumns count="7">
     <tableColumn id="1" name="temp_id"/>
     <tableColumn id="2" name="parent_id"/>
@@ -1105,8 +1120,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D37" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D38" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D38"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="language"/>
@@ -1132,8 +1147,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D12" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:D13" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:D13"/>
   <tableColumns count="4">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="max_length"/>
@@ -3844,10 +3859,10 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>69</v>
@@ -3867,10 +3882,10 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>70</v>
@@ -3913,13 +3928,13 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -3936,10 +3951,10 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>74</v>
@@ -3959,10 +3974,10 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F13" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>75</v>
@@ -3982,10 +3997,10 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>76</v>
@@ -4074,10 +4089,10 @@
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>80</v>
@@ -4097,10 +4112,10 @@
         <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F19" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>81</v>
@@ -4120,10 +4135,10 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F20" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>82</v>
@@ -4143,10 +4158,10 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>83</v>
@@ -4166,10 +4181,10 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>84</v>
@@ -4189,10 +4204,10 @@
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F23" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>85</v>
@@ -4222,7 +4237,27 @@
       </c>
     </row>
     <row r="25">
-      <c r="G25" s="1"/>
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="n">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="n">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="26">
       <c r="G26" s="1"/>
@@ -4622,23 +4657,19 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-          <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-              <x14:formula1>
-                <xm:f>validationTypes!$A$1:$A$15</xm:f>
-              </x14:formula1>
-              <xm:sqref>E1 E16:E176</xm:sqref>
-            </x14:dataValidation>
-            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-              <x14:formula1>
-                <xm:f>validationTypes!#REF!</xm:f>
-              </x14:formula1>
-              <xm:sqref>E2:E15</xm:sqref>
-            </x14:dataValidation>
-          </x14:dataValidations>
-        </ext>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>validationTypes!$A$1:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1 E16:E176</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>validationTypes!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E15</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -5684,16 +5715,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2">
@@ -5701,13 +5732,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3">
@@ -5715,13 +5746,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4">
@@ -5729,13 +5760,13 @@
         <v>1000</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5">
@@ -5743,13 +5774,13 @@
         <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
@@ -5757,13 +5788,13 @@
         <v>1002</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -5771,13 +5802,13 @@
         <v>1003</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8">
@@ -5785,13 +5816,13 @@
         <v>1004</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9">
@@ -5799,13 +5830,13 @@
         <v>1005</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10">
@@ -5813,13 +5844,13 @@
         <v>1006</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11">
@@ -5827,13 +5858,13 @@
         <v>1007</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
@@ -5841,13 +5872,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
@@ -5855,13 +5886,13 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -5869,13 +5900,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
@@ -5883,13 +5914,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16">
@@ -5897,52 +5928,52 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
         <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1008</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
         <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>1009</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D19" t="s">
         <v>117</v>
@@ -5953,7 +5984,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>118</v>
@@ -5967,7 +5998,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
         <v>120</v>
@@ -5981,7 +6012,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>122</v>
@@ -5995,7 +6026,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
         <v>124</v>
@@ -6006,55 +6037,55 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1010</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
         <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>12</v>
+        <v>1012</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
         <v>130</v>
@@ -6065,7 +6096,7 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
         <v>131</v>
@@ -6079,7 +6110,7 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>133</v>
@@ -6093,7 +6124,7 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
         <v>135</v>
@@ -6107,7 +6138,7 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
         <v>137</v>
@@ -6121,7 +6152,7 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
         <v>139</v>
@@ -6135,7 +6166,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
         <v>141</v>
@@ -6149,7 +6180,7 @@
         <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
         <v>143</v>
@@ -6163,7 +6194,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
         <v>145</v>
@@ -6177,7 +6208,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
         <v>147</v>
@@ -6191,13 +6222,27 @@
         <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
         <v>149</v>
       </c>
       <c r="D37" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -7248,19 +7293,19 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -7268,16 +7313,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C2" t="n">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3">
@@ -7285,16 +7330,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C3" t="n">
         <v>1001</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4">
@@ -7302,16 +7347,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C4" t="n">
         <v>1002</v>
       </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5">
@@ -7319,16 +7364,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C5" t="n">
         <v>1003</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6">
@@ -7336,16 +7381,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C6" t="n">
         <v>1004</v>
       </c>
       <c r="D6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7">
@@ -7353,16 +7398,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="n">
         <v>1005</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8">
@@ -7370,16 +7415,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C8" t="n">
         <v>1006</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
@@ -7387,16 +7432,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" t="n">
         <v>1007</v>
       </c>
       <c r="D9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10">
@@ -7404,16 +7449,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C10" t="n">
         <v>1008</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11">
@@ -7421,16 +7466,16 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C11" t="n">
         <v>1009</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
@@ -7438,16 +7483,16 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C12" t="n">
         <v>1010</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13">
@@ -7455,16 +7500,16 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C13" t="n">
         <v>1011</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E13" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14">
@@ -7472,16 +7517,16 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C14" t="n">
         <v>1012</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19">
@@ -8540,16 +8585,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E1"/>
     </row>
@@ -8558,13 +8603,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3">
@@ -8572,13 +8617,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4">
@@ -8586,13 +8631,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
         <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5">
@@ -8600,13 +8645,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
@@ -8614,13 +8659,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7">
@@ -8628,13 +8673,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8">
@@ -8642,13 +8687,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
@@ -8656,13 +8701,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10">
@@ -8670,13 +8715,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11">
@@ -8684,13 +8729,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
@@ -8698,13 +8743,27 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -10839,19 +10898,19 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -10859,16 +10918,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>366</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3">
@@ -10879,13 +10938,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4">
@@ -10899,10 +10958,10 @@
         <v>8766</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -11958,13 +12017,13 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -11972,10 +12031,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3">
@@ -11983,10 +12042,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
@@ -11994,10 +12053,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5">
@@ -12005,10 +12064,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6">
@@ -12016,10 +12075,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -12035,23 +12094,19 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-          <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-              <x14:formula1>
-                <xm:f>calendarFormats!$A:$A</xm:f>
-              </x14:formula1>
-              <xm:sqref>B7:B1048576</xm:sqref>
-            </x14:dataValidation>
-            <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-              <x14:formula1>
-                <xm:f>calendarFormats!#REF!</xm:f>
-              </x14:formula1>
-              <xm:sqref>B2:B5</xm:sqref>
-            </x14:dataValidation>
-          </x14:dataValidations>
-        </ext>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>calendarFormats!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>calendarFormats!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B5</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -13097,16 +13152,16 @@
   <sheetData>
     <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2">
@@ -13114,13 +13169,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3">
@@ -13128,13 +13183,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
@@ -13142,13 +13197,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5">
@@ -13156,13 +13211,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6">
@@ -13170,13 +13225,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7">
@@ -13184,13 +13239,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D7" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8">
@@ -13198,13 +13253,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D8" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9">
@@ -13212,13 +13267,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10">
@@ -13226,13 +13281,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11">
@@ -13240,13 +13295,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D11" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12">
@@ -13254,13 +13309,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13">
@@ -13268,13 +13323,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14">
@@ -13282,13 +13337,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15">
@@ -13296,13 +13351,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16">
@@ -13310,13 +13365,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17">
@@ -13324,13 +13379,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D17" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="18">
@@ -13338,13 +13393,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D18" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19">
@@ -13352,13 +13407,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20">
@@ -13366,13 +13421,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D20" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21">
@@ -13380,13 +13435,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D21" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22">
@@ -13394,13 +13449,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23">
@@ -13408,13 +13463,27 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D23" t="s">
-        <v>266</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24" t="s">
+        <v>270</v>
+      </c>
+      <c r="D24" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: moving towards date-restriction
</commit_message>
<xml_diff>
--- a/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
+++ b/inst/application/_utilities/MDR/XLSX/mdr-import_DQA.xlsx
@@ -755,139 +755,139 @@
     <t xml:space="preserve">dqa</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"FALL|AUFNAHMEANLASS:E\\\",\\\"FALL|AUFNAHMEANLASS:Z\\\",\\\"FALL|AUFNAHMEANLASS:N\\\",\\\"FALL|AUFNAHMEANLASS:R\\\",\\\"FALL|AUFNAHMEANLASS:V\\\",\\\"FALL|AUFNAHMEANLASS:A\\\",\\\"FALL|AUFNAHMEANLASS:G\\\",\\\"FALL|AUFNAHMEANLASS:B\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|AUFNAHMEANLASS%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_admitSource"],"fhir":["encounter.hospitalization.admitSource"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"AUFNAHMEANLASS\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"FALL|AUFNAHMEANLASS:E\\\",\\\"FALL|AUFNAHMEANLASS:Z\\\",\\\"FALL|AUFNAHMEANLASS:N\\\",\\\"FALL|AUFNAHMEANLASS:R\\\",\\\"FALL|AUFNAHMEANLASS:V\\\",\\\"FALL|AUFNAHMEANLASS:A\\\",\\\"FALL|AUFNAHMEANLASS:G\\\",\\\"FALL|AUFNAHMEANLASS:B\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|AUFNAHMEANLASS%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_type_concept_id = 43542355 AND observation_concept_id IN (4164916, 4194310, 4138807, 4216316, 4079617, 4146925, 4123917)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.admission\"],\"variable_name\":[\"encounter_hospitalization_admitSource\"],\"fhir\":[\"encounter.hospitalization.admitSource\"],\"source_variable_name\":[\"Aufnahmeanlass\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"E, Z, N, R, V, A, G, B\\\"]}\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.admission\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A2;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERTAGE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_days"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_TAGEN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERTAGE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 8512\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageindays\"],\"variable_name\":[\"encounter_subject_patient_age_days\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Tagen-am-Aufnahmetag\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[0],\\\"max\\\":[366],\\\"unit\\\":[\\\"d\\\"]}}\"],\"value_threshold\":[0],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageindays\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A3;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERJAHRE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_age_years"],"fhir":["undefined"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"ALTER_IN_JAHREN_AM_AUFNAHMETAG\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"nval_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'DEM|AUFNAHMEALTERJAHRE%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id = 4265453 AND unit_concept_id = 9448\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.ageinyears\"],\"variable_name\":[\"encounter_subject_patient_age_years\"],\"fhir\":[\"undefined\"],\"source_variable_name\":[\"Alter-in-Jahren-am-Aufnahmetag\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"range\\\":{\\\"min\\\":[1],\\\"max\\\":[150],\\\"unit\\\":[\\\"a\\\"]}}\"],\"value_threshold\":[5],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.ageinyears\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A4;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birthDate\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["patient_birthDate"],"fhir":["patient.birthDate"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"GEBURTSJAHR\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birth_date\"],\"source_table_name\":[\"i2b2miracum.patient_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"patient_dimension\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"i2b2miracum.patient_dimension\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"patient_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"year_of_birth\"],\"source_table_name\":[\"person\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"person\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"person\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"Geburtsjahr\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.birthdate\"],\"variable_name\":[\"patient_birthDate\"],\"fhir\":[\"patient.birthDate\"],\"source_variable_name\":[\"birthDate\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(19|20)([[:digit:]]{2})((-[[:digit:]]{2}){2})?$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Patient'\"]},\"helper_vars\":{\"patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.birthdate\"],\"fhir\":[\"patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A5;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"HD\\\"]}\"],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:HD' AND observation_blob NOT LIKE 'Code 2 from%'\\n\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'HD'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"HD\\\"]}\"],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:HD' AND observation_blob NOT LIKE 'Code 2 from%'\\n\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"plausibility_relation\":[\"{\\\"uniqueness\\\":{\\\"encounter_diagnosis_rank\\\":{\\\"name\\\":[\\\"Pl.uniqueness.Item03\\\"],\\\"description\\\":[\\\"Mit jeder Fallnummer darf nur eine Hauptdiagnose assoziiert sein.\\\"],\\\"all_observations\\\":[\\\"1\\\"],\\\"filter\\\":{\\\"i2b2\\\":[\\\"DIAGNOSEART:HD\\\"],\\\"p21csv\\\":[\\\"HD\\\"],\\\"p21staging\\\":[\\\"HD\\\"],\\\"omop\\\":[\\\"44786627\\\"]}}}}\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_principal\"],\"variable_name\":[\"condition_code_coding_code\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"p21.icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'HD'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_principal\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A6;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["condition_code_coding_code_rank2"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"ND\\\"]}\"],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code.rank2\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:ND' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'ND'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["condition_code_coding_code_rank2"],"fhir":["condition.code.coding.code"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[\"{\\\"filter_var\\\":[\\\"encounter_diagnosis_rank\\\"],\\\"filter_logic\\\":[\\\"ND\\\"]}\"],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD_Kode\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code.rank2\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(ICD10\\\\\\\\:)([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"data_map\":[1],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND modifier_cd = 'DIAGNOSEART:ND' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.condition_secondary\"],\"variable_name\":[\"condition_code_coding_code_rank2\"],\"fhir\":[\"condition.code.coding.code\"],\"source_variable_name\":[\"ICD-Kode\"],\"source_table_name\":[\"p21.icd\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:upper:]]){1}([[:digit:]]{1,2})((\\\\\\\\.)([[:digit:]]{1,2}))?(\\\\\\\\+|\\\\\\\\*|\\\\\\\\!)?$\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"icd\"],\"sql_where\":[\"Diagnoseart = 'ND'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.condition_secondary\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A7;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_diagnosis_rank"],"fhir":["encounter.diagnosis.rank"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"icd\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_diagnosis_rank"],"fhir":["encounter.diagnosis.rank"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"ICD.CSV\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"modifier_cd\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"DIAGNOSEART:HD, DIAGNOSEART:ND\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'ICD%' AND observation_blob NOT LIKE 'Code 2 from%'\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"condition_type_concept_id\"],\"source_table_name\":[\"condition_occurrence\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"44786627, 44786629\\\"]}\"],\"sql_from\":[\"condition_occurrence\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"condition_occurrence\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"condition_occurrence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.conditioncategory\"],\"variable_name\":[\"encounter_diagnosis_rank\"],\"fhir\":[\"encounter.diagnosis.rank\"],\"source_variable_name\":[\"Diagnoseart\"],\"source_table_name\":[\"p21.icd\"],\"constraints\":[\"{\\\"value_set\\\":[\\\"HD, ND\\\"]}\"],\"sql_from\":[\"icd\"]},\"helper_vars\":{\"condition_encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.icd\"],\"variable_name\":[\"condition_encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.conditioncategory\"],\"fhir\":[\"condition.encounter.identifier.value\"],\"sql_from\":[\"icd\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A8;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^FALL\\\\\\\\|ENTLASSGRUND\\\\\\\\:[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|ENTLASSGRUND%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"hospitalization.dischargeDisposition.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(aadvice|exp|home|hosp|oth|other\\\\\\\\-hcf|rehab|snf|alt\\\\\\\\-home|long|psy)$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_hospitalization_dischargeDisposition"],"fhir":["encounter.hospitalization.dischargeDisposition"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"ENTLASSUNGSGRUND\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"concept_cd\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^FALL\\\\\\\\|ENTLASSGRUND\\\\\\\\:[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"],\"sql_where\":[\"concept_cd LIKE 'FALL|ENTLASSGRUND%'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.observation_fact\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"observation_fact\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"observation_source_value\"],\"source_table_name\":[\"observation\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"sql_from\":[\"observation\"],\"sql_where\":[\"observation_concept_id IN (433128, 4021968, 4049607, 4052193, 4053230, 4082735, 4084500, 4084686, 4127600, 4139566, 4143443, 4147710, 4185328, 4185329, 4186037, 4203130, 4213258, 4216643, 4274958, 45878214)\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"observation\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"observation\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"Entlassungsgrund\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^[0-2](\\\\\\\\d){1,2}$\\\"]}\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.discharge\"],\"variable_name\":[\"encounter_hospitalization_dischargeDisposition\"],\"fhir\":[\"encounter.hospitalization.dischargeDisposition\"],\"source_variable_name\":[\"hospitalization.dischargeDisposition.coding.code\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^(aadvice|exp|home|hosp|oth|other\\\\\\\\-hcf|rehab|snf|alt\\\\\\\\-home|long|psy)$\\\"]}\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.discharge\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A9;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"encounter_mapping\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"encounter_mapping\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"patient_mapping\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"patient_mapping\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"subject.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_identifier_value"],"fhir":["encounter.identifier.value"],"plausibility_relation":["{\"uniqueness\":{\"patient_identifier_value\":{\"name\":[\"Pl.uniqueness.Item02\"],\"description\":[\"Mit jeder Fallnummer darf nur eine Patienten-ID assoziiert sein.\"]}}}"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH_INTERNES_KENNZEICHEN\"],\"source_table_name\":[\"FALL.CSV\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"restricting_date_var\":[\"start_date\"],\"data_map\":[1],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"patient_num\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"visit_dimension\"],\"sql_where\":[\"visit_blob = 'True encounter'\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"person_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"data_map\":[1],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"Patientennummer\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounter\"],\"variable_name\":[\"encounter_identifier_value\"],\"fhir\":[\"encounter.identifier.value\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"constraints\":[\"{\\\"regex\\\":[\\\"^([[:alnum:]]){1,}\\\"]}\"],\"data_map\":[1],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_subject_patient_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Patientennummer\"],\"source_variable_name\":[\"subject.reference\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_subject_patient_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounter\"],\"fhir\":[\"encounter.subject.patient.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A10;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"period.end\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_end"],"fhir":["encounter.period.end"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"ENTLASSUNGSDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"end_date\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"constraints\":[\"%Y-%m-%d\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"visit_end_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"Entlassungsdatum\"],\"source_table_name\":[\"p21.fall\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterend\"],\"variable_name\":[\"encounter_period_end\"],\"fhir\":[\"encounter.period.end\"],\"source_variable_name\":[\"period.end\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterend\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A11;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"visit_dimension\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"fall\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"period.start\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
+    <t xml:space="preserve">{"variable_name":["encounter_period_start"],"fhir":["encounter.period.start"],"csv":{"p21csv":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"AUFNAHMEDATUM\"],\"source_table_name\":[\"FALL.CSV\"]}}"]},"postgres":{"i2b2":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"start_date\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"constraints\":[\"%Y-%m-%d\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"visit_dimension\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"encounter_num\"],\"source_table_name\":[\"i2b2miracum.visit_dimension\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"start_date\"],\"sql_from\":[\"visit_dimension\"]}}}"],"omop":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"visit_start_date\"],\"source_table_name\":[\"visit_occurrence\"],\"sql_from\":[\"visit_occurence\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"visit_occurrence_id\"],\"source_table_name\":[\"visit_occurrence\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"visit_occurence\"],\"sql_where\":[\"gender_concept_id IN ('8507', '8532', '8551')\"]}}}"],"p21staging":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"Aufnahmedatum\"],\"source_table_name\":[\"p21.fall\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"],\"sql_where\":[\"Aufnahmeanlass != 'B' OR Aufnahmeanlass IS NULL\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"KH-internes-Kennzeichen\"],\"source_table_name\":[\"p21.fall\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"restricting_date_var\":[\"Aufnahmedatum\"],\"restricting_date_format\":[\"%Y%m%d%H%M\"],\"sql_from\":[\"fall\"]}}}"],"fhirgw":["{\"base\":{\"dqa_assessment\":[1],\"filter\":[null],\"key\":[\"dt.encounterstart\"],\"variable_name\":[\"encounter_period_start\"],\"fhir\":[\"encounter.period.start\"],\"source_variable_name\":[\"period.start\"],\"source_table_name\":[\"resources\"],\"sql_from\":[\"resources\"],\"sql_where\":[\"type = 'Encounter'\"]},\"helper_vars\":{\"encounter_identifier_value\":{\"dqa_assessment\":[0],\"designation\":[\"Fallnummer\"],\"source_variable_name\":[\"id\"],\"source_table_name\":[\"resources\"],\"variable_name\":[\"encounter_identifier_value\"],\"variable_type\":[\"string\"],\"key\":[\"dt.encounterstart\"],\"fhir\":[\"encounter.identifier.value\"],\"sql_from\":[\"resources\"]}}}"]}}</t>
   </si>
   <si>
     <t xml:space="preserve">=SVERWEIS($A12;dataelements!A:G;7;FALSCH)</t>
   </si>
   <si>
-    <t xml:space="preserve">{"variable_name":["encounter_subject_patient_gender"],"fhir":["encounter.subject.patient.gender"],"plausibility_relation":["{\"atemporal\":{\"condition_code_coding_code\":{\"name\":[\"Pl.atemporal.Item01\"],\"description\":[\"Nur bei weiblichen Patientinnen ist eine ICD-Diagnose aus dem ICD-Kapitel XV (ICD O00-O99) (Schwangerschaft, Geburt und Wochenbett) als Krankenhausdiagnose erlaubt.\"],\"filter\":{\"omop\":[\"^O[0-9]\"],\"i2b2\":[\"^(ICD10\\\\:)O[0-9]\"],\"p21csv\":[\"^O[0-9]\"],\"p21staging\":[\"^O[0-9]\"],\"fhirgw\":[\"^O[0-9]\"]},\"join_crit\":[\"encounter_identifier_v